<commit_message>
Updated Gantt Chart and Task Progress
</commit_message>
<xml_diff>
--- a/docs/gantt-chart/Lakeshore Misfits Project Gantt chart.xlsx
+++ b/docs/gantt-chart/Lakeshore Misfits Project Gantt chart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khngu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khngu\Documents\_GVSU\CIS 641\_Team_Project\_Term_Project\GVSU-CIS641-Lakeshore-Misfits\docs\gantt-chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C104B0-A72D-4BD7-B903-A5D8C23ABEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4A7960-3828-4C7D-B816-1ABEC16AB5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>0 - 8</t>
+  </si>
+  <si>
+    <t>Setup Global Color Palette State / Context</t>
   </si>
 </sst>
 </file>
@@ -938,7 +941,7 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1220,31 +1223,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="167" fontId="21" fillId="13" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1276,71 +1254,95 @@
     <xf numFmtId="167" fontId="21" fillId="13" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="5" borderId="8" xfId="10" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" xfId="10" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="12" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="19" fillId="10" borderId="9" xfId="10" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="10" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="19" fillId="5" borderId="8" xfId="10" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="8" xfId="10" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="12" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="11" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="19" fillId="10" borderId="9" xfId="10" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="10" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1358,40 +1360,6 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="61">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1582,6 +1550,40 @@
         <bottom style="thin">
           <color theme="0" tint="-4.9989318521683403E-2"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
       </border>
     </dxf>
     <dxf>
@@ -2521,10 +2523,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BT44"/>
+  <dimension ref="A1:BT45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="AL25" sqref="AL25"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:BT41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2538,9 +2540,9 @@
     <col min="8" max="8" width="2.6875" customWidth="1"/>
     <col min="9" max="9" width="6" hidden="1" customWidth="1"/>
     <col min="10" max="15" width="2.6875" customWidth="1"/>
-    <col min="16" max="18" width="2.6875" style="110" customWidth="1"/>
+    <col min="16" max="18" width="2.6875" style="101" customWidth="1"/>
     <col min="19" max="46" width="2.6875" customWidth="1"/>
-    <col min="47" max="51" width="2.6875" style="110" customWidth="1"/>
+    <col min="47" max="51" width="2.6875" style="101" customWidth="1"/>
     <col min="52" max="73" width="2.6875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2555,34 +2557,34 @@
       <c r="F1" s="19"/>
       <c r="G1" s="20"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="121" t="s">
+      <c r="J1" s="130" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="122"/>
-      <c r="L1" s="122"/>
-      <c r="M1" s="122"/>
-      <c r="N1" s="122"/>
-      <c r="O1" s="122"/>
-      <c r="P1" s="122"/>
-      <c r="Q1" s="127">
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="132">
         <f>DATE(2023,9,13)</f>
         <v>45182</v>
       </c>
-      <c r="R1" s="128"/>
-      <c r="S1" s="128"/>
-      <c r="T1" s="128"/>
-      <c r="U1" s="128"/>
-      <c r="V1" s="128"/>
-      <c r="W1" s="128"/>
-      <c r="X1" s="128"/>
-      <c r="Y1" s="128"/>
-      <c r="Z1" s="128"/>
-      <c r="AA1" s="144"/>
-      <c r="AU1" s="126"/>
-      <c r="AV1" s="126"/>
-      <c r="AW1" s="126"/>
-      <c r="AX1" s="126"/>
-      <c r="AY1" s="126"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
+      <c r="T1" s="133"/>
+      <c r="U1" s="133"/>
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="133"/>
+      <c r="Y1" s="133"/>
+      <c r="Z1" s="133"/>
+      <c r="AA1" s="113"/>
+      <c r="AU1"/>
+      <c r="AV1"/>
+      <c r="AW1"/>
+      <c r="AX1"/>
+      <c r="AY1"/>
     </row>
     <row r="2" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B2" s="91" t="s">
@@ -2595,34 +2597,34 @@
       <c r="E2" s="21"/>
       <c r="F2" s="22"/>
       <c r="G2" s="21"/>
-      <c r="I2" s="121" t="s">
+      <c r="I2" s="130" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="122"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
-      <c r="N2" s="122"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="123"/>
-      <c r="Q2" s="127">
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
+      <c r="P2" s="112"/>
+      <c r="Q2" s="132">
         <f>DATE(2023,10,16)</f>
         <v>45215</v>
       </c>
-      <c r="R2" s="128"/>
-      <c r="S2" s="128"/>
-      <c r="T2" s="128"/>
-      <c r="U2" s="128"/>
-      <c r="V2" s="128"/>
-      <c r="W2" s="128"/>
-      <c r="X2" s="128"/>
-      <c r="Y2" s="128"/>
-      <c r="Z2" s="128"/>
-      <c r="AU2" s="126"/>
-      <c r="AV2" s="126"/>
-      <c r="AW2" s="126"/>
-      <c r="AX2" s="126"/>
-      <c r="AY2" s="126"/>
+      <c r="R2" s="133"/>
+      <c r="S2" s="133"/>
+      <c r="T2" s="133"/>
+      <c r="U2" s="133"/>
+      <c r="V2" s="133"/>
+      <c r="W2" s="133"/>
+      <c r="X2" s="133"/>
+      <c r="Y2" s="133"/>
+      <c r="Z2" s="133"/>
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
     </row>
     <row r="3" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B3" s="91"/>
@@ -2631,33 +2633,33 @@
       <c r="E3" s="21"/>
       <c r="F3" s="22"/>
       <c r="G3" s="21"/>
-      <c r="J3" s="121" t="s">
+      <c r="J3" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="122"/>
-      <c r="L3" s="122"/>
-      <c r="M3" s="122"/>
-      <c r="N3" s="122"/>
-      <c r="O3" s="122"/>
-      <c r="P3" s="122"/>
-      <c r="Q3" s="123"/>
-      <c r="R3" s="125">
+      <c r="K3" s="131"/>
+      <c r="L3" s="131"/>
+      <c r="M3" s="131"/>
+      <c r="N3" s="131"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="131"/>
+      <c r="Q3" s="112"/>
+      <c r="R3" s="143">
         <v>1</v>
       </c>
-      <c r="S3" s="124"/>
-      <c r="T3" s="124"/>
-      <c r="U3" s="124"/>
-      <c r="V3" s="124"/>
-      <c r="W3" s="124"/>
-      <c r="X3" s="124"/>
-      <c r="Y3" s="124"/>
-      <c r="Z3" s="124"/>
-      <c r="AA3" s="124"/>
-      <c r="AU3" s="126"/>
-      <c r="AV3" s="126"/>
-      <c r="AW3" s="126"/>
-      <c r="AX3" s="126"/>
-      <c r="AY3" s="126"/>
+      <c r="S3" s="144"/>
+      <c r="T3" s="144"/>
+      <c r="U3" s="144"/>
+      <c r="V3" s="144"/>
+      <c r="W3" s="144"/>
+      <c r="X3" s="144"/>
+      <c r="Y3" s="144"/>
+      <c r="Z3" s="144"/>
+      <c r="AA3" s="144"/>
+      <c r="AU3"/>
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3"/>
+      <c r="AY3"/>
     </row>
     <row r="4" spans="1:72" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="12"/>
@@ -2667,87 +2669,87 @@
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="26"/>
-      <c r="J4" s="103" t="s">
+      <c r="J4" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="101"/>
-      <c r="L4" s="101"/>
-      <c r="M4" s="101"/>
-      <c r="N4" s="101"/>
-      <c r="O4" s="101"/>
-      <c r="P4" s="101"/>
-      <c r="Q4" s="101" t="s">
+      <c r="K4" s="134"/>
+      <c r="L4" s="134"/>
+      <c r="M4" s="134"/>
+      <c r="N4" s="134"/>
+      <c r="O4" s="134"/>
+      <c r="P4" s="134"/>
+      <c r="Q4" s="134" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="101"/>
-      <c r="S4" s="101"/>
-      <c r="T4" s="101"/>
-      <c r="U4" s="101"/>
-      <c r="V4" s="101"/>
-      <c r="W4" s="101"/>
-      <c r="X4" s="101" t="s">
+      <c r="R4" s="134"/>
+      <c r="S4" s="134"/>
+      <c r="T4" s="134"/>
+      <c r="U4" s="134"/>
+      <c r="V4" s="134"/>
+      <c r="W4" s="134"/>
+      <c r="X4" s="134" t="s">
         <v>43</v>
       </c>
-      <c r="Y4" s="101"/>
-      <c r="Z4" s="101"/>
-      <c r="AA4" s="101"/>
-      <c r="AB4" s="101"/>
-      <c r="AC4" s="101"/>
-      <c r="AD4" s="101"/>
-      <c r="AE4" s="101" t="s">
+      <c r="Y4" s="134"/>
+      <c r="Z4" s="134"/>
+      <c r="AA4" s="134"/>
+      <c r="AB4" s="134"/>
+      <c r="AC4" s="134"/>
+      <c r="AD4" s="134"/>
+      <c r="AE4" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="AF4" s="101"/>
-      <c r="AG4" s="101"/>
-      <c r="AH4" s="101"/>
-      <c r="AI4" s="101"/>
-      <c r="AJ4" s="101"/>
-      <c r="AK4" s="101"/>
-      <c r="AL4" s="101" t="s">
+      <c r="AF4" s="134"/>
+      <c r="AG4" s="134"/>
+      <c r="AH4" s="134"/>
+      <c r="AI4" s="134"/>
+      <c r="AJ4" s="134"/>
+      <c r="AK4" s="134"/>
+      <c r="AL4" s="134" t="s">
         <v>45</v>
       </c>
-      <c r="AM4" s="101"/>
-      <c r="AN4" s="101"/>
-      <c r="AO4" s="101"/>
-      <c r="AP4" s="101"/>
-      <c r="AQ4" s="101"/>
-      <c r="AR4" s="101"/>
-      <c r="AS4" s="101" t="s">
+      <c r="AM4" s="134"/>
+      <c r="AN4" s="134"/>
+      <c r="AO4" s="134"/>
+      <c r="AP4" s="134"/>
+      <c r="AQ4" s="134"/>
+      <c r="AR4" s="134"/>
+      <c r="AS4" s="134" t="s">
         <v>46</v>
       </c>
-      <c r="AT4" s="101"/>
-      <c r="AU4" s="101"/>
-      <c r="AV4" s="101"/>
-      <c r="AW4" s="101"/>
-      <c r="AX4" s="101"/>
-      <c r="AY4" s="101"/>
-      <c r="AZ4" s="101" t="s">
+      <c r="AT4" s="134"/>
+      <c r="AU4" s="134"/>
+      <c r="AV4" s="134"/>
+      <c r="AW4" s="134"/>
+      <c r="AX4" s="134"/>
+      <c r="AY4" s="134"/>
+      <c r="AZ4" s="134" t="s">
         <v>47</v>
       </c>
-      <c r="BA4" s="101"/>
-      <c r="BB4" s="101"/>
-      <c r="BC4" s="101"/>
-      <c r="BD4" s="101"/>
-      <c r="BE4" s="101"/>
-      <c r="BF4" s="101"/>
-      <c r="BG4" s="101" t="s">
+      <c r="BA4" s="134"/>
+      <c r="BB4" s="134"/>
+      <c r="BC4" s="134"/>
+      <c r="BD4" s="134"/>
+      <c r="BE4" s="134"/>
+      <c r="BF4" s="134"/>
+      <c r="BG4" s="134" t="s">
         <v>48</v>
       </c>
-      <c r="BH4" s="101"/>
-      <c r="BI4" s="101"/>
-      <c r="BJ4" s="101"/>
-      <c r="BK4" s="101"/>
-      <c r="BL4" s="101"/>
-      <c r="BM4" s="101"/>
-      <c r="BN4" s="101" t="s">
+      <c r="BH4" s="134"/>
+      <c r="BI4" s="134"/>
+      <c r="BJ4" s="134"/>
+      <c r="BK4" s="134"/>
+      <c r="BL4" s="134"/>
+      <c r="BM4" s="134"/>
+      <c r="BN4" s="134" t="s">
         <v>49</v>
       </c>
-      <c r="BO4" s="101"/>
-      <c r="BP4" s="101"/>
-      <c r="BQ4" s="101"/>
-      <c r="BR4" s="101"/>
-      <c r="BS4" s="101"/>
-      <c r="BT4" s="101"/>
+      <c r="BO4" s="134"/>
+      <c r="BP4" s="134"/>
+      <c r="BQ4" s="134"/>
+      <c r="BR4" s="134"/>
+      <c r="BS4" s="134"/>
+      <c r="BT4" s="134"/>
     </row>
     <row r="5" spans="1:72" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
@@ -2755,115 +2757,115 @@
         <v>13</v>
       </c>
       <c r="F5" s="28"/>
-      <c r="J5" s="103">
+      <c r="J5" s="136">
         <f>J6</f>
         <v>45215</v>
       </c>
-      <c r="K5" s="101"/>
-      <c r="L5" s="101"/>
-      <c r="M5" s="101"/>
-      <c r="N5" s="101"/>
-      <c r="O5" s="101"/>
-      <c r="P5" s="101"/>
-      <c r="Q5" s="101">
+      <c r="K5" s="134"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="134"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
+      <c r="Q5" s="134">
         <f>Q6</f>
         <v>45222</v>
       </c>
-      <c r="R5" s="101"/>
-      <c r="S5" s="101"/>
-      <c r="T5" s="101"/>
-      <c r="U5" s="101"/>
-      <c r="V5" s="101"/>
-      <c r="W5" s="101"/>
-      <c r="X5" s="101">
+      <c r="R5" s="134"/>
+      <c r="S5" s="134"/>
+      <c r="T5" s="134"/>
+      <c r="U5" s="134"/>
+      <c r="V5" s="134"/>
+      <c r="W5" s="134"/>
+      <c r="X5" s="134">
         <f>X6</f>
         <v>45229</v>
       </c>
-      <c r="Y5" s="101"/>
-      <c r="Z5" s="101"/>
-      <c r="AA5" s="101"/>
-      <c r="AB5" s="101"/>
-      <c r="AC5" s="101"/>
-      <c r="AD5" s="101"/>
-      <c r="AE5" s="101">
+      <c r="Y5" s="134"/>
+      <c r="Z5" s="134"/>
+      <c r="AA5" s="134"/>
+      <c r="AB5" s="134"/>
+      <c r="AC5" s="134"/>
+      <c r="AD5" s="134"/>
+      <c r="AE5" s="134">
         <f>AE6</f>
         <v>45236</v>
       </c>
-      <c r="AF5" s="101"/>
-      <c r="AG5" s="101"/>
-      <c r="AH5" s="101"/>
-      <c r="AI5" s="101"/>
-      <c r="AJ5" s="101"/>
-      <c r="AK5" s="101"/>
-      <c r="AL5" s="101">
+      <c r="AF5" s="134"/>
+      <c r="AG5" s="134"/>
+      <c r="AH5" s="134"/>
+      <c r="AI5" s="134"/>
+      <c r="AJ5" s="134"/>
+      <c r="AK5" s="134"/>
+      <c r="AL5" s="134">
         <f>AL6</f>
         <v>45243</v>
       </c>
-      <c r="AM5" s="101"/>
-      <c r="AN5" s="101"/>
-      <c r="AO5" s="101"/>
-      <c r="AP5" s="101"/>
-      <c r="AQ5" s="101"/>
-      <c r="AR5" s="101"/>
-      <c r="AS5" s="101">
+      <c r="AM5" s="134"/>
+      <c r="AN5" s="134"/>
+      <c r="AO5" s="134"/>
+      <c r="AP5" s="134"/>
+      <c r="AQ5" s="134"/>
+      <c r="AR5" s="134"/>
+      <c r="AS5" s="134">
         <f>AS6</f>
         <v>45250</v>
       </c>
-      <c r="AT5" s="101"/>
-      <c r="AU5" s="101"/>
-      <c r="AV5" s="101"/>
-      <c r="AW5" s="101"/>
-      <c r="AX5" s="101"/>
-      <c r="AY5" s="101"/>
-      <c r="AZ5" s="101">
+      <c r="AT5" s="134"/>
+      <c r="AU5" s="134"/>
+      <c r="AV5" s="134"/>
+      <c r="AW5" s="134"/>
+      <c r="AX5" s="134"/>
+      <c r="AY5" s="134"/>
+      <c r="AZ5" s="134">
         <f>AZ6</f>
         <v>45257</v>
       </c>
-      <c r="BA5" s="101"/>
-      <c r="BB5" s="101"/>
-      <c r="BC5" s="101"/>
-      <c r="BD5" s="101"/>
-      <c r="BE5" s="101"/>
-      <c r="BF5" s="101"/>
-      <c r="BG5" s="101">
+      <c r="BA5" s="134"/>
+      <c r="BB5" s="134"/>
+      <c r="BC5" s="134"/>
+      <c r="BD5" s="134"/>
+      <c r="BE5" s="134"/>
+      <c r="BF5" s="134"/>
+      <c r="BG5" s="134">
         <f>BG6</f>
         <v>45264</v>
       </c>
-      <c r="BH5" s="101"/>
-      <c r="BI5" s="101"/>
-      <c r="BJ5" s="101"/>
-      <c r="BK5" s="101"/>
-      <c r="BL5" s="101"/>
-      <c r="BM5" s="102"/>
-      <c r="BN5" s="101">
+      <c r="BH5" s="134"/>
+      <c r="BI5" s="134"/>
+      <c r="BJ5" s="134"/>
+      <c r="BK5" s="134"/>
+      <c r="BL5" s="134"/>
+      <c r="BM5" s="135"/>
+      <c r="BN5" s="134">
         <f>BN6</f>
         <v>45271</v>
       </c>
-      <c r="BO5" s="101"/>
-      <c r="BP5" s="101"/>
-      <c r="BQ5" s="101"/>
-      <c r="BR5" s="101"/>
-      <c r="BS5" s="101"/>
-      <c r="BT5" s="102"/>
+      <c r="BO5" s="134"/>
+      <c r="BP5" s="134"/>
+      <c r="BQ5" s="134"/>
+      <c r="BR5" s="134"/>
+      <c r="BS5" s="134"/>
+      <c r="BT5" s="135"/>
     </row>
     <row r="6" spans="1:72" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="106"/>
-      <c r="B6" s="107" t="s">
+      <c r="A6" s="137"/>
+      <c r="B6" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="109" t="s">
+      <c r="C6" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="104" t="s">
+      <c r="D6" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="104" t="s">
+      <c r="E6" s="142" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="104" t="s">
+      <c r="F6" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="104" t="s">
+      <c r="G6" s="142" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="29">
@@ -2890,15 +2892,15 @@
         <f t="shared" si="0"/>
         <v>45220</v>
       </c>
-      <c r="P6" s="112">
+      <c r="P6" s="103">
         <f t="shared" si="0"/>
         <v>45221</v>
       </c>
-      <c r="Q6" s="120">
+      <c r="Q6" s="111">
         <f>P6+1</f>
         <v>45222</v>
       </c>
-      <c r="R6" s="111">
+      <c r="R6" s="102">
         <f>Q6+1</f>
         <v>45223</v>
       </c>
@@ -3014,23 +3016,23 @@
         <f>AS6+1</f>
         <v>45251</v>
       </c>
-      <c r="AU6" s="111">
+      <c r="AU6" s="102">
         <f t="shared" si="0"/>
         <v>45252</v>
       </c>
-      <c r="AV6" s="111">
+      <c r="AV6" s="102">
         <f t="shared" si="0"/>
         <v>45253</v>
       </c>
-      <c r="AW6" s="111">
+      <c r="AW6" s="102">
         <f t="shared" si="0"/>
         <v>45254</v>
       </c>
-      <c r="AX6" s="111">
+      <c r="AX6" s="102">
         <f t="shared" si="0"/>
         <v>45255</v>
       </c>
-      <c r="AY6" s="112">
+      <c r="AY6" s="103">
         <f t="shared" si="0"/>
         <v>45256</v>
       </c>
@@ -3120,13 +3122,13 @@
       </c>
     </row>
     <row r="7" spans="1:72" s="24" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="106"/>
-      <c r="B7" s="108"/>
-      <c r="C7" s="105"/>
-      <c r="D7" s="105"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="105"/>
+      <c r="A7" s="137"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="141"/>
+      <c r="E7" s="141"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="141"/>
       <c r="J7" s="32" t="str">
         <f t="shared" ref="J7:AO7" si="8">LEFT(TEXT(J6,"ddd"),1)</f>
         <v>M</v>
@@ -3151,15 +3153,15 @@
         <f t="shared" si="8"/>
         <v>S</v>
       </c>
-      <c r="P7" s="113" t="str">
+      <c r="P7" s="104" t="str">
         <f t="shared" si="8"/>
         <v>S</v>
       </c>
-      <c r="Q7" s="113" t="str">
+      <c r="Q7" s="104" t="str">
         <f t="shared" si="8"/>
         <v>M</v>
       </c>
-      <c r="R7" s="113" t="str">
+      <c r="R7" s="104" t="str">
         <f t="shared" si="8"/>
         <v>T</v>
       </c>
@@ -3275,23 +3277,23 @@
         <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="AU7" s="113" t="str">
+      <c r="AU7" s="104" t="str">
         <f t="shared" si="9"/>
         <v>W</v>
       </c>
-      <c r="AV7" s="113" t="str">
+      <c r="AV7" s="104" t="str">
         <f t="shared" si="9"/>
         <v>T</v>
       </c>
-      <c r="AW7" s="113" t="str">
+      <c r="AW7" s="104" t="str">
         <f t="shared" si="9"/>
         <v>F</v>
       </c>
-      <c r="AX7" s="113" t="str">
+      <c r="AX7" s="104" t="str">
         <f t="shared" si="9"/>
         <v>S</v>
       </c>
-      <c r="AY7" s="113" t="str">
+      <c r="AY7" s="104" t="str">
         <f t="shared" si="9"/>
         <v>S</v>
       </c>
@@ -3400,9 +3402,9 @@
       <c r="M8" s="37"/>
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
-      <c r="P8" s="114"/>
-      <c r="Q8" s="114"/>
-      <c r="R8" s="114"/>
+      <c r="P8" s="105"/>
+      <c r="Q8" s="105"/>
+      <c r="R8" s="105"/>
       <c r="S8" s="37"/>
       <c r="T8" s="37"/>
       <c r="U8" s="37"/>
@@ -3431,11 +3433,11 @@
       <c r="AR8" s="37"/>
       <c r="AS8" s="37"/>
       <c r="AT8" s="37"/>
-      <c r="AU8" s="114"/>
-      <c r="AV8" s="114"/>
-      <c r="AW8" s="114"/>
-      <c r="AX8" s="114"/>
-      <c r="AY8" s="114"/>
+      <c r="AU8" s="105"/>
+      <c r="AV8" s="105"/>
+      <c r="AW8" s="105"/>
+      <c r="AX8" s="105"/>
+      <c r="AY8" s="105"/>
       <c r="AZ8" s="37"/>
       <c r="BA8" s="37"/>
       <c r="BB8" s="37"/>
@@ -3465,12 +3467,12 @@
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="130"/>
+      <c r="E9" s="115"/>
       <c r="F9" s="41"/>
       <c r="G9" s="42"/>
       <c r="H9" s="16"/>
       <c r="I9" s="5" t="str">
-        <f t="shared" ref="I9:I41" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="I9:I42" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="J9" s="43"/>
@@ -3479,11 +3481,11 @@
       <c r="M9" s="43"/>
       <c r="N9" s="43"/>
       <c r="O9" s="43"/>
-      <c r="P9" s="115" t="s">
+      <c r="P9" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="Q9" s="115"/>
-      <c r="R9" s="115"/>
+      <c r="Q9" s="106"/>
+      <c r="R9" s="106"/>
       <c r="S9" s="43"/>
       <c r="T9" s="43"/>
       <c r="U9" s="43"/>
@@ -3512,13 +3514,13 @@
       <c r="AR9" s="43"/>
       <c r="AS9" s="43"/>
       <c r="AT9" s="43"/>
-      <c r="AU9" s="115" t="s">
+      <c r="AU9" s="106" t="s">
         <v>34</v>
       </c>
-      <c r="AV9" s="115"/>
-      <c r="AW9" s="115"/>
-      <c r="AX9" s="115"/>
-      <c r="AY9" s="115"/>
+      <c r="AV9" s="106"/>
+      <c r="AW9" s="106"/>
+      <c r="AX9" s="106"/>
+      <c r="AY9" s="106"/>
       <c r="AZ9" s="43"/>
       <c r="BA9" s="43"/>
       <c r="BB9" s="43"/>
@@ -3533,15 +3535,15 @@
       <c r="BK9" s="43"/>
       <c r="BL9" s="43"/>
       <c r="BM9" s="43"/>
-      <c r="BN9" s="115" t="s">
+      <c r="BN9" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="BO9" s="115"/>
-      <c r="BP9" s="115"/>
-      <c r="BQ9" s="115"/>
-      <c r="BR9" s="115"/>
-      <c r="BS9" s="115"/>
-      <c r="BT9" s="115"/>
+      <c r="BO9" s="106"/>
+      <c r="BP9" s="106"/>
+      <c r="BQ9" s="106"/>
+      <c r="BR9" s="106"/>
+      <c r="BS9" s="106"/>
+      <c r="BT9" s="106"/>
     </row>
     <row r="10" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="13"/>
@@ -3554,7 +3556,7 @@
       <c r="D10" s="47">
         <v>0.5</v>
       </c>
-      <c r="E10" s="129" t="s">
+      <c r="E10" s="114" t="s">
         <v>93</v>
       </c>
       <c r="F10" s="48">
@@ -3575,9 +3577,9 @@
       <c r="M10" s="49"/>
       <c r="N10" s="49"/>
       <c r="O10" s="49"/>
-      <c r="P10" s="116"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="116"/>
+      <c r="P10" s="107"/>
+      <c r="Q10" s="107"/>
+      <c r="R10" s="107"/>
       <c r="S10" s="49"/>
       <c r="T10" s="49"/>
       <c r="U10" s="49"/>
@@ -3606,11 +3608,11 @@
       <c r="AR10" s="49"/>
       <c r="AS10" s="49"/>
       <c r="AT10" s="49"/>
-      <c r="AU10" s="116"/>
-      <c r="AV10" s="116"/>
-      <c r="AW10" s="116"/>
-      <c r="AX10" s="116"/>
-      <c r="AY10" s="116"/>
+      <c r="AU10" s="107"/>
+      <c r="AV10" s="107"/>
+      <c r="AW10" s="107"/>
+      <c r="AX10" s="107"/>
+      <c r="AY10" s="107"/>
       <c r="AZ10" s="49"/>
       <c r="BA10" s="49"/>
       <c r="BB10" s="49"/>
@@ -3625,13 +3627,13 @@
       <c r="BK10" s="49"/>
       <c r="BL10" s="49"/>
       <c r="BM10" s="49"/>
-      <c r="BN10" s="116"/>
-      <c r="BO10" s="116"/>
-      <c r="BP10" s="116"/>
-      <c r="BQ10" s="116"/>
-      <c r="BR10" s="116"/>
-      <c r="BS10" s="116"/>
-      <c r="BT10" s="116"/>
+      <c r="BN10" s="107"/>
+      <c r="BO10" s="107"/>
+      <c r="BP10" s="107"/>
+      <c r="BQ10" s="107"/>
+      <c r="BR10" s="107"/>
+      <c r="BS10" s="107"/>
+      <c r="BT10" s="107"/>
     </row>
     <row r="11" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
@@ -3644,7 +3646,7 @@
       <c r="D11" s="47">
         <v>0.5</v>
       </c>
-      <c r="E11" s="129" t="s">
+      <c r="E11" s="114" t="s">
         <v>93</v>
       </c>
       <c r="F11" s="48">
@@ -3665,9 +3667,9 @@
       <c r="M11" s="49"/>
       <c r="N11" s="49"/>
       <c r="O11" s="49"/>
-      <c r="P11" s="116"/>
-      <c r="Q11" s="116"/>
-      <c r="R11" s="116"/>
+      <c r="P11" s="107"/>
+      <c r="Q11" s="107"/>
+      <c r="R11" s="107"/>
       <c r="S11" s="49"/>
       <c r="T11" s="49"/>
       <c r="U11" s="49"/>
@@ -3696,11 +3698,11 @@
       <c r="AR11" s="49"/>
       <c r="AS11" s="49"/>
       <c r="AT11" s="49"/>
-      <c r="AU11" s="116"/>
-      <c r="AV11" s="116"/>
-      <c r="AW11" s="116"/>
-      <c r="AX11" s="116"/>
-      <c r="AY11" s="116"/>
+      <c r="AU11" s="107"/>
+      <c r="AV11" s="107"/>
+      <c r="AW11" s="107"/>
+      <c r="AX11" s="107"/>
+      <c r="AY11" s="107"/>
       <c r="AZ11" s="49"/>
       <c r="BA11" s="49"/>
       <c r="BB11" s="49"/>
@@ -3715,13 +3717,13 @@
       <c r="BK11" s="49"/>
       <c r="BL11" s="49"/>
       <c r="BM11" s="49"/>
-      <c r="BN11" s="116"/>
-      <c r="BO11" s="116"/>
-      <c r="BP11" s="116"/>
-      <c r="BQ11" s="116"/>
-      <c r="BR11" s="116"/>
-      <c r="BS11" s="116"/>
-      <c r="BT11" s="116"/>
+      <c r="BN11" s="107"/>
+      <c r="BO11" s="107"/>
+      <c r="BP11" s="107"/>
+      <c r="BQ11" s="107"/>
+      <c r="BR11" s="107"/>
+      <c r="BS11" s="107"/>
+      <c r="BT11" s="107"/>
     </row>
     <row r="12" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="13"/>
@@ -3734,7 +3736,7 @@
       <c r="D12" s="47">
         <v>1</v>
       </c>
-      <c r="E12" s="129">
+      <c r="E12" s="114">
         <v>0</v>
       </c>
       <c r="F12" s="48">
@@ -3756,9 +3758,9 @@
       <c r="M12" s="49"/>
       <c r="N12" s="49"/>
       <c r="O12" s="49"/>
-      <c r="P12" s="116"/>
-      <c r="Q12" s="116"/>
-      <c r="R12" s="116"/>
+      <c r="P12" s="107"/>
+      <c r="Q12" s="107"/>
+      <c r="R12" s="107"/>
       <c r="S12" s="49"/>
       <c r="T12" s="49"/>
       <c r="U12" s="49"/>
@@ -3787,11 +3789,11 @@
       <c r="AR12" s="49"/>
       <c r="AS12" s="49"/>
       <c r="AT12" s="49"/>
-      <c r="AU12" s="116"/>
-      <c r="AV12" s="116"/>
-      <c r="AW12" s="116"/>
-      <c r="AX12" s="116"/>
-      <c r="AY12" s="116"/>
+      <c r="AU12" s="107"/>
+      <c r="AV12" s="107"/>
+      <c r="AW12" s="107"/>
+      <c r="AX12" s="107"/>
+      <c r="AY12" s="107"/>
       <c r="AZ12" s="49"/>
       <c r="BA12" s="49"/>
       <c r="BB12" s="49"/>
@@ -3806,13 +3808,13 @@
       <c r="BK12" s="49"/>
       <c r="BL12" s="49"/>
       <c r="BM12" s="49"/>
-      <c r="BN12" s="116"/>
-      <c r="BO12" s="116"/>
-      <c r="BP12" s="116"/>
-      <c r="BQ12" s="116"/>
-      <c r="BR12" s="116"/>
-      <c r="BS12" s="116"/>
-      <c r="BT12" s="116"/>
+      <c r="BN12" s="107"/>
+      <c r="BO12" s="107"/>
+      <c r="BP12" s="107"/>
+      <c r="BQ12" s="107"/>
+      <c r="BR12" s="107"/>
+      <c r="BS12" s="107"/>
+      <c r="BT12" s="107"/>
     </row>
     <row r="13" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13"/>
@@ -3825,7 +3827,7 @@
       <c r="D13" s="47">
         <v>0.5</v>
       </c>
-      <c r="E13" s="138" t="s">
+      <c r="E13" s="123" t="s">
         <v>92</v>
       </c>
       <c r="F13" s="53">
@@ -3847,9 +3849,9 @@
       <c r="M13" s="49"/>
       <c r="N13" s="49"/>
       <c r="O13" s="49"/>
-      <c r="P13" s="116"/>
-      <c r="Q13" s="116"/>
-      <c r="R13" s="116"/>
+      <c r="P13" s="107"/>
+      <c r="Q13" s="107"/>
+      <c r="R13" s="107"/>
       <c r="S13" s="49"/>
       <c r="T13" s="49"/>
       <c r="U13" s="49"/>
@@ -3878,11 +3880,11 @@
       <c r="AR13" s="49"/>
       <c r="AS13" s="49"/>
       <c r="AT13" s="49"/>
-      <c r="AU13" s="116"/>
-      <c r="AV13" s="116"/>
-      <c r="AW13" s="116"/>
-      <c r="AX13" s="116"/>
-      <c r="AY13" s="116"/>
+      <c r="AU13" s="107"/>
+      <c r="AV13" s="107"/>
+      <c r="AW13" s="107"/>
+      <c r="AX13" s="107"/>
+      <c r="AY13" s="107"/>
       <c r="AZ13" s="49"/>
       <c r="BA13" s="49"/>
       <c r="BB13" s="49"/>
@@ -3897,13 +3899,13 @@
       <c r="BK13" s="49"/>
       <c r="BL13" s="49"/>
       <c r="BM13" s="49"/>
-      <c r="BN13" s="116"/>
-      <c r="BO13" s="116"/>
-      <c r="BP13" s="116"/>
-      <c r="BQ13" s="116"/>
-      <c r="BR13" s="116"/>
-      <c r="BS13" s="116"/>
-      <c r="BT13" s="116"/>
+      <c r="BN13" s="107"/>
+      <c r="BO13" s="107"/>
+      <c r="BP13" s="107"/>
+      <c r="BQ13" s="107"/>
+      <c r="BR13" s="107"/>
+      <c r="BS13" s="107"/>
+      <c r="BT13" s="107"/>
     </row>
     <row r="14" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="13"/>
@@ -3916,7 +3918,7 @@
       <c r="D14" s="52">
         <v>0.05</v>
       </c>
-      <c r="E14" s="138" t="s">
+      <c r="E14" s="123" t="s">
         <v>91</v>
       </c>
       <c r="F14" s="53">
@@ -3935,9 +3937,9 @@
       <c r="M14" s="49"/>
       <c r="N14" s="49"/>
       <c r="O14" s="49"/>
-      <c r="P14" s="116"/>
-      <c r="Q14" s="116"/>
-      <c r="R14" s="116"/>
+      <c r="P14" s="107"/>
+      <c r="Q14" s="107"/>
+      <c r="R14" s="107"/>
       <c r="S14" s="49"/>
       <c r="T14" s="49"/>
       <c r="U14" s="49"/>
@@ -3966,11 +3968,11 @@
       <c r="AR14" s="49"/>
       <c r="AS14" s="49"/>
       <c r="AT14" s="49"/>
-      <c r="AU14" s="116"/>
-      <c r="AV14" s="116"/>
-      <c r="AW14" s="116"/>
-      <c r="AX14" s="116"/>
-      <c r="AY14" s="116"/>
+      <c r="AU14" s="107"/>
+      <c r="AV14" s="107"/>
+      <c r="AW14" s="107"/>
+      <c r="AX14" s="107"/>
+      <c r="AY14" s="107"/>
       <c r="AZ14" s="49"/>
       <c r="BA14" s="49"/>
       <c r="BB14" s="49"/>
@@ -3985,13 +3987,13 @@
       <c r="BK14" s="49"/>
       <c r="BL14" s="49"/>
       <c r="BM14" s="49"/>
-      <c r="BN14" s="116"/>
-      <c r="BO14" s="116"/>
-      <c r="BP14" s="116"/>
-      <c r="BQ14" s="116"/>
-      <c r="BR14" s="116"/>
-      <c r="BS14" s="116"/>
-      <c r="BT14" s="116"/>
+      <c r="BN14" s="107"/>
+      <c r="BO14" s="107"/>
+      <c r="BP14" s="107"/>
+      <c r="BQ14" s="107"/>
+      <c r="BR14" s="107"/>
+      <c r="BS14" s="107"/>
+      <c r="BT14" s="107"/>
     </row>
     <row r="15" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="12"/>
@@ -4004,7 +4006,7 @@
       <c r="D15" s="52">
         <v>0.4</v>
       </c>
-      <c r="E15" s="129" t="s">
+      <c r="E15" s="114" t="s">
         <v>92</v>
       </c>
       <c r="F15" s="53">
@@ -4026,9 +4028,9 @@
       <c r="M15" s="49"/>
       <c r="N15" s="49"/>
       <c r="O15" s="49"/>
-      <c r="P15" s="116"/>
-      <c r="Q15" s="116"/>
-      <c r="R15" s="116"/>
+      <c r="P15" s="107"/>
+      <c r="Q15" s="107"/>
+      <c r="R15" s="107"/>
       <c r="S15" s="49"/>
       <c r="T15" s="49"/>
       <c r="U15" s="49"/>
@@ -4057,11 +4059,11 @@
       <c r="AR15" s="49"/>
       <c r="AS15" s="49"/>
       <c r="AT15" s="49"/>
-      <c r="AU15" s="116"/>
-      <c r="AV15" s="116"/>
-      <c r="AW15" s="116"/>
-      <c r="AX15" s="116"/>
-      <c r="AY15" s="116"/>
+      <c r="AU15" s="107"/>
+      <c r="AV15" s="107"/>
+      <c r="AW15" s="107"/>
+      <c r="AX15" s="107"/>
+      <c r="AY15" s="107"/>
       <c r="AZ15" s="49"/>
       <c r="BA15" s="49"/>
       <c r="BB15" s="49"/>
@@ -4076,13 +4078,13 @@
       <c r="BK15" s="49"/>
       <c r="BL15" s="49"/>
       <c r="BM15" s="49"/>
-      <c r="BN15" s="116"/>
-      <c r="BO15" s="116"/>
-      <c r="BP15" s="116"/>
-      <c r="BQ15" s="116"/>
-      <c r="BR15" s="116"/>
-      <c r="BS15" s="116"/>
-      <c r="BT15" s="116"/>
+      <c r="BN15" s="107"/>
+      <c r="BO15" s="107"/>
+      <c r="BP15" s="107"/>
+      <c r="BQ15" s="107"/>
+      <c r="BR15" s="107"/>
+      <c r="BS15" s="107"/>
+      <c r="BT15" s="107"/>
     </row>
     <row r="16" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="12"/>
@@ -4095,7 +4097,7 @@
       <c r="D16" s="52">
         <v>0</v>
       </c>
-      <c r="E16" s="138" t="s">
+      <c r="E16" s="123" t="s">
         <v>72</v>
       </c>
       <c r="F16" s="53">
@@ -4117,9 +4119,9 @@
       <c r="M16" s="49"/>
       <c r="N16" s="49"/>
       <c r="O16" s="49"/>
-      <c r="P16" s="116"/>
-      <c r="Q16" s="116"/>
-      <c r="R16" s="116"/>
+      <c r="P16" s="107"/>
+      <c r="Q16" s="107"/>
+      <c r="R16" s="107"/>
       <c r="S16" s="49"/>
       <c r="T16" s="49"/>
       <c r="U16" s="49"/>
@@ -4148,11 +4150,11 @@
       <c r="AR16" s="49"/>
       <c r="AS16" s="49"/>
       <c r="AT16" s="49"/>
-      <c r="AU16" s="116"/>
-      <c r="AV16" s="116"/>
-      <c r="AW16" s="116"/>
-      <c r="AX16" s="116"/>
-      <c r="AY16" s="116"/>
+      <c r="AU16" s="107"/>
+      <c r="AV16" s="107"/>
+      <c r="AW16" s="107"/>
+      <c r="AX16" s="107"/>
+      <c r="AY16" s="107"/>
       <c r="AZ16" s="49"/>
       <c r="BA16" s="49"/>
       <c r="BB16" s="49"/>
@@ -4167,13 +4169,13 @@
       <c r="BK16" s="49"/>
       <c r="BL16" s="49"/>
       <c r="BM16" s="49"/>
-      <c r="BN16" s="116"/>
-      <c r="BO16" s="116"/>
-      <c r="BP16" s="116"/>
-      <c r="BQ16" s="116"/>
-      <c r="BR16" s="116"/>
-      <c r="BS16" s="116"/>
-      <c r="BT16" s="116"/>
+      <c r="BN16" s="107"/>
+      <c r="BO16" s="107"/>
+      <c r="BP16" s="107"/>
+      <c r="BQ16" s="107"/>
+      <c r="BR16" s="107"/>
+      <c r="BS16" s="107"/>
+      <c r="BT16" s="107"/>
     </row>
     <row r="17" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="12"/>
@@ -4186,7 +4188,7 @@
       <c r="D17" s="52">
         <v>1</v>
       </c>
-      <c r="E17" s="138" t="s">
+      <c r="E17" s="123" t="s">
         <v>89</v>
       </c>
       <c r="F17" s="53">
@@ -4208,9 +4210,9 @@
       <c r="M17" s="49"/>
       <c r="N17" s="49"/>
       <c r="O17" s="49"/>
-      <c r="P17" s="116"/>
-      <c r="Q17" s="116"/>
-      <c r="R17" s="116"/>
+      <c r="P17" s="107"/>
+      <c r="Q17" s="107"/>
+      <c r="R17" s="107"/>
       <c r="S17" s="49"/>
       <c r="T17" s="49"/>
       <c r="U17" s="49"/>
@@ -4239,11 +4241,11 @@
       <c r="AR17" s="49"/>
       <c r="AS17" s="49"/>
       <c r="AT17" s="49"/>
-      <c r="AU17" s="116"/>
-      <c r="AV17" s="116"/>
-      <c r="AW17" s="116"/>
-      <c r="AX17" s="116"/>
-      <c r="AY17" s="116"/>
+      <c r="AU17" s="107"/>
+      <c r="AV17" s="107"/>
+      <c r="AW17" s="107"/>
+      <c r="AX17" s="107"/>
+      <c r="AY17" s="107"/>
       <c r="AZ17" s="49"/>
       <c r="BA17" s="49"/>
       <c r="BB17" s="49"/>
@@ -4258,13 +4260,13 @@
       <c r="BK17" s="49"/>
       <c r="BL17" s="49"/>
       <c r="BM17" s="49"/>
-      <c r="BN17" s="116"/>
-      <c r="BO17" s="116"/>
-      <c r="BP17" s="116"/>
-      <c r="BQ17" s="116"/>
-      <c r="BR17" s="116"/>
-      <c r="BS17" s="116"/>
-      <c r="BT17" s="116"/>
+      <c r="BN17" s="107"/>
+      <c r="BO17" s="107"/>
+      <c r="BP17" s="107"/>
+      <c r="BQ17" s="107"/>
+      <c r="BR17" s="107"/>
+      <c r="BS17" s="107"/>
+      <c r="BT17" s="107"/>
     </row>
     <row r="18" spans="1:72" s="44" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="13"/>
@@ -4273,7 +4275,7 @@
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="57"/>
-      <c r="E18" s="131"/>
+      <c r="E18" s="116"/>
       <c r="F18" s="58"/>
       <c r="G18" s="59"/>
       <c r="H18" s="16"/>
@@ -4281,21 +4283,21 @@
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="P18" s="117"/>
-      <c r="Q18" s="117"/>
-      <c r="R18" s="117"/>
-      <c r="AU18" s="117"/>
-      <c r="AV18" s="117"/>
-      <c r="AW18" s="117"/>
-      <c r="AX18" s="117"/>
-      <c r="AY18" s="117"/>
-      <c r="BN18" s="117"/>
-      <c r="BO18" s="117"/>
-      <c r="BP18" s="117"/>
-      <c r="BQ18" s="117"/>
-      <c r="BR18" s="117"/>
-      <c r="BS18" s="117"/>
-      <c r="BT18" s="117"/>
+      <c r="P18" s="108"/>
+      <c r="Q18" s="108"/>
+      <c r="R18" s="108"/>
+      <c r="AU18" s="108"/>
+      <c r="AV18" s="108"/>
+      <c r="AW18" s="108"/>
+      <c r="AX18" s="108"/>
+      <c r="AY18" s="108"/>
+      <c r="BN18" s="108"/>
+      <c r="BO18" s="108"/>
+      <c r="BP18" s="108"/>
+      <c r="BQ18" s="108"/>
+      <c r="BR18" s="108"/>
+      <c r="BS18" s="108"/>
+      <c r="BT18" s="108"/>
     </row>
     <row r="19" spans="1:72" s="44" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="13"/>
@@ -4308,7 +4310,7 @@
       <c r="D19" s="62">
         <v>0.5</v>
       </c>
-      <c r="E19" s="132"/>
+      <c r="E19" s="117"/>
       <c r="F19" s="63" t="e">
         <f>#REF!-2</f>
         <v>#REF!</v>
@@ -4328,9 +4330,9 @@
       <c r="M19" s="49"/>
       <c r="N19" s="49"/>
       <c r="O19" s="49"/>
-      <c r="P19" s="116"/>
-      <c r="Q19" s="116"/>
-      <c r="R19" s="116"/>
+      <c r="P19" s="107"/>
+      <c r="Q19" s="107"/>
+      <c r="R19" s="107"/>
       <c r="S19" s="49"/>
       <c r="T19" s="49"/>
       <c r="U19" s="49"/>
@@ -4359,11 +4361,11 @@
       <c r="AR19" s="49"/>
       <c r="AS19" s="49"/>
       <c r="AT19" s="49"/>
-      <c r="AU19" s="116"/>
-      <c r="AV19" s="116"/>
-      <c r="AW19" s="116"/>
-      <c r="AX19" s="116"/>
-      <c r="AY19" s="116"/>
+      <c r="AU19" s="107"/>
+      <c r="AV19" s="107"/>
+      <c r="AW19" s="107"/>
+      <c r="AX19" s="107"/>
+      <c r="AY19" s="107"/>
       <c r="AZ19" s="49"/>
       <c r="BA19" s="49"/>
       <c r="BB19" s="49"/>
@@ -4378,13 +4380,13 @@
       <c r="BK19" s="49"/>
       <c r="BL19" s="49"/>
       <c r="BM19" s="49"/>
-      <c r="BN19" s="116"/>
-      <c r="BO19" s="116"/>
-      <c r="BP19" s="116"/>
-      <c r="BQ19" s="116"/>
-      <c r="BR19" s="116"/>
-      <c r="BS19" s="116"/>
-      <c r="BT19" s="116"/>
+      <c r="BN19" s="107"/>
+      <c r="BO19" s="107"/>
+      <c r="BP19" s="107"/>
+      <c r="BQ19" s="107"/>
+      <c r="BR19" s="107"/>
+      <c r="BS19" s="107"/>
+      <c r="BT19" s="107"/>
     </row>
     <row r="20" spans="1:72" s="44" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="12"/>
@@ -4397,7 +4399,7 @@
       <c r="D20" s="62">
         <v>0.5</v>
       </c>
-      <c r="E20" s="132"/>
+      <c r="E20" s="117"/>
       <c r="F20" s="63" t="e">
         <f>F19+2</f>
         <v>#REF!</v>
@@ -4417,9 +4419,9 @@
       <c r="M20" s="49"/>
       <c r="N20" s="49"/>
       <c r="O20" s="49"/>
-      <c r="P20" s="116"/>
-      <c r="Q20" s="116"/>
-      <c r="R20" s="116"/>
+      <c r="P20" s="107"/>
+      <c r="Q20" s="107"/>
+      <c r="R20" s="107"/>
       <c r="S20" s="49"/>
       <c r="T20" s="49"/>
       <c r="U20" s="49"/>
@@ -4448,11 +4450,11 @@
       <c r="AR20" s="49"/>
       <c r="AS20" s="49"/>
       <c r="AT20" s="49"/>
-      <c r="AU20" s="116"/>
-      <c r="AV20" s="116"/>
-      <c r="AW20" s="116"/>
-      <c r="AX20" s="116"/>
-      <c r="AY20" s="116"/>
+      <c r="AU20" s="107"/>
+      <c r="AV20" s="107"/>
+      <c r="AW20" s="107"/>
+      <c r="AX20" s="107"/>
+      <c r="AY20" s="107"/>
       <c r="AZ20" s="49"/>
       <c r="BA20" s="49"/>
       <c r="BB20" s="49"/>
@@ -4467,13 +4469,13 @@
       <c r="BK20" s="49"/>
       <c r="BL20" s="49"/>
       <c r="BM20" s="49"/>
-      <c r="BN20" s="116"/>
-      <c r="BO20" s="116"/>
-      <c r="BP20" s="116"/>
-      <c r="BQ20" s="116"/>
-      <c r="BR20" s="116"/>
-      <c r="BS20" s="116"/>
-      <c r="BT20" s="116"/>
+      <c r="BN20" s="107"/>
+      <c r="BO20" s="107"/>
+      <c r="BP20" s="107"/>
+      <c r="BQ20" s="107"/>
+      <c r="BR20" s="107"/>
+      <c r="BS20" s="107"/>
+      <c r="BT20" s="107"/>
     </row>
     <row r="21" spans="1:72" s="44" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="12"/>
@@ -4484,7 +4486,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="62"/>
-      <c r="E21" s="132"/>
+      <c r="E21" s="117"/>
       <c r="F21" s="63" t="e">
         <f>G20</f>
         <v>#REF!</v>
@@ -4504,9 +4506,9 @@
       <c r="M21" s="49"/>
       <c r="N21" s="49"/>
       <c r="O21" s="49"/>
-      <c r="P21" s="116"/>
-      <c r="Q21" s="116"/>
-      <c r="R21" s="116"/>
+      <c r="P21" s="107"/>
+      <c r="Q21" s="107"/>
+      <c r="R21" s="107"/>
       <c r="S21" s="49"/>
       <c r="T21" s="49"/>
       <c r="U21" s="49"/>
@@ -4535,11 +4537,11 @@
       <c r="AR21" s="49"/>
       <c r="AS21" s="49"/>
       <c r="AT21" s="49"/>
-      <c r="AU21" s="116"/>
-      <c r="AV21" s="116"/>
-      <c r="AW21" s="116"/>
-      <c r="AX21" s="116"/>
-      <c r="AY21" s="116"/>
+      <c r="AU21" s="107"/>
+      <c r="AV21" s="107"/>
+      <c r="AW21" s="107"/>
+      <c r="AX21" s="107"/>
+      <c r="AY21" s="107"/>
       <c r="AZ21" s="49"/>
       <c r="BA21" s="49"/>
       <c r="BB21" s="49"/>
@@ -4554,13 +4556,13 @@
       <c r="BK21" s="49"/>
       <c r="BL21" s="49"/>
       <c r="BM21" s="49"/>
-      <c r="BN21" s="116"/>
-      <c r="BO21" s="116"/>
-      <c r="BP21" s="116"/>
-      <c r="BQ21" s="116"/>
-      <c r="BR21" s="116"/>
-      <c r="BS21" s="116"/>
-      <c r="BT21" s="116"/>
+      <c r="BN21" s="107"/>
+      <c r="BO21" s="107"/>
+      <c r="BP21" s="107"/>
+      <c r="BQ21" s="107"/>
+      <c r="BR21" s="107"/>
+      <c r="BS21" s="107"/>
+      <c r="BT21" s="107"/>
     </row>
     <row r="22" spans="1:72" s="44" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="12"/>
@@ -4571,7 +4573,7 @@
         <v>24</v>
       </c>
       <c r="D22" s="62"/>
-      <c r="E22" s="132"/>
+      <c r="E22" s="117"/>
       <c r="F22" s="63" t="e">
         <f>F21</f>
         <v>#REF!</v>
@@ -4591,9 +4593,9 @@
       <c r="M22" s="49"/>
       <c r="N22" s="49"/>
       <c r="O22" s="49"/>
-      <c r="P22" s="116"/>
-      <c r="Q22" s="116"/>
-      <c r="R22" s="116"/>
+      <c r="P22" s="107"/>
+      <c r="Q22" s="107"/>
+      <c r="R22" s="107"/>
       <c r="S22" s="49"/>
       <c r="T22" s="49"/>
       <c r="U22" s="49"/>
@@ -4622,11 +4624,11 @@
       <c r="AR22" s="49"/>
       <c r="AS22" s="49"/>
       <c r="AT22" s="49"/>
-      <c r="AU22" s="116"/>
-      <c r="AV22" s="116"/>
-      <c r="AW22" s="116"/>
-      <c r="AX22" s="116"/>
-      <c r="AY22" s="116"/>
+      <c r="AU22" s="107"/>
+      <c r="AV22" s="107"/>
+      <c r="AW22" s="107"/>
+      <c r="AX22" s="107"/>
+      <c r="AY22" s="107"/>
       <c r="AZ22" s="49"/>
       <c r="BA22" s="49"/>
       <c r="BB22" s="49"/>
@@ -4641,13 +4643,13 @@
       <c r="BK22" s="49"/>
       <c r="BL22" s="49"/>
       <c r="BM22" s="49"/>
-      <c r="BN22" s="116"/>
-      <c r="BO22" s="116"/>
-      <c r="BP22" s="116"/>
-      <c r="BQ22" s="116"/>
-      <c r="BR22" s="116"/>
-      <c r="BS22" s="116"/>
-      <c r="BT22" s="116"/>
+      <c r="BN22" s="107"/>
+      <c r="BO22" s="107"/>
+      <c r="BP22" s="107"/>
+      <c r="BQ22" s="107"/>
+      <c r="BR22" s="107"/>
+      <c r="BS22" s="107"/>
+      <c r="BT22" s="107"/>
     </row>
     <row r="23" spans="1:72" s="44" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="12"/>
@@ -4658,7 +4660,7 @@
         <v>25</v>
       </c>
       <c r="D23" s="62"/>
-      <c r="E23" s="132"/>
+      <c r="E23" s="117"/>
       <c r="F23" s="63" t="e">
         <f>F22</f>
         <v>#REF!</v>
@@ -4678,9 +4680,9 @@
       <c r="M23" s="49"/>
       <c r="N23" s="49"/>
       <c r="O23" s="49"/>
-      <c r="P23" s="116"/>
-      <c r="Q23" s="116"/>
-      <c r="R23" s="116"/>
+      <c r="P23" s="107"/>
+      <c r="Q23" s="107"/>
+      <c r="R23" s="107"/>
       <c r="S23" s="49"/>
       <c r="T23" s="49"/>
       <c r="U23" s="49"/>
@@ -4709,11 +4711,11 @@
       <c r="AR23" s="49"/>
       <c r="AS23" s="49"/>
       <c r="AT23" s="49"/>
-      <c r="AU23" s="116"/>
-      <c r="AV23" s="116"/>
-      <c r="AW23" s="116"/>
-      <c r="AX23" s="116"/>
-      <c r="AY23" s="116"/>
+      <c r="AU23" s="107"/>
+      <c r="AV23" s="107"/>
+      <c r="AW23" s="107"/>
+      <c r="AX23" s="107"/>
+      <c r="AY23" s="107"/>
       <c r="AZ23" s="49"/>
       <c r="BA23" s="49"/>
       <c r="BB23" s="49"/>
@@ -4728,13 +4730,13 @@
       <c r="BK23" s="49"/>
       <c r="BL23" s="49"/>
       <c r="BM23" s="49"/>
-      <c r="BN23" s="116"/>
-      <c r="BO23" s="116"/>
-      <c r="BP23" s="116"/>
-      <c r="BQ23" s="116"/>
-      <c r="BR23" s="116"/>
-      <c r="BS23" s="116"/>
-      <c r="BT23" s="116"/>
+      <c r="BN23" s="107"/>
+      <c r="BO23" s="107"/>
+      <c r="BP23" s="107"/>
+      <c r="BQ23" s="107"/>
+      <c r="BR23" s="107"/>
+      <c r="BS23" s="107"/>
+      <c r="BT23" s="107"/>
     </row>
     <row r="24" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="12"/>
@@ -4743,7 +4745,7 @@
       </c>
       <c r="C24" s="65"/>
       <c r="D24" s="66"/>
-      <c r="E24" s="133"/>
+      <c r="E24" s="118"/>
       <c r="F24" s="67"/>
       <c r="G24" s="68"/>
       <c r="H24" s="16"/>
@@ -4757,9 +4759,9 @@
       <c r="M24" s="69"/>
       <c r="N24" s="69"/>
       <c r="O24" s="69"/>
-      <c r="P24" s="118"/>
-      <c r="Q24" s="118"/>
-      <c r="R24" s="118"/>
+      <c r="P24" s="109"/>
+      <c r="Q24" s="109"/>
+      <c r="R24" s="109"/>
       <c r="S24" s="69"/>
       <c r="T24" s="69"/>
       <c r="U24" s="69"/>
@@ -4788,11 +4790,11 @@
       <c r="AR24" s="69"/>
       <c r="AS24" s="69"/>
       <c r="AT24" s="69"/>
-      <c r="AU24" s="118"/>
-      <c r="AV24" s="118"/>
-      <c r="AW24" s="118"/>
-      <c r="AX24" s="118"/>
-      <c r="AY24" s="118"/>
+      <c r="AU24" s="109"/>
+      <c r="AV24" s="109"/>
+      <c r="AW24" s="109"/>
+      <c r="AX24" s="109"/>
+      <c r="AY24" s="109"/>
       <c r="AZ24" s="69"/>
       <c r="BA24" s="69"/>
       <c r="BB24" s="69"/>
@@ -4807,13 +4809,13 @@
       <c r="BK24" s="69"/>
       <c r="BL24" s="69"/>
       <c r="BM24" s="69"/>
-      <c r="BN24" s="118"/>
-      <c r="BO24" s="118"/>
-      <c r="BP24" s="118"/>
-      <c r="BQ24" s="118"/>
-      <c r="BR24" s="118"/>
-      <c r="BS24" s="118"/>
-      <c r="BT24" s="118"/>
+      <c r="BN24" s="109"/>
+      <c r="BO24" s="109"/>
+      <c r="BP24" s="109"/>
+      <c r="BQ24" s="109"/>
+      <c r="BR24" s="109"/>
+      <c r="BS24" s="109"/>
+      <c r="BT24" s="109"/>
     </row>
     <row r="25" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="12"/>
@@ -4824,9 +4826,9 @@
         <v>35</v>
       </c>
       <c r="D25" s="72">
-        <v>0</v>
-      </c>
-      <c r="E25" s="135">
+        <v>1</v>
+      </c>
+      <c r="E25" s="120">
         <v>1</v>
       </c>
       <c r="F25" s="73">
@@ -4848,9 +4850,9 @@
       <c r="M25" s="49"/>
       <c r="N25" s="49"/>
       <c r="O25" s="49"/>
-      <c r="P25" s="116"/>
-      <c r="Q25" s="116"/>
-      <c r="R25" s="116"/>
+      <c r="P25" s="107"/>
+      <c r="Q25" s="107"/>
+      <c r="R25" s="107"/>
       <c r="S25" s="49"/>
       <c r="T25" s="49"/>
       <c r="U25" s="49"/>
@@ -4879,11 +4881,11 @@
       <c r="AR25" s="49"/>
       <c r="AS25" s="49"/>
       <c r="AT25" s="49"/>
-      <c r="AU25" s="116"/>
-      <c r="AV25" s="116"/>
-      <c r="AW25" s="116"/>
-      <c r="AX25" s="116"/>
-      <c r="AY25" s="116"/>
+      <c r="AU25" s="107"/>
+      <c r="AV25" s="107"/>
+      <c r="AW25" s="107"/>
+      <c r="AX25" s="107"/>
+      <c r="AY25" s="107"/>
       <c r="AZ25" s="49"/>
       <c r="BA25" s="49"/>
       <c r="BB25" s="49"/>
@@ -4898,13 +4900,13 @@
       <c r="BK25" s="49"/>
       <c r="BL25" s="49"/>
       <c r="BM25" s="49"/>
-      <c r="BN25" s="116"/>
-      <c r="BO25" s="116"/>
-      <c r="BP25" s="116"/>
-      <c r="BQ25" s="116"/>
-      <c r="BR25" s="116"/>
-      <c r="BS25" s="116"/>
-      <c r="BT25" s="116"/>
+      <c r="BN25" s="107"/>
+      <c r="BO25" s="107"/>
+      <c r="BP25" s="107"/>
+      <c r="BQ25" s="107"/>
+      <c r="BR25" s="107"/>
+      <c r="BS25" s="107"/>
+      <c r="BT25" s="107"/>
     </row>
     <row r="26" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="12"/>
@@ -4915,9 +4917,9 @@
         <v>35</v>
       </c>
       <c r="D26" s="72">
-        <v>0</v>
-      </c>
-      <c r="E26" s="135">
+        <v>1</v>
+      </c>
+      <c r="E26" s="120">
         <v>1</v>
       </c>
       <c r="F26" s="73">
@@ -4939,9 +4941,9 @@
       <c r="M26" s="49"/>
       <c r="N26" s="49"/>
       <c r="O26" s="49"/>
-      <c r="P26" s="116"/>
-      <c r="Q26" s="116"/>
-      <c r="R26" s="116"/>
+      <c r="P26" s="107"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="107"/>
       <c r="S26" s="49"/>
       <c r="T26" s="49"/>
       <c r="U26" s="49"/>
@@ -4970,11 +4972,11 @@
       <c r="AR26" s="49"/>
       <c r="AS26" s="49"/>
       <c r="AT26" s="49"/>
-      <c r="AU26" s="116"/>
-      <c r="AV26" s="116"/>
-      <c r="AW26" s="116"/>
-      <c r="AX26" s="116"/>
-      <c r="AY26" s="116"/>
+      <c r="AU26" s="107"/>
+      <c r="AV26" s="107"/>
+      <c r="AW26" s="107"/>
+      <c r="AX26" s="107"/>
+      <c r="AY26" s="107"/>
       <c r="AZ26" s="49"/>
       <c r="BA26" s="49"/>
       <c r="BB26" s="49"/>
@@ -4989,26 +4991,26 @@
       <c r="BK26" s="49"/>
       <c r="BL26" s="49"/>
       <c r="BM26" s="49"/>
-      <c r="BN26" s="116"/>
-      <c r="BO26" s="116"/>
-      <c r="BP26" s="116"/>
-      <c r="BQ26" s="116"/>
-      <c r="BR26" s="116"/>
-      <c r="BS26" s="116"/>
-      <c r="BT26" s="116"/>
+      <c r="BN26" s="107"/>
+      <c r="BO26" s="107"/>
+      <c r="BP26" s="107"/>
+      <c r="BQ26" s="107"/>
+      <c r="BR26" s="107"/>
+      <c r="BS26" s="107"/>
+      <c r="BT26" s="107"/>
     </row>
     <row r="27" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="12"/>
       <c r="B27" s="70" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="C27" s="71" t="s">
         <v>35</v>
       </c>
       <c r="D27" s="72">
-        <v>0</v>
-      </c>
-      <c r="E27" s="135">
+        <v>0.1</v>
+      </c>
+      <c r="E27" s="120">
         <v>2</v>
       </c>
       <c r="F27" s="73">
@@ -5030,9 +5032,9 @@
       <c r="M27" s="49"/>
       <c r="N27" s="49"/>
       <c r="O27" s="49"/>
-      <c r="P27" s="116"/>
-      <c r="Q27" s="116"/>
-      <c r="R27" s="116"/>
+      <c r="P27" s="107"/>
+      <c r="Q27" s="107"/>
+      <c r="R27" s="107"/>
       <c r="S27" s="49"/>
       <c r="T27" s="49"/>
       <c r="U27" s="49"/>
@@ -5061,11 +5063,11 @@
       <c r="AR27" s="49"/>
       <c r="AS27" s="49"/>
       <c r="AT27" s="49"/>
-      <c r="AU27" s="116"/>
-      <c r="AV27" s="116"/>
-      <c r="AW27" s="116"/>
-      <c r="AX27" s="116"/>
-      <c r="AY27" s="116"/>
+      <c r="AU27" s="107"/>
+      <c r="AV27" s="107"/>
+      <c r="AW27" s="107"/>
+      <c r="AX27" s="107"/>
+      <c r="AY27" s="107"/>
       <c r="AZ27" s="49"/>
       <c r="BA27" s="49"/>
       <c r="BB27" s="49"/>
@@ -5080,40 +5082,40 @@
       <c r="BK27" s="49"/>
       <c r="BL27" s="49"/>
       <c r="BM27" s="49"/>
-      <c r="BN27" s="116"/>
-      <c r="BO27" s="116"/>
-      <c r="BP27" s="116"/>
-      <c r="BQ27" s="116"/>
-      <c r="BR27" s="116"/>
-      <c r="BS27" s="116"/>
-      <c r="BT27" s="116"/>
+      <c r="BN27" s="107"/>
+      <c r="BO27" s="107"/>
+      <c r="BP27" s="107"/>
+      <c r="BQ27" s="107"/>
+      <c r="BR27" s="107"/>
+      <c r="BS27" s="107"/>
+      <c r="BT27" s="107"/>
     </row>
     <row r="28" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="12"/>
       <c r="B28" s="70" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C28" s="71" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="D28" s="72">
-        <v>0</v>
-      </c>
-      <c r="E28" s="135">
-        <v>2</v>
+        <v>0.05</v>
+      </c>
+      <c r="E28" s="121" t="s">
+        <v>55</v>
       </c>
       <c r="F28" s="73">
         <f>DATE(2023,10,23)</f>
         <v>45222</v>
       </c>
       <c r="G28" s="73">
-        <f>F28+6</f>
-        <v>45228</v>
+        <f>F28+13</f>
+        <v>45235</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="5">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J28" s="49"/>
       <c r="K28" s="49"/>
@@ -5121,9 +5123,9 @@
       <c r="M28" s="49"/>
       <c r="N28" s="49"/>
       <c r="O28" s="49"/>
-      <c r="P28" s="116"/>
-      <c r="Q28" s="116"/>
-      <c r="R28" s="116"/>
+      <c r="P28" s="107"/>
+      <c r="Q28" s="107"/>
+      <c r="R28" s="107"/>
       <c r="S28" s="49"/>
       <c r="T28" s="49"/>
       <c r="U28" s="49"/>
@@ -5152,11 +5154,11 @@
       <c r="AR28" s="49"/>
       <c r="AS28" s="49"/>
       <c r="AT28" s="49"/>
-      <c r="AU28" s="116"/>
-      <c r="AV28" s="116"/>
-      <c r="AW28" s="116"/>
-      <c r="AX28" s="116"/>
-      <c r="AY28" s="116"/>
+      <c r="AU28" s="107"/>
+      <c r="AV28" s="107"/>
+      <c r="AW28" s="107"/>
+      <c r="AX28" s="107"/>
+      <c r="AY28" s="107"/>
       <c r="AZ28" s="49"/>
       <c r="BA28" s="49"/>
       <c r="BB28" s="49"/>
@@ -5171,40 +5173,40 @@
       <c r="BK28" s="49"/>
       <c r="BL28" s="49"/>
       <c r="BM28" s="49"/>
-      <c r="BN28" s="116"/>
-      <c r="BO28" s="116"/>
-      <c r="BP28" s="116"/>
-      <c r="BQ28" s="116"/>
-      <c r="BR28" s="116"/>
-      <c r="BS28" s="116"/>
-      <c r="BT28" s="116"/>
+      <c r="BN28" s="107"/>
+      <c r="BO28" s="107"/>
+      <c r="BP28" s="107"/>
+      <c r="BQ28" s="107"/>
+      <c r="BR28" s="107"/>
+      <c r="BS28" s="107"/>
+      <c r="BT28" s="107"/>
     </row>
     <row r="29" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="12"/>
       <c r="B29" s="70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" s="71" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="D29" s="72">
         <v>0</v>
       </c>
-      <c r="E29" s="136" t="s">
-        <v>55</v>
+      <c r="E29" s="120">
+        <v>2</v>
       </c>
       <c r="F29" s="73">
-        <f>G26+1</f>
+        <f>DATE(2023,10,23)</f>
         <v>45222</v>
       </c>
       <c r="G29" s="73">
-        <f>F29+13</f>
-        <v>45235</v>
+        <f>F29+6</f>
+        <v>45228</v>
       </c>
       <c r="H29" s="16"/>
       <c r="I29" s="5">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="J29" s="49"/>
       <c r="K29" s="49"/>
@@ -5212,9 +5214,9 @@
       <c r="M29" s="49"/>
       <c r="N29" s="49"/>
       <c r="O29" s="49"/>
-      <c r="P29" s="116"/>
-      <c r="Q29" s="116"/>
-      <c r="R29" s="116"/>
+      <c r="P29" s="107"/>
+      <c r="Q29" s="107"/>
+      <c r="R29" s="107"/>
       <c r="S29" s="49"/>
       <c r="T29" s="49"/>
       <c r="U29" s="49"/>
@@ -5243,11 +5245,11 @@
       <c r="AR29" s="49"/>
       <c r="AS29" s="49"/>
       <c r="AT29" s="49"/>
-      <c r="AU29" s="116"/>
-      <c r="AV29" s="116"/>
-      <c r="AW29" s="116"/>
-      <c r="AX29" s="116"/>
-      <c r="AY29" s="116"/>
+      <c r="AU29" s="107"/>
+      <c r="AV29" s="107"/>
+      <c r="AW29" s="107"/>
+      <c r="AX29" s="107"/>
+      <c r="AY29" s="107"/>
       <c r="AZ29" s="49"/>
       <c r="BA29" s="49"/>
       <c r="BB29" s="49"/>
@@ -5262,47 +5264,50 @@
       <c r="BK29" s="49"/>
       <c r="BL29" s="49"/>
       <c r="BM29" s="49"/>
-      <c r="BN29" s="116"/>
-      <c r="BO29" s="116"/>
-      <c r="BP29" s="116"/>
-      <c r="BQ29" s="116"/>
-      <c r="BR29" s="116"/>
-      <c r="BS29" s="116"/>
-      <c r="BT29" s="116"/>
+      <c r="BN29" s="107"/>
+      <c r="BO29" s="107"/>
+      <c r="BP29" s="107"/>
+      <c r="BQ29" s="107"/>
+      <c r="BR29" s="107"/>
+      <c r="BS29" s="107"/>
+      <c r="BT29" s="107"/>
     </row>
     <row r="30" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="12"/>
       <c r="B30" s="70" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="C30" s="71" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D30" s="72">
         <v>0</v>
       </c>
-      <c r="E30" s="137" t="s">
-        <v>56</v>
+      <c r="E30" s="121" t="s">
+        <v>55</v>
       </c>
       <c r="F30" s="73">
-        <f>G28+1</f>
-        <v>45229</v>
+        <f>G26+1</f>
+        <v>45222</v>
       </c>
       <c r="G30" s="73">
         <f>F30+13</f>
-        <v>45242</v>
+        <v>45235</v>
       </c>
       <c r="H30" s="16"/>
-      <c r="I30" s="5"/>
+      <c r="I30" s="5">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
       <c r="J30" s="49"/>
       <c r="K30" s="49"/>
       <c r="L30" s="49"/>
       <c r="M30" s="49"/>
       <c r="N30" s="49"/>
       <c r="O30" s="49"/>
-      <c r="P30" s="116"/>
-      <c r="Q30" s="116"/>
-      <c r="R30" s="116"/>
+      <c r="P30" s="107"/>
+      <c r="Q30" s="107"/>
+      <c r="R30" s="107"/>
       <c r="S30" s="49"/>
       <c r="T30" s="49"/>
       <c r="U30" s="49"/>
@@ -5331,11 +5336,11 @@
       <c r="AR30" s="49"/>
       <c r="AS30" s="49"/>
       <c r="AT30" s="49"/>
-      <c r="AU30" s="116"/>
-      <c r="AV30" s="116"/>
-      <c r="AW30" s="116"/>
-      <c r="AX30" s="116"/>
-      <c r="AY30" s="116"/>
+      <c r="AU30" s="107"/>
+      <c r="AV30" s="107"/>
+      <c r="AW30" s="107"/>
+      <c r="AX30" s="107"/>
+      <c r="AY30" s="107"/>
       <c r="AZ30" s="49"/>
       <c r="BA30" s="49"/>
       <c r="BB30" s="49"/>
@@ -5350,18 +5355,18 @@
       <c r="BK30" s="49"/>
       <c r="BL30" s="49"/>
       <c r="BM30" s="49"/>
-      <c r="BN30" s="116"/>
-      <c r="BO30" s="116"/>
-      <c r="BP30" s="116"/>
-      <c r="BQ30" s="116"/>
-      <c r="BR30" s="116"/>
-      <c r="BS30" s="116"/>
-      <c r="BT30" s="116"/>
+      <c r="BN30" s="107"/>
+      <c r="BO30" s="107"/>
+      <c r="BP30" s="107"/>
+      <c r="BQ30" s="107"/>
+      <c r="BR30" s="107"/>
+      <c r="BS30" s="107"/>
+      <c r="BT30" s="107"/>
     </row>
     <row r="31" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="12"/>
       <c r="B31" s="70" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C31" s="71" t="s">
         <v>31</v>
@@ -5369,11 +5374,11 @@
       <c r="D31" s="72">
         <v>0</v>
       </c>
-      <c r="E31" s="137" t="s">
+      <c r="E31" s="122" t="s">
         <v>56</v>
       </c>
       <c r="F31" s="73">
-        <f>G28+1</f>
+        <f>G29+1</f>
         <v>45229</v>
       </c>
       <c r="G31" s="73">
@@ -5381,19 +5386,16 @@
         <v>45242</v>
       </c>
       <c r="H31" s="16"/>
-      <c r="I31" s="5">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
+      <c r="I31" s="5"/>
       <c r="J31" s="49"/>
       <c r="K31" s="49"/>
       <c r="L31" s="49"/>
       <c r="M31" s="49"/>
       <c r="N31" s="49"/>
       <c r="O31" s="49"/>
-      <c r="P31" s="116"/>
-      <c r="Q31" s="116"/>
-      <c r="R31" s="116"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="107"/>
+      <c r="R31" s="107"/>
       <c r="S31" s="49"/>
       <c r="T31" s="49"/>
       <c r="U31" s="49"/>
@@ -5422,11 +5424,11 @@
       <c r="AR31" s="49"/>
       <c r="AS31" s="49"/>
       <c r="AT31" s="49"/>
-      <c r="AU31" s="116"/>
-      <c r="AV31" s="116"/>
-      <c r="AW31" s="116"/>
-      <c r="AX31" s="116"/>
-      <c r="AY31" s="116"/>
+      <c r="AU31" s="107"/>
+      <c r="AV31" s="107"/>
+      <c r="AW31" s="107"/>
+      <c r="AX31" s="107"/>
+      <c r="AY31" s="107"/>
       <c r="AZ31" s="49"/>
       <c r="BA31" s="49"/>
       <c r="BB31" s="49"/>
@@ -5441,18 +5443,18 @@
       <c r="BK31" s="49"/>
       <c r="BL31" s="49"/>
       <c r="BM31" s="49"/>
-      <c r="BN31" s="116"/>
-      <c r="BO31" s="116"/>
-      <c r="BP31" s="116"/>
-      <c r="BQ31" s="116"/>
-      <c r="BR31" s="116"/>
-      <c r="BS31" s="116"/>
-      <c r="BT31" s="116"/>
+      <c r="BN31" s="107"/>
+      <c r="BO31" s="107"/>
+      <c r="BP31" s="107"/>
+      <c r="BQ31" s="107"/>
+      <c r="BR31" s="107"/>
+      <c r="BS31" s="107"/>
+      <c r="BT31" s="107"/>
     </row>
     <row r="32" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="12"/>
       <c r="B32" s="70" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="C32" s="71" t="s">
         <v>31</v>
@@ -5460,16 +5462,16 @@
       <c r="D32" s="72">
         <v>0</v>
       </c>
-      <c r="E32" s="135" t="s">
-        <v>63</v>
+      <c r="E32" s="122" t="s">
+        <v>56</v>
       </c>
       <c r="F32" s="73">
         <f>G29+1</f>
-        <v>45236</v>
+        <v>45229</v>
       </c>
       <c r="G32" s="73">
         <f>F32+13</f>
-        <v>45249</v>
+        <v>45242</v>
       </c>
       <c r="H32" s="16"/>
       <c r="I32" s="5">
@@ -5482,9 +5484,9 @@
       <c r="M32" s="49"/>
       <c r="N32" s="49"/>
       <c r="O32" s="49"/>
-      <c r="P32" s="116"/>
-      <c r="Q32" s="116"/>
-      <c r="R32" s="116"/>
+      <c r="P32" s="107"/>
+      <c r="Q32" s="107"/>
+      <c r="R32" s="107"/>
       <c r="S32" s="49"/>
       <c r="T32" s="49"/>
       <c r="U32" s="49"/>
@@ -5513,11 +5515,11 @@
       <c r="AR32" s="49"/>
       <c r="AS32" s="49"/>
       <c r="AT32" s="49"/>
-      <c r="AU32" s="116"/>
-      <c r="AV32" s="116"/>
-      <c r="AW32" s="116"/>
-      <c r="AX32" s="116"/>
-      <c r="AY32" s="116"/>
+      <c r="AU32" s="107"/>
+      <c r="AV32" s="107"/>
+      <c r="AW32" s="107"/>
+      <c r="AX32" s="107"/>
+      <c r="AY32" s="107"/>
       <c r="AZ32" s="49"/>
       <c r="BA32" s="49"/>
       <c r="BB32" s="49"/>
@@ -5532,18 +5534,18 @@
       <c r="BK32" s="49"/>
       <c r="BL32" s="49"/>
       <c r="BM32" s="49"/>
-      <c r="BN32" s="116"/>
-      <c r="BO32" s="116"/>
-      <c r="BP32" s="116"/>
-      <c r="BQ32" s="116"/>
-      <c r="BR32" s="116"/>
-      <c r="BS32" s="116"/>
-      <c r="BT32" s="116"/>
+      <c r="BN32" s="107"/>
+      <c r="BO32" s="107"/>
+      <c r="BP32" s="107"/>
+      <c r="BQ32" s="107"/>
+      <c r="BR32" s="107"/>
+      <c r="BS32" s="107"/>
+      <c r="BT32" s="107"/>
     </row>
     <row r="33" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="12"/>
       <c r="B33" s="70" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C33" s="71" t="s">
         <v>31</v>
@@ -5551,21 +5553,21 @@
       <c r="D33" s="72">
         <v>0</v>
       </c>
-      <c r="E33" s="135" t="s">
-        <v>64</v>
+      <c r="E33" s="120" t="s">
+        <v>63</v>
       </c>
       <c r="F33" s="73">
-        <f>G32+1</f>
-        <v>45250</v>
+        <f>G30+1</f>
+        <v>45236</v>
       </c>
       <c r="G33" s="73">
-        <f>F33+1</f>
-        <v>45251</v>
+        <f>F33+13</f>
+        <v>45249</v>
       </c>
       <c r="H33" s="16"/>
       <c r="I33" s="5">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J33" s="49"/>
       <c r="K33" s="49"/>
@@ -5573,9 +5575,9 @@
       <c r="M33" s="49"/>
       <c r="N33" s="49"/>
       <c r="O33" s="49"/>
-      <c r="P33" s="116"/>
-      <c r="Q33" s="116"/>
-      <c r="R33" s="116"/>
+      <c r="P33" s="107"/>
+      <c r="Q33" s="107"/>
+      <c r="R33" s="107"/>
       <c r="S33" s="49"/>
       <c r="T33" s="49"/>
       <c r="U33" s="49"/>
@@ -5604,11 +5606,11 @@
       <c r="AR33" s="49"/>
       <c r="AS33" s="49"/>
       <c r="AT33" s="49"/>
-      <c r="AU33" s="116"/>
-      <c r="AV33" s="116"/>
-      <c r="AW33" s="116"/>
-      <c r="AX33" s="116"/>
-      <c r="AY33" s="116"/>
+      <c r="AU33" s="107"/>
+      <c r="AV33" s="107"/>
+      <c r="AW33" s="107"/>
+      <c r="AX33" s="107"/>
+      <c r="AY33" s="107"/>
       <c r="AZ33" s="49"/>
       <c r="BA33" s="49"/>
       <c r="BB33" s="49"/>
@@ -5623,208 +5625,210 @@
       <c r="BK33" s="49"/>
       <c r="BL33" s="49"/>
       <c r="BM33" s="49"/>
-      <c r="BN33" s="116"/>
-      <c r="BO33" s="116"/>
-      <c r="BP33" s="116"/>
-      <c r="BQ33" s="116"/>
-      <c r="BR33" s="116"/>
-      <c r="BS33" s="116"/>
-      <c r="BT33" s="116"/>
+      <c r="BN33" s="107"/>
+      <c r="BO33" s="107"/>
+      <c r="BP33" s="107"/>
+      <c r="BQ33" s="107"/>
+      <c r="BR33" s="107"/>
+      <c r="BS33" s="107"/>
+      <c r="BT33" s="107"/>
     </row>
     <row r="34" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="12"/>
-      <c r="B34" s="74" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="75"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="134"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="78"/>
+      <c r="B34" s="70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="72">
+        <v>0</v>
+      </c>
+      <c r="E34" s="120" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="73">
+        <f>G33+1</f>
+        <v>45250</v>
+      </c>
+      <c r="G34" s="73">
+        <f>F34+1</f>
+        <v>45251</v>
+      </c>
       <c r="H34" s="16"/>
-      <c r="I34" s="5" t="str">
+      <c r="I34" s="5">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="J34" s="79"/>
-      <c r="K34" s="79"/>
-      <c r="L34" s="79"/>
-      <c r="M34" s="79"/>
-      <c r="N34" s="79"/>
-      <c r="O34" s="79"/>
-      <c r="P34" s="119"/>
-      <c r="Q34" s="119"/>
-      <c r="R34" s="119"/>
-      <c r="S34" s="79"/>
-      <c r="T34" s="79"/>
-      <c r="U34" s="79"/>
-      <c r="V34" s="79"/>
-      <c r="W34" s="79"/>
-      <c r="X34" s="79"/>
-      <c r="Y34" s="79"/>
-      <c r="Z34" s="79"/>
-      <c r="AA34" s="79"/>
-      <c r="AB34" s="79"/>
-      <c r="AC34" s="79"/>
-      <c r="AD34" s="79"/>
-      <c r="AE34" s="79"/>
-      <c r="AF34" s="79"/>
-      <c r="AG34" s="79"/>
-      <c r="AH34" s="79"/>
-      <c r="AI34" s="79"/>
-      <c r="AJ34" s="79"/>
-      <c r="AK34" s="79"/>
-      <c r="AL34" s="79"/>
-      <c r="AM34" s="79"/>
-      <c r="AN34" s="79"/>
-      <c r="AO34" s="79"/>
-      <c r="AP34" s="79"/>
-      <c r="AQ34" s="79"/>
-      <c r="AR34" s="79"/>
-      <c r="AS34" s="79"/>
-      <c r="AT34" s="79"/>
-      <c r="AU34" s="119"/>
-      <c r="AV34" s="119"/>
-      <c r="AW34" s="119"/>
-      <c r="AX34" s="119"/>
-      <c r="AY34" s="119"/>
-      <c r="AZ34" s="79"/>
-      <c r="BA34" s="79"/>
-      <c r="BB34" s="79"/>
-      <c r="BC34" s="79"/>
-      <c r="BD34" s="79"/>
-      <c r="BE34" s="79"/>
-      <c r="BF34" s="79"/>
-      <c r="BG34" s="79"/>
-      <c r="BH34" s="79"/>
-      <c r="BI34" s="79"/>
-      <c r="BJ34" s="79"/>
-      <c r="BK34" s="79"/>
-      <c r="BL34" s="79"/>
-      <c r="BM34" s="79"/>
-      <c r="BN34" s="119"/>
-      <c r="BO34" s="119"/>
-      <c r="BP34" s="119"/>
-      <c r="BQ34" s="119"/>
-      <c r="BR34" s="119"/>
-      <c r="BS34" s="119"/>
-      <c r="BT34" s="119"/>
+        <v>2</v>
+      </c>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="107"/>
+      <c r="Q34" s="107"/>
+      <c r="R34" s="107"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
+      <c r="U34" s="49"/>
+      <c r="V34" s="49"/>
+      <c r="W34" s="49"/>
+      <c r="X34" s="49"/>
+      <c r="Y34" s="49"/>
+      <c r="Z34" s="49"/>
+      <c r="AA34" s="49"/>
+      <c r="AB34" s="49"/>
+      <c r="AC34" s="49"/>
+      <c r="AD34" s="49"/>
+      <c r="AE34" s="49"/>
+      <c r="AF34" s="49"/>
+      <c r="AG34" s="49"/>
+      <c r="AH34" s="49"/>
+      <c r="AI34" s="49"/>
+      <c r="AJ34" s="49"/>
+      <c r="AK34" s="49"/>
+      <c r="AL34" s="49"/>
+      <c r="AM34" s="49"/>
+      <c r="AN34" s="49"/>
+      <c r="AO34" s="49"/>
+      <c r="AP34" s="49"/>
+      <c r="AQ34" s="49"/>
+      <c r="AR34" s="49"/>
+      <c r="AS34" s="49"/>
+      <c r="AT34" s="49"/>
+      <c r="AU34" s="107"/>
+      <c r="AV34" s="107"/>
+      <c r="AW34" s="107"/>
+      <c r="AX34" s="107"/>
+      <c r="AY34" s="107"/>
+      <c r="AZ34" s="49"/>
+      <c r="BA34" s="49"/>
+      <c r="BB34" s="49"/>
+      <c r="BC34" s="49"/>
+      <c r="BD34" s="49"/>
+      <c r="BE34" s="49"/>
+      <c r="BF34" s="49"/>
+      <c r="BG34" s="49"/>
+      <c r="BH34" s="49"/>
+      <c r="BI34" s="49"/>
+      <c r="BJ34" s="49"/>
+      <c r="BK34" s="49"/>
+      <c r="BL34" s="49"/>
+      <c r="BM34" s="49"/>
+      <c r="BN34" s="107"/>
+      <c r="BO34" s="107"/>
+      <c r="BP34" s="107"/>
+      <c r="BQ34" s="107"/>
+      <c r="BR34" s="107"/>
+      <c r="BS34" s="107"/>
+      <c r="BT34" s="107"/>
     </row>
     <row r="35" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="12"/>
-      <c r="B35" s="80" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="D35" s="82">
-        <v>1</v>
-      </c>
-      <c r="E35" s="139" t="s">
-        <v>71</v>
-      </c>
-      <c r="F35" s="83">
-        <f>DATE(2023,10,13)</f>
-        <v>45212</v>
-      </c>
-      <c r="G35" s="83">
-        <f>DATE(2023,10,18)</f>
-        <v>45217</v>
-      </c>
+      <c r="B35" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="75"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="119"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="78"/>
       <c r="H35" s="16"/>
-      <c r="I35" s="5">
+      <c r="I35" s="5" t="str">
         <f t="shared" si="11"/>
-        <v>6</v>
-      </c>
-      <c r="J35" s="49"/>
-      <c r="K35" s="49"/>
-      <c r="L35" s="49"/>
-      <c r="M35" s="49"/>
-      <c r="N35" s="49"/>
-      <c r="O35" s="49"/>
-      <c r="P35" s="116"/>
-      <c r="Q35" s="116"/>
-      <c r="R35" s="116"/>
-      <c r="S35" s="49"/>
-      <c r="T35" s="49"/>
-      <c r="U35" s="49"/>
-      <c r="V35" s="49"/>
-      <c r="W35" s="49"/>
-      <c r="X35" s="49"/>
-      <c r="Y35" s="49"/>
-      <c r="Z35" s="49"/>
-      <c r="AA35" s="49"/>
-      <c r="AB35" s="49"/>
-      <c r="AC35" s="49"/>
-      <c r="AD35" s="49"/>
-      <c r="AE35" s="49"/>
-      <c r="AF35" s="49"/>
-      <c r="AG35" s="49"/>
-      <c r="AH35" s="49"/>
-      <c r="AI35" s="49"/>
-      <c r="AJ35" s="49"/>
-      <c r="AK35" s="49"/>
-      <c r="AL35" s="49"/>
-      <c r="AM35" s="49"/>
-      <c r="AN35" s="49"/>
-      <c r="AO35" s="49"/>
-      <c r="AP35" s="49"/>
-      <c r="AQ35" s="49"/>
-      <c r="AR35" s="49"/>
-      <c r="AS35" s="49"/>
-      <c r="AT35" s="49"/>
-      <c r="AU35" s="116"/>
-      <c r="AV35" s="116"/>
-      <c r="AW35" s="116"/>
-      <c r="AX35" s="116"/>
-      <c r="AY35" s="116"/>
-      <c r="AZ35" s="49"/>
-      <c r="BA35" s="49"/>
-      <c r="BB35" s="49"/>
-      <c r="BC35" s="49"/>
-      <c r="BD35" s="49"/>
-      <c r="BE35" s="49"/>
-      <c r="BF35" s="49"/>
-      <c r="BG35" s="49"/>
-      <c r="BH35" s="49"/>
-      <c r="BI35" s="49"/>
-      <c r="BJ35" s="49"/>
-      <c r="BK35" s="49"/>
-      <c r="BL35" s="49"/>
-      <c r="BM35" s="49"/>
-      <c r="BN35" s="116"/>
-      <c r="BO35" s="116"/>
-      <c r="BP35" s="116"/>
-      <c r="BQ35" s="116"/>
-      <c r="BR35" s="116"/>
-      <c r="BS35" s="116"/>
-      <c r="BT35" s="116"/>
+        <v/>
+      </c>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="79"/>
+      <c r="O35" s="79"/>
+      <c r="P35" s="110"/>
+      <c r="Q35" s="110"/>
+      <c r="R35" s="110"/>
+      <c r="S35" s="79"/>
+      <c r="T35" s="79"/>
+      <c r="U35" s="79"/>
+      <c r="V35" s="79"/>
+      <c r="W35" s="79"/>
+      <c r="X35" s="79"/>
+      <c r="Y35" s="79"/>
+      <c r="Z35" s="79"/>
+      <c r="AA35" s="79"/>
+      <c r="AB35" s="79"/>
+      <c r="AC35" s="79"/>
+      <c r="AD35" s="79"/>
+      <c r="AE35" s="79"/>
+      <c r="AF35" s="79"/>
+      <c r="AG35" s="79"/>
+      <c r="AH35" s="79"/>
+      <c r="AI35" s="79"/>
+      <c r="AJ35" s="79"/>
+      <c r="AK35" s="79"/>
+      <c r="AL35" s="79"/>
+      <c r="AM35" s="79"/>
+      <c r="AN35" s="79"/>
+      <c r="AO35" s="79"/>
+      <c r="AP35" s="79"/>
+      <c r="AQ35" s="79"/>
+      <c r="AR35" s="79"/>
+      <c r="AS35" s="79"/>
+      <c r="AT35" s="79"/>
+      <c r="AU35" s="110"/>
+      <c r="AV35" s="110"/>
+      <c r="AW35" s="110"/>
+      <c r="AX35" s="110"/>
+      <c r="AY35" s="110"/>
+      <c r="AZ35" s="79"/>
+      <c r="BA35" s="79"/>
+      <c r="BB35" s="79"/>
+      <c r="BC35" s="79"/>
+      <c r="BD35" s="79"/>
+      <c r="BE35" s="79"/>
+      <c r="BF35" s="79"/>
+      <c r="BG35" s="79"/>
+      <c r="BH35" s="79"/>
+      <c r="BI35" s="79"/>
+      <c r="BJ35" s="79"/>
+      <c r="BK35" s="79"/>
+      <c r="BL35" s="79"/>
+      <c r="BM35" s="79"/>
+      <c r="BN35" s="110"/>
+      <c r="BO35" s="110"/>
+      <c r="BP35" s="110"/>
+      <c r="BQ35" s="110"/>
+      <c r="BR35" s="110"/>
+      <c r="BS35" s="110"/>
+      <c r="BT35" s="110"/>
     </row>
     <row r="36" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="12"/>
       <c r="B36" s="80" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C36" s="81" t="s">
         <v>31</v>
       </c>
       <c r="D36" s="82">
-        <v>0</v>
-      </c>
-      <c r="E36" s="139">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="E36" s="124" t="s">
+        <v>71</v>
       </c>
       <c r="F36" s="83">
-        <v>45257</v>
+        <f>DATE(2023,10,13)</f>
+        <v>45212</v>
       </c>
       <c r="G36" s="83">
-        <v>45263</v>
+        <f>DATE(2023,10,18)</f>
+        <v>45217</v>
       </c>
       <c r="H36" s="16"/>
       <c r="I36" s="5">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J36" s="49"/>
       <c r="K36" s="49"/>
@@ -5832,9 +5836,9 @@
       <c r="M36" s="49"/>
       <c r="N36" s="49"/>
       <c r="O36" s="49"/>
-      <c r="P36" s="116"/>
-      <c r="Q36" s="116"/>
-      <c r="R36" s="116"/>
+      <c r="P36" s="107"/>
+      <c r="Q36" s="107"/>
+      <c r="R36" s="107"/>
       <c r="S36" s="49"/>
       <c r="T36" s="49"/>
       <c r="U36" s="49"/>
@@ -5863,11 +5867,11 @@
       <c r="AR36" s="49"/>
       <c r="AS36" s="49"/>
       <c r="AT36" s="49"/>
-      <c r="AU36" s="116"/>
-      <c r="AV36" s="116"/>
-      <c r="AW36" s="116"/>
-      <c r="AX36" s="116"/>
-      <c r="AY36" s="116"/>
+      <c r="AU36" s="107"/>
+      <c r="AV36" s="107"/>
+      <c r="AW36" s="107"/>
+      <c r="AX36" s="107"/>
+      <c r="AY36" s="107"/>
       <c r="AZ36" s="49"/>
       <c r="BA36" s="49"/>
       <c r="BB36" s="49"/>
@@ -5882,18 +5886,18 @@
       <c r="BK36" s="49"/>
       <c r="BL36" s="49"/>
       <c r="BM36" s="49"/>
-      <c r="BN36" s="116"/>
-      <c r="BO36" s="116"/>
-      <c r="BP36" s="116"/>
-      <c r="BQ36" s="116"/>
-      <c r="BR36" s="116"/>
-      <c r="BS36" s="116"/>
-      <c r="BT36" s="116"/>
+      <c r="BN36" s="107"/>
+      <c r="BO36" s="107"/>
+      <c r="BP36" s="107"/>
+      <c r="BQ36" s="107"/>
+      <c r="BR36" s="107"/>
+      <c r="BS36" s="107"/>
+      <c r="BT36" s="107"/>
     </row>
     <row r="37" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="12"/>
       <c r="B37" s="80" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C37" s="81" t="s">
         <v>31</v>
@@ -5901,24 +5905,29 @@
       <c r="D37" s="82">
         <v>0</v>
       </c>
-      <c r="E37" s="139"/>
+      <c r="E37" s="124">
+        <v>7</v>
+      </c>
       <c r="F37" s="83">
-        <v>45229</v>
+        <v>45257</v>
       </c>
       <c r="G37" s="83">
         <v>45263</v>
       </c>
       <c r="H37" s="16"/>
-      <c r="I37" s="5"/>
+      <c r="I37" s="5">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
       <c r="J37" s="49"/>
       <c r="K37" s="49"/>
       <c r="L37" s="49"/>
       <c r="M37" s="49"/>
       <c r="N37" s="49"/>
       <c r="O37" s="49"/>
-      <c r="P37" s="116"/>
-      <c r="Q37" s="116"/>
-      <c r="R37" s="116"/>
+      <c r="P37" s="107"/>
+      <c r="Q37" s="107"/>
+      <c r="R37" s="107"/>
       <c r="S37" s="49"/>
       <c r="T37" s="49"/>
       <c r="U37" s="49"/>
@@ -5947,11 +5956,11 @@
       <c r="AR37" s="49"/>
       <c r="AS37" s="49"/>
       <c r="AT37" s="49"/>
-      <c r="AU37" s="116"/>
-      <c r="AV37" s="116"/>
-      <c r="AW37" s="116"/>
-      <c r="AX37" s="116"/>
-      <c r="AY37" s="116"/>
+      <c r="AU37" s="107"/>
+      <c r="AV37" s="107"/>
+      <c r="AW37" s="107"/>
+      <c r="AX37" s="107"/>
+      <c r="AY37" s="107"/>
       <c r="AZ37" s="49"/>
       <c r="BA37" s="49"/>
       <c r="BB37" s="49"/>
@@ -5966,18 +5975,18 @@
       <c r="BK37" s="49"/>
       <c r="BL37" s="49"/>
       <c r="BM37" s="49"/>
-      <c r="BN37" s="116"/>
-      <c r="BO37" s="116"/>
-      <c r="BP37" s="116"/>
-      <c r="BQ37" s="116"/>
-      <c r="BR37" s="116"/>
-      <c r="BS37" s="116"/>
-      <c r="BT37" s="116"/>
+      <c r="BN37" s="107"/>
+      <c r="BO37" s="107"/>
+      <c r="BP37" s="107"/>
+      <c r="BQ37" s="107"/>
+      <c r="BR37" s="107"/>
+      <c r="BS37" s="107"/>
+      <c r="BT37" s="107"/>
     </row>
     <row r="38" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="12"/>
       <c r="B38" s="80" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C38" s="81" t="s">
         <v>31</v>
@@ -5985,29 +5994,24 @@
       <c r="D38" s="82">
         <v>0</v>
       </c>
-      <c r="E38" s="145" t="s">
-        <v>79</v>
-      </c>
+      <c r="E38" s="124"/>
       <c r="F38" s="83">
-        <v>45257</v>
+        <v>45229</v>
       </c>
       <c r="G38" s="83">
-        <v>45270</v>
+        <v>45263</v>
       </c>
       <c r="H38" s="16"/>
-      <c r="I38" s="5">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
+      <c r="I38" s="5"/>
       <c r="J38" s="49"/>
       <c r="K38" s="49"/>
       <c r="L38" s="49"/>
       <c r="M38" s="49"/>
       <c r="N38" s="49"/>
       <c r="O38" s="49"/>
-      <c r="P38" s="116"/>
-      <c r="Q38" s="116"/>
-      <c r="R38" s="116"/>
+      <c r="P38" s="107"/>
+      <c r="Q38" s="107"/>
+      <c r="R38" s="107"/>
       <c r="S38" s="49"/>
       <c r="T38" s="49"/>
       <c r="U38" s="49"/>
@@ -6036,11 +6040,11 @@
       <c r="AR38" s="49"/>
       <c r="AS38" s="49"/>
       <c r="AT38" s="49"/>
-      <c r="AU38" s="116"/>
-      <c r="AV38" s="116"/>
-      <c r="AW38" s="116"/>
-      <c r="AX38" s="116"/>
-      <c r="AY38" s="116"/>
+      <c r="AU38" s="107"/>
+      <c r="AV38" s="107"/>
+      <c r="AW38" s="107"/>
+      <c r="AX38" s="107"/>
+      <c r="AY38" s="107"/>
       <c r="AZ38" s="49"/>
       <c r="BA38" s="49"/>
       <c r="BB38" s="49"/>
@@ -6055,18 +6059,18 @@
       <c r="BK38" s="49"/>
       <c r="BL38" s="49"/>
       <c r="BM38" s="49"/>
-      <c r="BN38" s="116"/>
-      <c r="BO38" s="116"/>
-      <c r="BP38" s="116"/>
-      <c r="BQ38" s="116"/>
-      <c r="BR38" s="116"/>
-      <c r="BS38" s="116"/>
-      <c r="BT38" s="116"/>
+      <c r="BN38" s="107"/>
+      <c r="BO38" s="107"/>
+      <c r="BP38" s="107"/>
+      <c r="BQ38" s="107"/>
+      <c r="BR38" s="107"/>
+      <c r="BS38" s="107"/>
+      <c r="BT38" s="107"/>
     </row>
     <row r="39" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="12"/>
       <c r="B39" s="80" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C39" s="81" t="s">
         <v>31</v>
@@ -6074,11 +6078,11 @@
       <c r="D39" s="82">
         <v>0</v>
       </c>
-      <c r="E39" s="143" t="s">
-        <v>88</v>
+      <c r="E39" s="129" t="s">
+        <v>79</v>
       </c>
       <c r="F39" s="83">
-        <v>45264</v>
+        <v>45257</v>
       </c>
       <c r="G39" s="83">
         <v>45270</v>
@@ -6086,7 +6090,7 @@
       <c r="H39" s="16"/>
       <c r="I39" s="5">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J39" s="49"/>
       <c r="K39" s="49"/>
@@ -6094,9 +6098,9 @@
       <c r="M39" s="49"/>
       <c r="N39" s="49"/>
       <c r="O39" s="49"/>
-      <c r="P39" s="116"/>
-      <c r="Q39" s="116"/>
-      <c r="R39" s="116"/>
+      <c r="P39" s="107"/>
+      <c r="Q39" s="107"/>
+      <c r="R39" s="107"/>
       <c r="S39" s="49"/>
       <c r="T39" s="49"/>
       <c r="U39" s="49"/>
@@ -6125,11 +6129,11 @@
       <c r="AR39" s="49"/>
       <c r="AS39" s="49"/>
       <c r="AT39" s="49"/>
-      <c r="AU39" s="116"/>
-      <c r="AV39" s="116"/>
-      <c r="AW39" s="116"/>
-      <c r="AX39" s="116"/>
-      <c r="AY39" s="116"/>
+      <c r="AU39" s="107"/>
+      <c r="AV39" s="107"/>
+      <c r="AW39" s="107"/>
+      <c r="AX39" s="107"/>
+      <c r="AY39" s="107"/>
       <c r="AZ39" s="49"/>
       <c r="BA39" s="49"/>
       <c r="BB39" s="49"/>
@@ -6144,184 +6148,288 @@
       <c r="BK39" s="49"/>
       <c r="BL39" s="49"/>
       <c r="BM39" s="49"/>
-      <c r="BN39" s="116"/>
-      <c r="BO39" s="116"/>
-      <c r="BP39" s="116"/>
-      <c r="BQ39" s="116"/>
-      <c r="BR39" s="116"/>
-      <c r="BS39" s="116"/>
-      <c r="BT39" s="116"/>
+      <c r="BN39" s="107"/>
+      <c r="BO39" s="107"/>
+      <c r="BP39" s="107"/>
+      <c r="BQ39" s="107"/>
+      <c r="BR39" s="107"/>
+      <c r="BS39" s="107"/>
+      <c r="BT39" s="107"/>
     </row>
     <row r="40" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="12"/>
-      <c r="B40" s="140" t="s">
+      <c r="B40" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" s="82">
+        <v>0</v>
+      </c>
+      <c r="E40" s="128" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="83">
+        <v>45264</v>
+      </c>
+      <c r="G40" s="83">
+        <v>45270</v>
+      </c>
+      <c r="H40" s="16"/>
+      <c r="I40" s="5">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="49"/>
+      <c r="N40" s="49"/>
+      <c r="O40" s="49"/>
+      <c r="P40" s="107"/>
+      <c r="Q40" s="107"/>
+      <c r="R40" s="107"/>
+      <c r="S40" s="49"/>
+      <c r="T40" s="49"/>
+      <c r="U40" s="49"/>
+      <c r="V40" s="49"/>
+      <c r="W40" s="49"/>
+      <c r="X40" s="49"/>
+      <c r="Y40" s="49"/>
+      <c r="Z40" s="49"/>
+      <c r="AA40" s="49"/>
+      <c r="AB40" s="49"/>
+      <c r="AC40" s="49"/>
+      <c r="AD40" s="49"/>
+      <c r="AE40" s="49"/>
+      <c r="AF40" s="49"/>
+      <c r="AG40" s="49"/>
+      <c r="AH40" s="49"/>
+      <c r="AI40" s="49"/>
+      <c r="AJ40" s="49"/>
+      <c r="AK40" s="49"/>
+      <c r="AL40" s="49"/>
+      <c r="AM40" s="49"/>
+      <c r="AN40" s="49"/>
+      <c r="AO40" s="49"/>
+      <c r="AP40" s="49"/>
+      <c r="AQ40" s="49"/>
+      <c r="AR40" s="49"/>
+      <c r="AS40" s="49"/>
+      <c r="AT40" s="49"/>
+      <c r="AU40" s="107"/>
+      <c r="AV40" s="107"/>
+      <c r="AW40" s="107"/>
+      <c r="AX40" s="107"/>
+      <c r="AY40" s="107"/>
+      <c r="AZ40" s="49"/>
+      <c r="BA40" s="49"/>
+      <c r="BB40" s="49"/>
+      <c r="BC40" s="49"/>
+      <c r="BD40" s="49"/>
+      <c r="BE40" s="49"/>
+      <c r="BF40" s="49"/>
+      <c r="BG40" s="49"/>
+      <c r="BH40" s="49"/>
+      <c r="BI40" s="49"/>
+      <c r="BJ40" s="49"/>
+      <c r="BK40" s="49"/>
+      <c r="BL40" s="49"/>
+      <c r="BM40" s="49"/>
+      <c r="BN40" s="107"/>
+      <c r="BO40" s="107"/>
+      <c r="BP40" s="107"/>
+      <c r="BQ40" s="107"/>
+      <c r="BR40" s="107"/>
+      <c r="BS40" s="107"/>
+      <c r="BT40" s="107"/>
+    </row>
+    <row r="41" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="12"/>
+      <c r="B41" s="125" t="s">
         <v>82</v>
       </c>
-      <c r="C40" s="141"/>
-      <c r="D40" s="142"/>
-      <c r="E40" s="84"/>
-      <c r="F40" s="85"/>
-      <c r="G40" s="85"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="5" t="str">
+      <c r="C41" s="126"/>
+      <c r="D41" s="127"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="85"/>
+      <c r="G41" s="85"/>
+      <c r="H41" s="16"/>
+      <c r="I41" s="5" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="J40" s="43"/>
-      <c r="K40" s="43"/>
-      <c r="L40" s="43"/>
-      <c r="M40" s="43"/>
-      <c r="N40" s="43"/>
-      <c r="O40" s="43"/>
-      <c r="P40" s="115"/>
-      <c r="Q40" s="115"/>
-      <c r="R40" s="115"/>
-      <c r="S40" s="43"/>
-      <c r="T40" s="43"/>
-      <c r="U40" s="43"/>
-      <c r="V40" s="43"/>
-      <c r="W40" s="43"/>
-      <c r="X40" s="43"/>
-      <c r="Y40" s="43"/>
-      <c r="Z40" s="43"/>
-      <c r="AA40" s="43"/>
-      <c r="AB40" s="43"/>
-      <c r="AC40" s="43"/>
-      <c r="AD40" s="43"/>
-      <c r="AE40" s="43"/>
-      <c r="AF40" s="43"/>
-      <c r="AG40" s="43"/>
-      <c r="AH40" s="43"/>
-      <c r="AI40" s="43"/>
-      <c r="AJ40" s="43"/>
-      <c r="AK40" s="43"/>
-      <c r="AL40" s="43"/>
-      <c r="AM40" s="43"/>
-      <c r="AN40" s="43"/>
-      <c r="AO40" s="43"/>
-      <c r="AP40" s="43"/>
-      <c r="AQ40" s="43"/>
-      <c r="AR40" s="43"/>
-      <c r="AS40" s="43"/>
-      <c r="AT40" s="43"/>
-      <c r="AU40" s="115"/>
-      <c r="AV40" s="115"/>
-      <c r="AW40" s="115"/>
-      <c r="AX40" s="115"/>
-      <c r="AY40" s="115"/>
-      <c r="AZ40" s="43"/>
-      <c r="BA40" s="43"/>
-      <c r="BB40" s="43"/>
-      <c r="BC40" s="43"/>
-      <c r="BD40" s="43"/>
-      <c r="BE40" s="43"/>
-      <c r="BF40" s="43"/>
-      <c r="BG40" s="43"/>
-      <c r="BH40" s="43"/>
-      <c r="BI40" s="43"/>
-      <c r="BJ40" s="43"/>
-      <c r="BK40" s="43"/>
-      <c r="BL40" s="43"/>
-      <c r="BM40" s="43"/>
-      <c r="BN40" s="115"/>
-      <c r="BO40" s="115"/>
-      <c r="BP40" s="115"/>
-      <c r="BQ40" s="115"/>
-      <c r="BR40" s="115"/>
-      <c r="BS40" s="115"/>
-      <c r="BT40" s="115"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="43"/>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="43"/>
+      <c r="O41" s="43"/>
+      <c r="P41" s="106"/>
+      <c r="Q41" s="106"/>
+      <c r="R41" s="106"/>
+      <c r="S41" s="43"/>
+      <c r="T41" s="43"/>
+      <c r="U41" s="43"/>
+      <c r="V41" s="43"/>
+      <c r="W41" s="43"/>
+      <c r="X41" s="43"/>
+      <c r="Y41" s="43"/>
+      <c r="Z41" s="43"/>
+      <c r="AA41" s="43"/>
+      <c r="AB41" s="43"/>
+      <c r="AC41" s="43"/>
+      <c r="AD41" s="43"/>
+      <c r="AE41" s="43"/>
+      <c r="AF41" s="43"/>
+      <c r="AG41" s="43"/>
+      <c r="AH41" s="43"/>
+      <c r="AI41" s="43"/>
+      <c r="AJ41" s="43"/>
+      <c r="AK41" s="43"/>
+      <c r="AL41" s="43"/>
+      <c r="AM41" s="43"/>
+      <c r="AN41" s="43"/>
+      <c r="AO41" s="43"/>
+      <c r="AP41" s="43"/>
+      <c r="AQ41" s="43"/>
+      <c r="AR41" s="43"/>
+      <c r="AS41" s="43"/>
+      <c r="AT41" s="43"/>
+      <c r="AU41" s="106"/>
+      <c r="AV41" s="106"/>
+      <c r="AW41" s="106"/>
+      <c r="AX41" s="106"/>
+      <c r="AY41" s="106"/>
+      <c r="AZ41" s="43"/>
+      <c r="BA41" s="43"/>
+      <c r="BB41" s="43"/>
+      <c r="BC41" s="43"/>
+      <c r="BD41" s="43"/>
+      <c r="BE41" s="43"/>
+      <c r="BF41" s="43"/>
+      <c r="BG41" s="43"/>
+      <c r="BH41" s="43"/>
+      <c r="BI41" s="43"/>
+      <c r="BJ41" s="43"/>
+      <c r="BK41" s="43"/>
+      <c r="BL41" s="43"/>
+      <c r="BM41" s="43"/>
+      <c r="BN41" s="106"/>
+      <c r="BO41" s="106"/>
+      <c r="BP41" s="106"/>
+      <c r="BQ41" s="106"/>
+      <c r="BR41" s="106"/>
+      <c r="BS41" s="106"/>
+      <c r="BT41" s="106"/>
     </row>
-    <row r="41" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
-      <c r="B41" s="86" t="s">
+    <row r="42" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="13"/>
+      <c r="B42" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="87"/>
-      <c r="D41" s="88"/>
-      <c r="E41" s="88"/>
-      <c r="F41" s="89"/>
-      <c r="G41" s="90"/>
-      <c r="H41" s="90"/>
-      <c r="I41" s="90" t="str">
+      <c r="C42" s="87"/>
+      <c r="D42" s="88"/>
+      <c r="E42" s="88"/>
+      <c r="F42" s="89"/>
+      <c r="G42" s="90"/>
+      <c r="H42" s="90"/>
+      <c r="I42" s="90" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="J41" s="90"/>
-      <c r="K41" s="90"/>
-      <c r="L41" s="90"/>
-      <c r="M41" s="90"/>
-      <c r="N41" s="90"/>
-      <c r="O41" s="90"/>
-      <c r="P41" s="90"/>
-      <c r="Q41" s="90"/>
-      <c r="R41" s="90"/>
-      <c r="S41" s="90"/>
-      <c r="T41" s="90"/>
-      <c r="U41" s="90"/>
-      <c r="V41" s="90"/>
-      <c r="W41" s="90"/>
-      <c r="X41" s="90"/>
-      <c r="Y41" s="90"/>
-      <c r="Z41" s="90"/>
-      <c r="AA41" s="90"/>
-      <c r="AB41" s="90"/>
-      <c r="AC41" s="90"/>
-      <c r="AD41" s="90"/>
-      <c r="AE41" s="90"/>
-      <c r="AF41" s="90"/>
-      <c r="AG41" s="90"/>
-      <c r="AH41" s="90"/>
-      <c r="AI41" s="90"/>
-      <c r="AJ41" s="90"/>
-      <c r="AK41" s="90"/>
-      <c r="AL41" s="90"/>
-      <c r="AM41" s="90"/>
-      <c r="AN41" s="90"/>
-      <c r="AO41" s="90"/>
-      <c r="AP41" s="90"/>
-      <c r="AQ41" s="90"/>
-      <c r="AR41" s="90"/>
-      <c r="AS41" s="90"/>
-      <c r="AT41" s="90"/>
-      <c r="AU41" s="90"/>
-      <c r="AV41" s="90"/>
-      <c r="AW41" s="90"/>
-      <c r="AX41" s="90"/>
-      <c r="AY41" s="90"/>
-      <c r="AZ41" s="90"/>
-      <c r="BA41" s="90"/>
-      <c r="BB41" s="90"/>
-      <c r="BC41" s="90"/>
-      <c r="BD41" s="90"/>
-      <c r="BE41" s="90"/>
-      <c r="BF41" s="90"/>
-      <c r="BG41" s="90"/>
-      <c r="BH41" s="90"/>
-      <c r="BI41" s="90"/>
-      <c r="BJ41" s="90"/>
-      <c r="BK41" s="90"/>
-      <c r="BL41" s="90"/>
-      <c r="BM41" s="90"/>
-      <c r="BN41" s="90"/>
-      <c r="BO41" s="90"/>
-      <c r="BP41" s="90"/>
-      <c r="BQ41" s="90"/>
-      <c r="BR41" s="90"/>
-      <c r="BS41" s="90"/>
-      <c r="BT41" s="90"/>
+      <c r="J42" s="90"/>
+      <c r="K42" s="90"/>
+      <c r="L42" s="90"/>
+      <c r="M42" s="90"/>
+      <c r="N42" s="90"/>
+      <c r="O42" s="90"/>
+      <c r="P42" s="90"/>
+      <c r="Q42" s="90"/>
+      <c r="R42" s="90"/>
+      <c r="S42" s="90"/>
+      <c r="T42" s="90"/>
+      <c r="U42" s="90"/>
+      <c r="V42" s="90"/>
+      <c r="W42" s="90"/>
+      <c r="X42" s="90"/>
+      <c r="Y42" s="90"/>
+      <c r="Z42" s="90"/>
+      <c r="AA42" s="90"/>
+      <c r="AB42" s="90"/>
+      <c r="AC42" s="90"/>
+      <c r="AD42" s="90"/>
+      <c r="AE42" s="90"/>
+      <c r="AF42" s="90"/>
+      <c r="AG42" s="90"/>
+      <c r="AH42" s="90"/>
+      <c r="AI42" s="90"/>
+      <c r="AJ42" s="90"/>
+      <c r="AK42" s="90"/>
+      <c r="AL42" s="90"/>
+      <c r="AM42" s="90"/>
+      <c r="AN42" s="90"/>
+      <c r="AO42" s="90"/>
+      <c r="AP42" s="90"/>
+      <c r="AQ42" s="90"/>
+      <c r="AR42" s="90"/>
+      <c r="AS42" s="90"/>
+      <c r="AT42" s="90"/>
+      <c r="AU42" s="90"/>
+      <c r="AV42" s="90"/>
+      <c r="AW42" s="90"/>
+      <c r="AX42" s="90"/>
+      <c r="AY42" s="90"/>
+      <c r="AZ42" s="90"/>
+      <c r="BA42" s="90"/>
+      <c r="BB42" s="90"/>
+      <c r="BC42" s="90"/>
+      <c r="BD42" s="90"/>
+      <c r="BE42" s="90"/>
+      <c r="BF42" s="90"/>
+      <c r="BG42" s="90"/>
+      <c r="BH42" s="90"/>
+      <c r="BI42" s="90"/>
+      <c r="BJ42" s="90"/>
+      <c r="BK42" s="90"/>
+      <c r="BL42" s="90"/>
+      <c r="BM42" s="90"/>
+      <c r="BN42" s="90"/>
+      <c r="BO42" s="90"/>
+      <c r="BP42" s="90"/>
+      <c r="BQ42" s="90"/>
+      <c r="BR42" s="90"/>
+      <c r="BS42" s="90"/>
+      <c r="BT42" s="90"/>
     </row>
-    <row r="42" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H42" s="3"/>
+    <row r="43" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H43" s="3"/>
     </row>
-    <row r="43" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C43" s="15"/>
-      <c r="G43" s="14"/>
+    <row r="44" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C44" s="15"/>
+      <c r="G44" s="14"/>
     </row>
-    <row r="44" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C44" s="4"/>
+    <row r="45" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C45" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="AZ5:BF5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="R3:AA3"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="J5:P5"/>
+    <mergeCell ref="Q5:W5"/>
+    <mergeCell ref="X5:AD5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="Q1:Z1"/>
     <mergeCell ref="BN5:BT5"/>
@@ -6334,28 +6442,13 @@
     <mergeCell ref="AZ4:BF4"/>
     <mergeCell ref="BG4:BM4"/>
     <mergeCell ref="BN4:BT4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="R3:AA3"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="J3:P3"/>
     <mergeCell ref="BG5:BM5"/>
-    <mergeCell ref="J5:P5"/>
-    <mergeCell ref="Q5:W5"/>
-    <mergeCell ref="X5:AD5"/>
     <mergeCell ref="AE5:AK5"/>
     <mergeCell ref="AL5:AR5"/>
     <mergeCell ref="AS5:AY5"/>
-    <mergeCell ref="AZ5:BF5"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
-  <conditionalFormatting sqref="D25:D33 D34:E34 D40:E41 D35:D39 D8:E24">
+  <conditionalFormatting sqref="D35:E35 D41:E42 D36:D40 D8:E24 D25:D34">
     <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6385,7 +6478,7 @@
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J25:BL33 BN25:BT33">
+  <conditionalFormatting sqref="J25:BL34 BN25:BT34">
     <cfRule type="expression" dxfId="47" priority="51">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
@@ -6393,7 +6486,7 @@
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J36:BL39">
+  <conditionalFormatting sqref="J37:BL40">
     <cfRule type="expression" dxfId="45" priority="85">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
@@ -6401,7 +6494,7 @@
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN5:BS8 J5:BL9 BN9:BT39 J12:BL39 J10:BM11">
+  <conditionalFormatting sqref="BN5:BS8 J5:BL9 J10:BM11 BN9:BT40 J12:BL40">
     <cfRule type="expression" dxfId="43" priority="50">
       <formula>AND(TODAY()&gt;=J$6, TODAY()&lt;K$6)</formula>
     </cfRule>
@@ -6422,7 +6515,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BU$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM25:BM33">
+  <conditionalFormatting sqref="BM25:BM34">
     <cfRule type="expression" dxfId="38" priority="97">
       <formula>AND(task_start&lt;=BM$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$6)</formula>
     </cfRule>
@@ -6430,7 +6523,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BU$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM35:BM37">
+  <conditionalFormatting sqref="BM36:BM38">
     <cfRule type="expression" dxfId="36" priority="101">
       <formula>AND(task_start&lt;=BM$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$6)</formula>
     </cfRule>
@@ -6438,7 +6531,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BU$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT5:BT8 BM5:BM9 BM12:BM37">
+  <conditionalFormatting sqref="BT5:BT8 BM5:BM9 BM12:BM38">
     <cfRule type="expression" dxfId="34" priority="104">
       <formula>AND(TODAY()&gt;=BM$6, TODAY()&lt;BU$6)</formula>
     </cfRule>
@@ -6448,7 +6541,7 @@
       <formula>AND(TODAY()&gt;=J$6, TODAY()&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J35:BL35">
+  <conditionalFormatting sqref="J36:BL36">
     <cfRule type="expression" dxfId="32" priority="34">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
@@ -6472,7 +6565,7 @@
       <formula>AND(task_end&gt;=BN$6,task_start&lt;BO$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN36:BO39">
+  <conditionalFormatting sqref="BN37:BO40">
     <cfRule type="expression" dxfId="26" priority="30">
       <formula>AND(task_start&lt;=BN$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BN$6)</formula>
     </cfRule>
@@ -6480,7 +6573,7 @@
       <formula>AND(task_end&gt;=BN$6,task_start&lt;BO$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN35:BO35">
+  <conditionalFormatting sqref="BN36:BO36">
     <cfRule type="expression" dxfId="24" priority="24">
       <formula>AND(task_start&lt;=BN$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BN$6)</formula>
     </cfRule>
@@ -6504,7 +6597,7 @@
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP36:BT39">
+  <conditionalFormatting sqref="BP37:BT40">
     <cfRule type="expression" dxfId="18" priority="22">
       <formula>AND(task_start&lt;=BP$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BP$6)</formula>
     </cfRule>
@@ -6512,7 +6605,7 @@
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP35:BT35">
+  <conditionalFormatting sqref="BP36:BT36">
     <cfRule type="expression" dxfId="16" priority="16">
       <formula>AND(task_start&lt;=BP$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BP$6)</formula>
     </cfRule>
@@ -6520,64 +6613,64 @@
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM38:BM39">
-    <cfRule type="expression" dxfId="2" priority="14">
+  <conditionalFormatting sqref="BM39:BM40">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>AND(task_start&lt;=BM$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="15" stopIfTrue="1">
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BN$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM38:BM39">
-    <cfRule type="expression" dxfId="0" priority="13">
+  <conditionalFormatting sqref="BM39:BM40">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>AND(TODAY()&gt;=BM$6, TODAY()&lt;BN$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10:BK10 BL10:BM11">
-    <cfRule type="expression" dxfId="14" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN10:BO10">
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="9" priority="9">
       <formula>AND(task_start&lt;=BN$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BN$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>AND(task_end&gt;=BN$6,task_start&lt;BO$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP10:BT10">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>AND(task_start&lt;=BP$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BP$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J11:BK11">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BN11:BO11">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>AND(task_start&lt;=BN$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BN$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
       <formula>AND(task_end&gt;=BN$6,task_start&lt;BO$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BP11:BT11">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(task_start&lt;=BP$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BP$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6591,8 +6684,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A13:A14" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A18" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A24" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A34" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A41" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A35" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A42" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="R3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -6604,7 +6697,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId3"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -6627,7 +6720,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D25:D33 D34:E34 D40:E41 D35:D39 D8:E24</xm:sqref>
+          <xm:sqref>D35:E35 D41:E42 D36:D40 D8:E24 D25:D34</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -7074,15 +7167,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -7100,6 +7184,15 @@
     <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7124,14 +7217,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -7150,6 +7235,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>

<commit_message>
Reviewed and updated Gantt Chart
</commit_message>
<xml_diff>
--- a/docs/gantt-chart/Lakeshore Misfits Project Gantt chart.xlsx
+++ b/docs/gantt-chart/Lakeshore Misfits Project Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khngu\Documents\_GVSU\CIS 641\_Team_Project\_Term_Project\GVSU-CIS641-Lakeshore-Misfits\docs\gantt-chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5BF993-232A-453F-94C4-0747599B782D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7EBBF3-F6F2-42FA-B96E-D8A7D0FBF5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -207,12 +207,6 @@
     <t>Create API Services</t>
   </si>
   <si>
-    <t>Populate Page Layouts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Munmi </t>
-  </si>
-  <si>
     <t>SPRINT</t>
   </si>
   <si>
@@ -333,7 +327,22 @@
     <t>Setup Global Color Palette State / Context</t>
   </si>
   <si>
-    <t>Setup Color Service / Utilize TinyColor 2 Library</t>
+    <t>Munmi / Khiem</t>
+  </si>
+  <si>
+    <t>Learn &amp; Utilize TinyColor 2 Library</t>
+  </si>
+  <si>
+    <t>2 &amp; 4</t>
+  </si>
+  <si>
+    <t>Create and Implement UI Components</t>
+  </si>
+  <si>
+    <t>Create and Implement Model Classes</t>
+  </si>
+  <si>
+    <t>Populate Page Layouts (Static)</t>
   </si>
 </sst>
 </file>
@@ -2523,10 +2532,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BT45"/>
+  <dimension ref="A1:BT47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="BS44" sqref="B1:BT44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2549,7 +2558,7 @@
     <row r="1" spans="1:72" ht="90" customHeight="1" x14ac:dyDescent="2.25">
       <c r="A1" s="13"/>
       <c r="B1" s="93" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="18"/>
@@ -2558,7 +2567,7 @@
       <c r="G1" s="20"/>
       <c r="I1" s="1"/>
       <c r="J1" s="137" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K1" s="138"/>
       <c r="L1" s="138"/>
@@ -2588,17 +2597,17 @@
     </row>
     <row r="2" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.9">
       <c r="B2" s="91" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C2" s="92" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="21"/>
       <c r="F2" s="22"/>
       <c r="G2" s="21"/>
       <c r="I2" s="137" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J2" s="138"/>
       <c r="K2" s="138"/>
@@ -2860,7 +2869,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="131" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F6" s="131" t="s">
         <v>3</v>
@@ -3463,7 +3472,7 @@
     <row r="9" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="13"/>
       <c r="B9" s="38" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C9" s="39"/>
       <c r="D9" s="40"/>
@@ -3472,7 +3481,7 @@
       <c r="G9" s="42"/>
       <c r="H9" s="16"/>
       <c r="I9" s="5" t="str">
-        <f t="shared" ref="I9:I42" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="I9:I44" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="J9" s="43"/>
@@ -3536,7 +3545,7 @@
       <c r="BL9" s="43"/>
       <c r="BM9" s="43"/>
       <c r="BN9" s="106" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="BO9" s="106"/>
       <c r="BP9" s="106"/>
@@ -3548,7 +3557,7 @@
     <row r="10" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="13"/>
       <c r="B10" s="45" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C10" s="46" t="s">
         <v>31</v>
@@ -3557,7 +3566,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E10" s="114" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F10" s="48">
         <f>Q1</f>
@@ -3638,7 +3647,7 @@
     <row r="11" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
       <c r="B11" s="45" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C11" s="46" t="s">
         <v>31</v>
@@ -3647,7 +3656,7 @@
         <v>0.5</v>
       </c>
       <c r="E11" s="114" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F11" s="48">
         <f>DATE(2023,9,20)</f>
@@ -3728,7 +3737,7 @@
     <row r="12" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="13"/>
       <c r="B12" s="45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C12" s="46" t="s">
         <v>31</v>
@@ -3819,7 +3828,7 @@
     <row r="13" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="13"/>
       <c r="B13" s="50" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" s="51" t="s">
         <v>31</v>
@@ -3828,20 +3837,20 @@
         <v>0.5</v>
       </c>
       <c r="E13" s="123" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F13" s="53">
         <f>DATE(2023,10,13)</f>
         <v>45212</v>
       </c>
       <c r="G13" s="53">
-        <f>DATE(2023,11,21)</f>
-        <v>45251</v>
+        <f>DATE(2023,12,3)</f>
+        <v>45263</v>
       </c>
       <c r="H13" s="16"/>
       <c r="I13" s="5">
         <f t="shared" si="11"/>
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J13" s="49"/>
       <c r="K13" s="49"/>
@@ -3910,7 +3919,7 @@
     <row r="14" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="13"/>
       <c r="B14" s="50" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C14" s="51" t="s">
         <v>31</v>
@@ -3919,15 +3928,15 @@
         <v>0.4</v>
       </c>
       <c r="E14" s="123" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F14" s="53">
         <f>Project_Start</f>
         <v>45215</v>
       </c>
       <c r="G14" s="53">
-        <f>DATE(2023,11,21)</f>
-        <v>45251</v>
+        <f>DATE(2023,12,3)</f>
+        <v>45263</v>
       </c>
       <c r="H14" s="16"/>
       <c r="I14" s="5"/>
@@ -3998,7 +4007,7 @@
     <row r="15" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="12"/>
       <c r="B15" s="50" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>31</v>
@@ -4007,20 +4016,20 @@
         <v>0.4</v>
       </c>
       <c r="E15" s="114" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F15" s="53">
         <f>DATE(2023,9,27)</f>
         <v>45196</v>
       </c>
       <c r="G15" s="53">
-        <f>DATE(2023,11,21)</f>
-        <v>45251</v>
+        <f>DATE(2023,12,3)</f>
+        <v>45263</v>
       </c>
       <c r="H15" s="16"/>
       <c r="I15" s="5">
         <f t="shared" si="11"/>
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="J15" s="49"/>
       <c r="K15" s="49"/>
@@ -4089,7 +4098,7 @@
     <row r="16" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="12"/>
       <c r="B16" s="50" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C16" s="51" t="s">
         <v>31</v>
@@ -4098,20 +4107,20 @@
         <v>0.1</v>
       </c>
       <c r="E16" s="123" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F16" s="53">
         <f>DATE(2023,10,25)</f>
         <v>45224</v>
       </c>
       <c r="G16" s="53">
-        <f>DATE(2023,11,21)</f>
-        <v>45251</v>
+        <f>DATE(2023,12,3)</f>
+        <v>45263</v>
       </c>
       <c r="H16" s="16"/>
       <c r="I16" s="5">
         <f t="shared" si="11"/>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="J16" s="49"/>
       <c r="K16" s="49"/>
@@ -4180,7 +4189,7 @@
     <row r="17" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="12"/>
       <c r="B17" s="50" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>31</v>
@@ -4189,7 +4198,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="123" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F17" s="53">
         <f>DATE(2023,10,12)</f>
@@ -5002,7 +5011,7 @@
     <row r="27" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="12"/>
       <c r="B27" s="70" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C27" s="71" t="s">
         <v>35</v>
@@ -5093,30 +5102,27 @@
     <row r="28" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="12"/>
       <c r="B28" s="70" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C28" s="71" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="72">
-        <v>0.5</v>
-      </c>
-      <c r="E28" s="121" t="s">
-        <v>55</v>
+        <v>1</v>
+      </c>
+      <c r="E28" s="122">
+        <v>2</v>
       </c>
       <c r="F28" s="73">
         <f>DATE(2023,10,23)</f>
         <v>45222</v>
       </c>
       <c r="G28" s="73">
-        <f>F28+13</f>
-        <v>45235</v>
+        <f>F28+6</f>
+        <v>45228</v>
       </c>
       <c r="H28" s="16"/>
-      <c r="I28" s="5">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
+      <c r="I28" s="5"/>
       <c r="J28" s="49"/>
       <c r="K28" s="49"/>
       <c r="L28" s="49"/>
@@ -5184,29 +5190,29 @@
     <row r="29" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="12"/>
       <c r="B29" s="70" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="C29" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="72">
+        <v>0.8</v>
+      </c>
+      <c r="E29" s="121" t="s">
         <v>53</v>
-      </c>
-      <c r="D29" s="72">
-        <v>0</v>
-      </c>
-      <c r="E29" s="120">
-        <v>2</v>
       </c>
       <c r="F29" s="73">
         <f>DATE(2023,10,23)</f>
         <v>45222</v>
       </c>
       <c r="G29" s="73">
-        <f>F29+6</f>
-        <v>45228</v>
+        <f>F29+13</f>
+        <v>45235</v>
       </c>
       <c r="H29" s="16"/>
       <c r="I29" s="5">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J29" s="49"/>
       <c r="K29" s="49"/>
@@ -5275,29 +5281,29 @@
     <row r="30" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="12"/>
       <c r="B30" s="70" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C30" s="71" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="D30" s="72">
         <v>0.2</v>
       </c>
-      <c r="E30" s="121" t="s">
-        <v>55</v>
+      <c r="E30" s="120" t="s">
+        <v>54</v>
       </c>
       <c r="F30" s="73">
-        <f>G26+1</f>
-        <v>45222</v>
+        <f>G27+1</f>
+        <v>45229</v>
       </c>
       <c r="G30" s="73">
-        <f>F30+13</f>
-        <v>45235</v>
+        <f>F30+12</f>
+        <v>45241</v>
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="5">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J30" s="49"/>
       <c r="K30" s="49"/>
@@ -5366,27 +5372,30 @@
     <row r="31" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="12"/>
       <c r="B31" s="70" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="C31" s="71" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D31" s="72">
-        <v>0.3</v>
-      </c>
-      <c r="E31" s="122" t="s">
-        <v>56</v>
+        <v>1</v>
+      </c>
+      <c r="E31" s="121" t="s">
+        <v>53</v>
       </c>
       <c r="F31" s="73">
-        <f>G29+1</f>
-        <v>45229</v>
+        <f>G26+1</f>
+        <v>45222</v>
       </c>
       <c r="G31" s="73">
         <f>F31+13</f>
-        <v>45242</v>
+        <v>45235</v>
       </c>
       <c r="H31" s="16"/>
-      <c r="I31" s="5"/>
+      <c r="I31" s="5">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
       <c r="J31" s="49"/>
       <c r="K31" s="49"/>
       <c r="L31" s="49"/>
@@ -5454,30 +5463,27 @@
     <row r="32" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="12"/>
       <c r="B32" s="70" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="C32" s="71" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D32" s="72">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="E32" s="122" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="F32" s="73">
-        <f>G29+1</f>
-        <v>45229</v>
+        <f>DATE(2023,10,23)</f>
+        <v>45222</v>
       </c>
       <c r="G32" s="73">
-        <f>F32+13</f>
-        <v>45242</v>
+        <f>DATE(2023,11,11)</f>
+        <v>45241</v>
       </c>
       <c r="H32" s="16"/>
-      <c r="I32" s="5">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
+      <c r="I32" s="5"/>
       <c r="J32" s="49"/>
       <c r="K32" s="49"/>
       <c r="L32" s="49"/>
@@ -5545,30 +5551,27 @@
     <row r="33" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="12"/>
       <c r="B33" s="70" t="s">
-        <v>60</v>
+        <v>95</v>
       </c>
       <c r="C33" s="71" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D33" s="72">
-        <v>0</v>
-      </c>
-      <c r="E33" s="120" t="s">
-        <v>62</v>
+        <v>0.8</v>
+      </c>
+      <c r="E33" s="122" t="s">
+        <v>94</v>
       </c>
       <c r="F33" s="73">
-        <f>G30+1</f>
-        <v>45236</v>
+        <f>DATE(2023,10,23)</f>
+        <v>45222</v>
       </c>
       <c r="G33" s="73">
-        <f>F33+13</f>
-        <v>45249</v>
+        <f>DATE(2023,11,11)</f>
+        <v>45241</v>
       </c>
       <c r="H33" s="16"/>
-      <c r="I33" s="5">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
+      <c r="I33" s="5"/>
       <c r="J33" s="49"/>
       <c r="K33" s="49"/>
       <c r="L33" s="49"/>
@@ -5636,29 +5639,29 @@
     <row r="34" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="12"/>
       <c r="B34" s="70" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C34" s="71" t="s">
         <v>31</v>
       </c>
       <c r="D34" s="72">
-        <v>0</v>
-      </c>
-      <c r="E34" s="120" t="s">
-        <v>63</v>
+        <v>0.2</v>
+      </c>
+      <c r="E34" s="122" t="s">
+        <v>60</v>
       </c>
       <c r="F34" s="73">
-        <f>G33+1</f>
-        <v>45250</v>
+        <f>DATE(2023,11,6)</f>
+        <v>45236</v>
       </c>
       <c r="G34" s="73">
-        <f>F34+1</f>
-        <v>45251</v>
+        <f>F34+13</f>
+        <v>45249</v>
       </c>
       <c r="H34" s="16"/>
       <c r="I34" s="5">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J34" s="49"/>
       <c r="K34" s="49"/>
@@ -5726,109 +5729,121 @@
     </row>
     <row r="35" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="12"/>
-      <c r="B35" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="75"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="119"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="78"/>
+      <c r="B35" s="70" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="D35" s="72">
+        <v>0.1</v>
+      </c>
+      <c r="E35" s="120" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="73">
+        <f>G31+1</f>
+        <v>45236</v>
+      </c>
+      <c r="G35" s="73">
+        <f>F35+13</f>
+        <v>45249</v>
+      </c>
       <c r="H35" s="16"/>
-      <c r="I35" s="5" t="str">
+      <c r="I35" s="5">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="79"/>
-      <c r="N35" s="79"/>
-      <c r="O35" s="79"/>
-      <c r="P35" s="110"/>
-      <c r="Q35" s="110"/>
-      <c r="R35" s="110"/>
-      <c r="S35" s="79"/>
-      <c r="T35" s="79"/>
-      <c r="U35" s="79"/>
-      <c r="V35" s="79"/>
-      <c r="W35" s="79"/>
-      <c r="X35" s="79"/>
-      <c r="Y35" s="79"/>
-      <c r="Z35" s="79"/>
-      <c r="AA35" s="79"/>
-      <c r="AB35" s="79"/>
-      <c r="AC35" s="79"/>
-      <c r="AD35" s="79"/>
-      <c r="AE35" s="79"/>
-      <c r="AF35" s="79"/>
-      <c r="AG35" s="79"/>
-      <c r="AH35" s="79"/>
-      <c r="AI35" s="79"/>
-      <c r="AJ35" s="79"/>
-      <c r="AK35" s="79"/>
-      <c r="AL35" s="79"/>
-      <c r="AM35" s="79"/>
-      <c r="AN35" s="79"/>
-      <c r="AO35" s="79"/>
-      <c r="AP35" s="79"/>
-      <c r="AQ35" s="79"/>
-      <c r="AR35" s="79"/>
-      <c r="AS35" s="79"/>
-      <c r="AT35" s="79"/>
-      <c r="AU35" s="110"/>
-      <c r="AV35" s="110"/>
-      <c r="AW35" s="110"/>
-      <c r="AX35" s="110"/>
-      <c r="AY35" s="110"/>
-      <c r="AZ35" s="79"/>
-      <c r="BA35" s="79"/>
-      <c r="BB35" s="79"/>
-      <c r="BC35" s="79"/>
-      <c r="BD35" s="79"/>
-      <c r="BE35" s="79"/>
-      <c r="BF35" s="79"/>
-      <c r="BG35" s="79"/>
-      <c r="BH35" s="79"/>
-      <c r="BI35" s="79"/>
-      <c r="BJ35" s="79"/>
-      <c r="BK35" s="79"/>
-      <c r="BL35" s="79"/>
-      <c r="BM35" s="79"/>
-      <c r="BN35" s="110"/>
-      <c r="BO35" s="110"/>
-      <c r="BP35" s="110"/>
-      <c r="BQ35" s="110"/>
-      <c r="BR35" s="110"/>
-      <c r="BS35" s="110"/>
-      <c r="BT35" s="110"/>
+        <v>14</v>
+      </c>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="49"/>
+      <c r="O35" s="49"/>
+      <c r="P35" s="107"/>
+      <c r="Q35" s="107"/>
+      <c r="R35" s="107"/>
+      <c r="S35" s="49"/>
+      <c r="T35" s="49"/>
+      <c r="U35" s="49"/>
+      <c r="V35" s="49"/>
+      <c r="W35" s="49"/>
+      <c r="X35" s="49"/>
+      <c r="Y35" s="49"/>
+      <c r="Z35" s="49"/>
+      <c r="AA35" s="49"/>
+      <c r="AB35" s="49"/>
+      <c r="AC35" s="49"/>
+      <c r="AD35" s="49"/>
+      <c r="AE35" s="49"/>
+      <c r="AF35" s="49"/>
+      <c r="AG35" s="49"/>
+      <c r="AH35" s="49"/>
+      <c r="AI35" s="49"/>
+      <c r="AJ35" s="49"/>
+      <c r="AK35" s="49"/>
+      <c r="AL35" s="49"/>
+      <c r="AM35" s="49"/>
+      <c r="AN35" s="49"/>
+      <c r="AO35" s="49"/>
+      <c r="AP35" s="49"/>
+      <c r="AQ35" s="49"/>
+      <c r="AR35" s="49"/>
+      <c r="AS35" s="49"/>
+      <c r="AT35" s="49"/>
+      <c r="AU35" s="107"/>
+      <c r="AV35" s="107"/>
+      <c r="AW35" s="107"/>
+      <c r="AX35" s="107"/>
+      <c r="AY35" s="107"/>
+      <c r="AZ35" s="49"/>
+      <c r="BA35" s="49"/>
+      <c r="BB35" s="49"/>
+      <c r="BC35" s="49"/>
+      <c r="BD35" s="49"/>
+      <c r="BE35" s="49"/>
+      <c r="BF35" s="49"/>
+      <c r="BG35" s="49"/>
+      <c r="BH35" s="49"/>
+      <c r="BI35" s="49"/>
+      <c r="BJ35" s="49"/>
+      <c r="BK35" s="49"/>
+      <c r="BL35" s="49"/>
+      <c r="BM35" s="49"/>
+      <c r="BN35" s="107"/>
+      <c r="BO35" s="107"/>
+      <c r="BP35" s="107"/>
+      <c r="BQ35" s="107"/>
+      <c r="BR35" s="107"/>
+      <c r="BS35" s="107"/>
+      <c r="BT35" s="107"/>
     </row>
     <row r="36" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="12"/>
-      <c r="B36" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="81" t="s">
+      <c r="B36" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="82">
-        <v>1</v>
-      </c>
-      <c r="E36" s="124" t="s">
-        <v>70</v>
-      </c>
-      <c r="F36" s="83">
-        <f>DATE(2023,10,13)</f>
-        <v>45212</v>
-      </c>
-      <c r="G36" s="83">
-        <f>DATE(2023,10,18)</f>
-        <v>45217</v>
+      <c r="D36" s="72">
+        <v>0</v>
+      </c>
+      <c r="E36" s="120" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" s="73">
+        <f>DATE(2023,11,20)</f>
+        <v>45250</v>
+      </c>
+      <c r="G36" s="73">
+        <f>F36+13</f>
+        <v>45263</v>
       </c>
       <c r="H36" s="16"/>
       <c r="I36" s="5">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J36" s="49"/>
       <c r="K36" s="49"/>
@@ -5896,113 +5911,110 @@
     </row>
     <row r="37" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="12"/>
-      <c r="B37" s="80" t="s">
+      <c r="B37" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="C37" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="82">
-        <v>0</v>
-      </c>
-      <c r="E37" s="124">
-        <v>7</v>
-      </c>
-      <c r="F37" s="83">
-        <v>45257</v>
-      </c>
-      <c r="G37" s="83">
-        <v>45263</v>
-      </c>
+      <c r="C37" s="75"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="119"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="78"/>
       <c r="H37" s="16"/>
-      <c r="I37" s="5">
+      <c r="I37" s="5" t="str">
         <f t="shared" si="11"/>
-        <v>7</v>
-      </c>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="49"/>
-      <c r="O37" s="49"/>
-      <c r="P37" s="107"/>
-      <c r="Q37" s="107"/>
-      <c r="R37" s="107"/>
-      <c r="S37" s="49"/>
-      <c r="T37" s="49"/>
-      <c r="U37" s="49"/>
-      <c r="V37" s="49"/>
-      <c r="W37" s="49"/>
-      <c r="X37" s="49"/>
-      <c r="Y37" s="49"/>
-      <c r="Z37" s="49"/>
-      <c r="AA37" s="49"/>
-      <c r="AB37" s="49"/>
-      <c r="AC37" s="49"/>
-      <c r="AD37" s="49"/>
-      <c r="AE37" s="49"/>
-      <c r="AF37" s="49"/>
-      <c r="AG37" s="49"/>
-      <c r="AH37" s="49"/>
-      <c r="AI37" s="49"/>
-      <c r="AJ37" s="49"/>
-      <c r="AK37" s="49"/>
-      <c r="AL37" s="49"/>
-      <c r="AM37" s="49"/>
-      <c r="AN37" s="49"/>
-      <c r="AO37" s="49"/>
-      <c r="AP37" s="49"/>
-      <c r="AQ37" s="49"/>
-      <c r="AR37" s="49"/>
-      <c r="AS37" s="49"/>
-      <c r="AT37" s="49"/>
-      <c r="AU37" s="107"/>
-      <c r="AV37" s="107"/>
-      <c r="AW37" s="107"/>
-      <c r="AX37" s="107"/>
-      <c r="AY37" s="107"/>
-      <c r="AZ37" s="49"/>
-      <c r="BA37" s="49"/>
-      <c r="BB37" s="49"/>
-      <c r="BC37" s="49"/>
-      <c r="BD37" s="49"/>
-      <c r="BE37" s="49"/>
-      <c r="BF37" s="49"/>
-      <c r="BG37" s="49"/>
-      <c r="BH37" s="49"/>
-      <c r="BI37" s="49"/>
-      <c r="BJ37" s="49"/>
-      <c r="BK37" s="49"/>
-      <c r="BL37" s="49"/>
-      <c r="BM37" s="49"/>
-      <c r="BN37" s="107"/>
-      <c r="BO37" s="107"/>
-      <c r="BP37" s="107"/>
-      <c r="BQ37" s="107"/>
-      <c r="BR37" s="107"/>
-      <c r="BS37" s="107"/>
-      <c r="BT37" s="107"/>
+        <v/>
+      </c>
+      <c r="J37" s="79"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="79"/>
+      <c r="N37" s="79"/>
+      <c r="O37" s="79"/>
+      <c r="P37" s="110"/>
+      <c r="Q37" s="110"/>
+      <c r="R37" s="110"/>
+      <c r="S37" s="79"/>
+      <c r="T37" s="79"/>
+      <c r="U37" s="79"/>
+      <c r="V37" s="79"/>
+      <c r="W37" s="79"/>
+      <c r="X37" s="79"/>
+      <c r="Y37" s="79"/>
+      <c r="Z37" s="79"/>
+      <c r="AA37" s="79"/>
+      <c r="AB37" s="79"/>
+      <c r="AC37" s="79"/>
+      <c r="AD37" s="79"/>
+      <c r="AE37" s="79"/>
+      <c r="AF37" s="79"/>
+      <c r="AG37" s="79"/>
+      <c r="AH37" s="79"/>
+      <c r="AI37" s="79"/>
+      <c r="AJ37" s="79"/>
+      <c r="AK37" s="79"/>
+      <c r="AL37" s="79"/>
+      <c r="AM37" s="79"/>
+      <c r="AN37" s="79"/>
+      <c r="AO37" s="79"/>
+      <c r="AP37" s="79"/>
+      <c r="AQ37" s="79"/>
+      <c r="AR37" s="79"/>
+      <c r="AS37" s="79"/>
+      <c r="AT37" s="79"/>
+      <c r="AU37" s="110"/>
+      <c r="AV37" s="110"/>
+      <c r="AW37" s="110"/>
+      <c r="AX37" s="110"/>
+      <c r="AY37" s="110"/>
+      <c r="AZ37" s="79"/>
+      <c r="BA37" s="79"/>
+      <c r="BB37" s="79"/>
+      <c r="BC37" s="79"/>
+      <c r="BD37" s="79"/>
+      <c r="BE37" s="79"/>
+      <c r="BF37" s="79"/>
+      <c r="BG37" s="79"/>
+      <c r="BH37" s="79"/>
+      <c r="BI37" s="79"/>
+      <c r="BJ37" s="79"/>
+      <c r="BK37" s="79"/>
+      <c r="BL37" s="79"/>
+      <c r="BM37" s="79"/>
+      <c r="BN37" s="110"/>
+      <c r="BO37" s="110"/>
+      <c r="BP37" s="110"/>
+      <c r="BQ37" s="110"/>
+      <c r="BR37" s="110"/>
+      <c r="BS37" s="110"/>
+      <c r="BT37" s="110"/>
     </row>
     <row r="38" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="12"/>
       <c r="B38" s="80" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C38" s="81" t="s">
         <v>31</v>
       </c>
       <c r="D38" s="82">
-        <v>0</v>
-      </c>
-      <c r="E38" s="124"/>
+        <v>1</v>
+      </c>
+      <c r="E38" s="124" t="s">
+        <v>68</v>
+      </c>
       <c r="F38" s="83">
-        <v>45229</v>
+        <f>DATE(2023,10,13)</f>
+        <v>45212</v>
       </c>
       <c r="G38" s="83">
-        <v>45263</v>
+        <f>DATE(2023,10,18)</f>
+        <v>45217</v>
       </c>
       <c r="H38" s="16"/>
-      <c r="I38" s="5"/>
+      <c r="I38" s="5">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
       <c r="J38" s="49"/>
       <c r="K38" s="49"/>
       <c r="L38" s="49"/>
@@ -6070,7 +6082,7 @@
     <row r="39" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="12"/>
       <c r="B39" s="80" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C39" s="81" t="s">
         <v>31</v>
@@ -6078,19 +6090,19 @@
       <c r="D39" s="82">
         <v>0</v>
       </c>
-      <c r="E39" s="129" t="s">
-        <v>78</v>
+      <c r="E39" s="124">
+        <v>7</v>
       </c>
       <c r="F39" s="83">
         <v>45257</v>
       </c>
       <c r="G39" s="83">
-        <v>45270</v>
+        <v>45263</v>
       </c>
       <c r="H39" s="16"/>
       <c r="I39" s="5">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="J39" s="49"/>
       <c r="K39" s="49"/>
@@ -6159,7 +6171,7 @@
     <row r="40" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="12"/>
       <c r="B40" s="80" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C40" s="81" t="s">
         <v>31</v>
@@ -6167,20 +6179,15 @@
       <c r="D40" s="82">
         <v>0</v>
       </c>
-      <c r="E40" s="128" t="s">
-        <v>87</v>
-      </c>
+      <c r="E40" s="124"/>
       <c r="F40" s="83">
-        <v>45264</v>
+        <v>45229</v>
       </c>
       <c r="G40" s="83">
-        <v>45270</v>
+        <v>45263</v>
       </c>
       <c r="H40" s="16"/>
-      <c r="I40" s="5">
-        <f t="shared" si="11"/>
-        <v>7</v>
-      </c>
+      <c r="I40" s="5"/>
       <c r="J40" s="49"/>
       <c r="K40" s="49"/>
       <c r="L40" s="49"/>
@@ -6247,171 +6254,349 @@
     </row>
     <row r="41" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="12"/>
-      <c r="B41" s="125" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" s="126"/>
-      <c r="D41" s="127"/>
-      <c r="E41" s="84"/>
-      <c r="F41" s="85"/>
-      <c r="G41" s="85"/>
+      <c r="B41" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="82">
+        <v>0</v>
+      </c>
+      <c r="E41" s="129" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" s="83">
+        <v>45257</v>
+      </c>
+      <c r="G41" s="83">
+        <v>45270</v>
+      </c>
       <c r="H41" s="16"/>
-      <c r="I41" s="5" t="str">
+      <c r="I41" s="5">
+        <f t="shared" si="11"/>
+        <v>14</v>
+      </c>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="49"/>
+      <c r="O41" s="49"/>
+      <c r="P41" s="107"/>
+      <c r="Q41" s="107"/>
+      <c r="R41" s="107"/>
+      <c r="S41" s="49"/>
+      <c r="T41" s="49"/>
+      <c r="U41" s="49"/>
+      <c r="V41" s="49"/>
+      <c r="W41" s="49"/>
+      <c r="X41" s="49"/>
+      <c r="Y41" s="49"/>
+      <c r="Z41" s="49"/>
+      <c r="AA41" s="49"/>
+      <c r="AB41" s="49"/>
+      <c r="AC41" s="49"/>
+      <c r="AD41" s="49"/>
+      <c r="AE41" s="49"/>
+      <c r="AF41" s="49"/>
+      <c r="AG41" s="49"/>
+      <c r="AH41" s="49"/>
+      <c r="AI41" s="49"/>
+      <c r="AJ41" s="49"/>
+      <c r="AK41" s="49"/>
+      <c r="AL41" s="49"/>
+      <c r="AM41" s="49"/>
+      <c r="AN41" s="49"/>
+      <c r="AO41" s="49"/>
+      <c r="AP41" s="49"/>
+      <c r="AQ41" s="49"/>
+      <c r="AR41" s="49"/>
+      <c r="AS41" s="49"/>
+      <c r="AT41" s="49"/>
+      <c r="AU41" s="107"/>
+      <c r="AV41" s="107"/>
+      <c r="AW41" s="107"/>
+      <c r="AX41" s="107"/>
+      <c r="AY41" s="107"/>
+      <c r="AZ41" s="49"/>
+      <c r="BA41" s="49"/>
+      <c r="BB41" s="49"/>
+      <c r="BC41" s="49"/>
+      <c r="BD41" s="49"/>
+      <c r="BE41" s="49"/>
+      <c r="BF41" s="49"/>
+      <c r="BG41" s="49"/>
+      <c r="BH41" s="49"/>
+      <c r="BI41" s="49"/>
+      <c r="BJ41" s="49"/>
+      <c r="BK41" s="49"/>
+      <c r="BL41" s="49"/>
+      <c r="BM41" s="49"/>
+      <c r="BN41" s="107"/>
+      <c r="BO41" s="107"/>
+      <c r="BP41" s="107"/>
+      <c r="BQ41" s="107"/>
+      <c r="BR41" s="107"/>
+      <c r="BS41" s="107"/>
+      <c r="BT41" s="107"/>
+    </row>
+    <row r="42" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A42" s="12"/>
+      <c r="B42" s="80" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="82">
+        <v>0</v>
+      </c>
+      <c r="E42" s="128" t="s">
+        <v>85</v>
+      </c>
+      <c r="F42" s="83">
+        <v>45264</v>
+      </c>
+      <c r="G42" s="83">
+        <v>45270</v>
+      </c>
+      <c r="H42" s="16"/>
+      <c r="I42" s="5">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="49"/>
+      <c r="P42" s="107"/>
+      <c r="Q42" s="107"/>
+      <c r="R42" s="107"/>
+      <c r="S42" s="49"/>
+      <c r="T42" s="49"/>
+      <c r="U42" s="49"/>
+      <c r="V42" s="49"/>
+      <c r="W42" s="49"/>
+      <c r="X42" s="49"/>
+      <c r="Y42" s="49"/>
+      <c r="Z42" s="49"/>
+      <c r="AA42" s="49"/>
+      <c r="AB42" s="49"/>
+      <c r="AC42" s="49"/>
+      <c r="AD42" s="49"/>
+      <c r="AE42" s="49"/>
+      <c r="AF42" s="49"/>
+      <c r="AG42" s="49"/>
+      <c r="AH42" s="49"/>
+      <c r="AI42" s="49"/>
+      <c r="AJ42" s="49"/>
+      <c r="AK42" s="49"/>
+      <c r="AL42" s="49"/>
+      <c r="AM42" s="49"/>
+      <c r="AN42" s="49"/>
+      <c r="AO42" s="49"/>
+      <c r="AP42" s="49"/>
+      <c r="AQ42" s="49"/>
+      <c r="AR42" s="49"/>
+      <c r="AS42" s="49"/>
+      <c r="AT42" s="49"/>
+      <c r="AU42" s="107"/>
+      <c r="AV42" s="107"/>
+      <c r="AW42" s="107"/>
+      <c r="AX42" s="107"/>
+      <c r="AY42" s="107"/>
+      <c r="AZ42" s="49"/>
+      <c r="BA42" s="49"/>
+      <c r="BB42" s="49"/>
+      <c r="BC42" s="49"/>
+      <c r="BD42" s="49"/>
+      <c r="BE42" s="49"/>
+      <c r="BF42" s="49"/>
+      <c r="BG42" s="49"/>
+      <c r="BH42" s="49"/>
+      <c r="BI42" s="49"/>
+      <c r="BJ42" s="49"/>
+      <c r="BK42" s="49"/>
+      <c r="BL42" s="49"/>
+      <c r="BM42" s="49"/>
+      <c r="BN42" s="107"/>
+      <c r="BO42" s="107"/>
+      <c r="BP42" s="107"/>
+      <c r="BQ42" s="107"/>
+      <c r="BR42" s="107"/>
+      <c r="BS42" s="107"/>
+      <c r="BT42" s="107"/>
+    </row>
+    <row r="43" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="12"/>
+      <c r="B43" s="125" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="126"/>
+      <c r="D43" s="127"/>
+      <c r="E43" s="84"/>
+      <c r="F43" s="85"/>
+      <c r="G43" s="85"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="5" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
-      <c r="M41" s="43"/>
-      <c r="N41" s="43"/>
-      <c r="O41" s="43"/>
-      <c r="P41" s="106"/>
-      <c r="Q41" s="106"/>
-      <c r="R41" s="106"/>
-      <c r="S41" s="43"/>
-      <c r="T41" s="43"/>
-      <c r="U41" s="43"/>
-      <c r="V41" s="43"/>
-      <c r="W41" s="43"/>
-      <c r="X41" s="43"/>
-      <c r="Y41" s="43"/>
-      <c r="Z41" s="43"/>
-      <c r="AA41" s="43"/>
-      <c r="AB41" s="43"/>
-      <c r="AC41" s="43"/>
-      <c r="AD41" s="43"/>
-      <c r="AE41" s="43"/>
-      <c r="AF41" s="43"/>
-      <c r="AG41" s="43"/>
-      <c r="AH41" s="43"/>
-      <c r="AI41" s="43"/>
-      <c r="AJ41" s="43"/>
-      <c r="AK41" s="43"/>
-      <c r="AL41" s="43"/>
-      <c r="AM41" s="43"/>
-      <c r="AN41" s="43"/>
-      <c r="AO41" s="43"/>
-      <c r="AP41" s="43"/>
-      <c r="AQ41" s="43"/>
-      <c r="AR41" s="43"/>
-      <c r="AS41" s="43"/>
-      <c r="AT41" s="43"/>
-      <c r="AU41" s="106"/>
-      <c r="AV41" s="106"/>
-      <c r="AW41" s="106"/>
-      <c r="AX41" s="106"/>
-      <c r="AY41" s="106"/>
-      <c r="AZ41" s="43"/>
-      <c r="BA41" s="43"/>
-      <c r="BB41" s="43"/>
-      <c r="BC41" s="43"/>
-      <c r="BD41" s="43"/>
-      <c r="BE41" s="43"/>
-      <c r="BF41" s="43"/>
-      <c r="BG41" s="43"/>
-      <c r="BH41" s="43"/>
-      <c r="BI41" s="43"/>
-      <c r="BJ41" s="43"/>
-      <c r="BK41" s="43"/>
-      <c r="BL41" s="43"/>
-      <c r="BM41" s="43"/>
-      <c r="BN41" s="106"/>
-      <c r="BO41" s="106"/>
-      <c r="BP41" s="106"/>
-      <c r="BQ41" s="106"/>
-      <c r="BR41" s="106"/>
-      <c r="BS41" s="106"/>
-      <c r="BT41" s="106"/>
+      <c r="J43" s="43"/>
+      <c r="K43" s="43"/>
+      <c r="L43" s="43"/>
+      <c r="M43" s="43"/>
+      <c r="N43" s="43"/>
+      <c r="O43" s="43"/>
+      <c r="P43" s="106"/>
+      <c r="Q43" s="106"/>
+      <c r="R43" s="106"/>
+      <c r="S43" s="43"/>
+      <c r="T43" s="43"/>
+      <c r="U43" s="43"/>
+      <c r="V43" s="43"/>
+      <c r="W43" s="43"/>
+      <c r="X43" s="43"/>
+      <c r="Y43" s="43"/>
+      <c r="Z43" s="43"/>
+      <c r="AA43" s="43"/>
+      <c r="AB43" s="43"/>
+      <c r="AC43" s="43"/>
+      <c r="AD43" s="43"/>
+      <c r="AE43" s="43"/>
+      <c r="AF43" s="43"/>
+      <c r="AG43" s="43"/>
+      <c r="AH43" s="43"/>
+      <c r="AI43" s="43"/>
+      <c r="AJ43" s="43"/>
+      <c r="AK43" s="43"/>
+      <c r="AL43" s="43"/>
+      <c r="AM43" s="43"/>
+      <c r="AN43" s="43"/>
+      <c r="AO43" s="43"/>
+      <c r="AP43" s="43"/>
+      <c r="AQ43" s="43"/>
+      <c r="AR43" s="43"/>
+      <c r="AS43" s="43"/>
+      <c r="AT43" s="43"/>
+      <c r="AU43" s="106"/>
+      <c r="AV43" s="106"/>
+      <c r="AW43" s="106"/>
+      <c r="AX43" s="106"/>
+      <c r="AY43" s="106"/>
+      <c r="AZ43" s="43"/>
+      <c r="BA43" s="43"/>
+      <c r="BB43" s="43"/>
+      <c r="BC43" s="43"/>
+      <c r="BD43" s="43"/>
+      <c r="BE43" s="43"/>
+      <c r="BF43" s="43"/>
+      <c r="BG43" s="43"/>
+      <c r="BH43" s="43"/>
+      <c r="BI43" s="43"/>
+      <c r="BJ43" s="43"/>
+      <c r="BK43" s="43"/>
+      <c r="BL43" s="43"/>
+      <c r="BM43" s="43"/>
+      <c r="BN43" s="106"/>
+      <c r="BO43" s="106"/>
+      <c r="BP43" s="106"/>
+      <c r="BQ43" s="106"/>
+      <c r="BR43" s="106"/>
+      <c r="BS43" s="106"/>
+      <c r="BT43" s="106"/>
     </row>
-    <row r="42" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="13"/>
-      <c r="B42" s="86" t="s">
+    <row r="44" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="13"/>
+      <c r="B44" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C42" s="87"/>
-      <c r="D42" s="88"/>
-      <c r="E42" s="88"/>
-      <c r="F42" s="89"/>
-      <c r="G42" s="90"/>
-      <c r="H42" s="90"/>
-      <c r="I42" s="90" t="str">
+      <c r="C44" s="87"/>
+      <c r="D44" s="88"/>
+      <c r="E44" s="88"/>
+      <c r="F44" s="89"/>
+      <c r="G44" s="90"/>
+      <c r="H44" s="90"/>
+      <c r="I44" s="90" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="J42" s="90"/>
-      <c r="K42" s="90"/>
-      <c r="L42" s="90"/>
-      <c r="M42" s="90"/>
-      <c r="N42" s="90"/>
-      <c r="O42" s="90"/>
-      <c r="P42" s="90"/>
-      <c r="Q42" s="90"/>
-      <c r="R42" s="90"/>
-      <c r="S42" s="90"/>
-      <c r="T42" s="90"/>
-      <c r="U42" s="90"/>
-      <c r="V42" s="90"/>
-      <c r="W42" s="90"/>
-      <c r="X42" s="90"/>
-      <c r="Y42" s="90"/>
-      <c r="Z42" s="90"/>
-      <c r="AA42" s="90"/>
-      <c r="AB42" s="90"/>
-      <c r="AC42" s="90"/>
-      <c r="AD42" s="90"/>
-      <c r="AE42" s="90"/>
-      <c r="AF42" s="90"/>
-      <c r="AG42" s="90"/>
-      <c r="AH42" s="90"/>
-      <c r="AI42" s="90"/>
-      <c r="AJ42" s="90"/>
-      <c r="AK42" s="90"/>
-      <c r="AL42" s="90"/>
-      <c r="AM42" s="90"/>
-      <c r="AN42" s="90"/>
-      <c r="AO42" s="90"/>
-      <c r="AP42" s="90"/>
-      <c r="AQ42" s="90"/>
-      <c r="AR42" s="90"/>
-      <c r="AS42" s="90"/>
-      <c r="AT42" s="90"/>
-      <c r="AU42" s="90"/>
-      <c r="AV42" s="90"/>
-      <c r="AW42" s="90"/>
-      <c r="AX42" s="90"/>
-      <c r="AY42" s="90"/>
-      <c r="AZ42" s="90"/>
-      <c r="BA42" s="90"/>
-      <c r="BB42" s="90"/>
-      <c r="BC42" s="90"/>
-      <c r="BD42" s="90"/>
-      <c r="BE42" s="90"/>
-      <c r="BF42" s="90"/>
-      <c r="BG42" s="90"/>
-      <c r="BH42" s="90"/>
-      <c r="BI42" s="90"/>
-      <c r="BJ42" s="90"/>
-      <c r="BK42" s="90"/>
-      <c r="BL42" s="90"/>
-      <c r="BM42" s="90"/>
-      <c r="BN42" s="90"/>
-      <c r="BO42" s="90"/>
-      <c r="BP42" s="90"/>
-      <c r="BQ42" s="90"/>
-      <c r="BR42" s="90"/>
-      <c r="BS42" s="90"/>
-      <c r="BT42" s="90"/>
-    </row>
-    <row r="43" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H43" s="3"/>
-    </row>
-    <row r="44" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C44" s="15"/>
-      <c r="G44" s="14"/>
+      <c r="J44" s="90"/>
+      <c r="K44" s="90"/>
+      <c r="L44" s="90"/>
+      <c r="M44" s="90"/>
+      <c r="N44" s="90"/>
+      <c r="O44" s="90"/>
+      <c r="P44" s="90"/>
+      <c r="Q44" s="90"/>
+      <c r="R44" s="90"/>
+      <c r="S44" s="90"/>
+      <c r="T44" s="90"/>
+      <c r="U44" s="90"/>
+      <c r="V44" s="90"/>
+      <c r="W44" s="90"/>
+      <c r="X44" s="90"/>
+      <c r="Y44" s="90"/>
+      <c r="Z44" s="90"/>
+      <c r="AA44" s="90"/>
+      <c r="AB44" s="90"/>
+      <c r="AC44" s="90"/>
+      <c r="AD44" s="90"/>
+      <c r="AE44" s="90"/>
+      <c r="AF44" s="90"/>
+      <c r="AG44" s="90"/>
+      <c r="AH44" s="90"/>
+      <c r="AI44" s="90"/>
+      <c r="AJ44" s="90"/>
+      <c r="AK44" s="90"/>
+      <c r="AL44" s="90"/>
+      <c r="AM44" s="90"/>
+      <c r="AN44" s="90"/>
+      <c r="AO44" s="90"/>
+      <c r="AP44" s="90"/>
+      <c r="AQ44" s="90"/>
+      <c r="AR44" s="90"/>
+      <c r="AS44" s="90"/>
+      <c r="AT44" s="90"/>
+      <c r="AU44" s="90"/>
+      <c r="AV44" s="90"/>
+      <c r="AW44" s="90"/>
+      <c r="AX44" s="90"/>
+      <c r="AY44" s="90"/>
+      <c r="AZ44" s="90"/>
+      <c r="BA44" s="90"/>
+      <c r="BB44" s="90"/>
+      <c r="BC44" s="90"/>
+      <c r="BD44" s="90"/>
+      <c r="BE44" s="90"/>
+      <c r="BF44" s="90"/>
+      <c r="BG44" s="90"/>
+      <c r="BH44" s="90"/>
+      <c r="BI44" s="90"/>
+      <c r="BJ44" s="90"/>
+      <c r="BK44" s="90"/>
+      <c r="BL44" s="90"/>
+      <c r="BM44" s="90"/>
+      <c r="BN44" s="90"/>
+      <c r="BO44" s="90"/>
+      <c r="BP44" s="90"/>
+      <c r="BQ44" s="90"/>
+      <c r="BR44" s="90"/>
+      <c r="BS44" s="90"/>
+      <c r="BT44" s="90"/>
     </row>
     <row r="45" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C45" s="4"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C46" s="15"/>
+      <c r="G46" s="14"/>
+    </row>
+    <row r="47" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C47" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="31">
@@ -6448,7 +6633,7 @@
     <mergeCell ref="X5:AD5"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
-  <conditionalFormatting sqref="D35:E35 D41:E42 D36:D40 D8:E24 D25:D34">
+  <conditionalFormatting sqref="D37:E37 D43:E44 D38:D42 D8:E24 D25:D36">
     <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6478,7 +6663,7 @@
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J25:BL34 BN25:BT34">
+  <conditionalFormatting sqref="J25:BL36 BN25:BT36">
     <cfRule type="expression" dxfId="47" priority="51">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
@@ -6486,7 +6671,7 @@
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J37:BL40">
+  <conditionalFormatting sqref="J39:BL42">
     <cfRule type="expression" dxfId="45" priority="85">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
@@ -6494,7 +6679,7 @@
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN5:BS8 J5:BL9 J10:BM11 BN9:BT40 J12:BL40">
+  <conditionalFormatting sqref="BN5:BS8 J5:BL9 J10:BM11 BN9:BT42 J12:BL42">
     <cfRule type="expression" dxfId="43" priority="50">
       <formula>AND(TODAY()&gt;=J$6, TODAY()&lt;K$6)</formula>
     </cfRule>
@@ -6515,7 +6700,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BU$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM25:BM34">
+  <conditionalFormatting sqref="BM25:BM36">
     <cfRule type="expression" dxfId="38" priority="97">
       <formula>AND(task_start&lt;=BM$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$6)</formula>
     </cfRule>
@@ -6523,7 +6708,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BU$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM36:BM38">
+  <conditionalFormatting sqref="BM38:BM40">
     <cfRule type="expression" dxfId="36" priority="101">
       <formula>AND(task_start&lt;=BM$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$6)</formula>
     </cfRule>
@@ -6531,7 +6716,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BU$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT5:BT8 BM5:BM9 BM12:BM38">
+  <conditionalFormatting sqref="BT5:BT8 BM5:BM9 BM12:BM40">
     <cfRule type="expression" dxfId="34" priority="104">
       <formula>AND(TODAY()&gt;=BM$6, TODAY()&lt;BU$6)</formula>
     </cfRule>
@@ -6541,7 +6726,7 @@
       <formula>AND(TODAY()&gt;=J$6, TODAY()&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J36:BL36">
+  <conditionalFormatting sqref="J38:BL38">
     <cfRule type="expression" dxfId="32" priority="34">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
@@ -6565,7 +6750,7 @@
       <formula>AND(task_end&gt;=BN$6,task_start&lt;BO$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN37:BO40">
+  <conditionalFormatting sqref="BN39:BO42">
     <cfRule type="expression" dxfId="26" priority="30">
       <formula>AND(task_start&lt;=BN$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BN$6)</formula>
     </cfRule>
@@ -6573,7 +6758,7 @@
       <formula>AND(task_end&gt;=BN$6,task_start&lt;BO$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN36:BO36">
+  <conditionalFormatting sqref="BN38:BO38">
     <cfRule type="expression" dxfId="24" priority="24">
       <formula>AND(task_start&lt;=BN$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BN$6)</formula>
     </cfRule>
@@ -6597,7 +6782,7 @@
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP37:BT40">
+  <conditionalFormatting sqref="BP39:BT42">
     <cfRule type="expression" dxfId="18" priority="22">
       <formula>AND(task_start&lt;=BP$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BP$6)</formula>
     </cfRule>
@@ -6605,7 +6790,7 @@
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP36:BT36">
+  <conditionalFormatting sqref="BP38:BT38">
     <cfRule type="expression" dxfId="16" priority="16">
       <formula>AND(task_start&lt;=BP$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BP$6)</formula>
     </cfRule>
@@ -6613,7 +6798,7 @@
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM39:BM40">
+  <conditionalFormatting sqref="BM41:BM42">
     <cfRule type="expression" dxfId="14" priority="14">
       <formula>AND(task_start&lt;=BM$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$6)</formula>
     </cfRule>
@@ -6621,7 +6806,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BN$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM39:BM40">
+  <conditionalFormatting sqref="BM41:BM42">
     <cfRule type="expression" dxfId="12" priority="13">
       <formula>AND(TODAY()&gt;=BM$6, TODAY()&lt;BN$6)</formula>
     </cfRule>
@@ -6684,8 +6869,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A13:A14" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A18" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A24" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A35" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A42" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A37" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A44" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="R3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -6697,7 +6882,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="44" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <pageSetup paperSize="3" scale="55" orientation="landscape" r:id="rId3"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -6720,7 +6905,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D35:E35 D41:E42 D36:D40 D8:E24 D25:D34</xm:sqref>
+          <xm:sqref>D37:E37 D43:E44 D38:D42 D8:E24 D25:D36</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Added this weeks meeting minutes and updated the gantt chart and schedule.
</commit_message>
<xml_diff>
--- a/docs/gantt-chart/Lakeshore Misfits Project Gantt chart.xlsx
+++ b/docs/gantt-chart/Lakeshore Misfits Project Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khngu\Documents\_GVSU\CIS 641\_Team_Project\_Term_Project\GVSU-CIS641-Lakeshore-Misfits\docs\gantt-chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7EBBF3-F6F2-42FA-B96E-D8A7D0FBF5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA759487-953C-40CE-B324-5139641E60AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="16395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="101">
   <si>
     <t>Insert new rows ABOVE this one</t>
   </si>
@@ -258,9 +258,6 @@
     <t>0 - 1</t>
   </si>
   <si>
-    <t>1 - 6</t>
-  </si>
-  <si>
     <t>Prepare Final Deliverables</t>
   </si>
   <si>
@@ -343,6 +340,18 @@
   </si>
   <si>
     <t>Populate Page Layouts (Static)</t>
+  </si>
+  <si>
+    <t>4 - 6</t>
+  </si>
+  <si>
+    <t>2 - 4</t>
+  </si>
+  <si>
+    <t>UI Cleanup &amp; Facelift</t>
+  </si>
+  <si>
+    <t>0 - 7</t>
   </si>
 </sst>
 </file>
@@ -1315,43 +1324,43 @@
     <xf numFmtId="0" fontId="19" fillId="10" borderId="9" xfId="10" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -2532,10 +2541,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BT47"/>
+  <dimension ref="A1:BT48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="BS44" sqref="B1:BT44"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="BT44" sqref="A1:BT44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2566,28 +2575,28 @@
       <c r="F1" s="19"/>
       <c r="G1" s="20"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="137" t="s">
-        <v>80</v>
-      </c>
-      <c r="K1" s="138"/>
-      <c r="L1" s="138"/>
-      <c r="M1" s="138"/>
-      <c r="N1" s="138"/>
-      <c r="O1" s="138"/>
-      <c r="P1" s="138"/>
-      <c r="Q1" s="135">
+      <c r="J1" s="130" t="s">
+        <v>79</v>
+      </c>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="131"/>
+      <c r="P1" s="131"/>
+      <c r="Q1" s="132">
         <f>DATE(2023,9,13)</f>
         <v>45182</v>
       </c>
-      <c r="R1" s="136"/>
-      <c r="S1" s="136"/>
-      <c r="T1" s="136"/>
-      <c r="U1" s="136"/>
-      <c r="V1" s="136"/>
-      <c r="W1" s="136"/>
-      <c r="X1" s="136"/>
-      <c r="Y1" s="136"/>
-      <c r="Z1" s="136"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
+      <c r="T1" s="133"/>
+      <c r="U1" s="133"/>
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="133"/>
+      <c r="Y1" s="133"/>
+      <c r="Z1" s="133"/>
       <c r="AA1" s="113"/>
       <c r="AU1"/>
       <c r="AV1"/>
@@ -2606,29 +2615,29 @@
       <c r="E2" s="21"/>
       <c r="F2" s="22"/>
       <c r="G2" s="21"/>
-      <c r="I2" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="O2" s="138"/>
+      <c r="I2" s="130" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="131"/>
+      <c r="M2" s="131"/>
+      <c r="N2" s="131"/>
+      <c r="O2" s="131"/>
       <c r="P2" s="112"/>
-      <c r="Q2" s="135">
+      <c r="Q2" s="132">
         <f>DATE(2023,10,16)</f>
         <v>45215</v>
       </c>
-      <c r="R2" s="136"/>
-      <c r="S2" s="136"/>
-      <c r="T2" s="136"/>
-      <c r="U2" s="136"/>
-      <c r="V2" s="136"/>
-      <c r="W2" s="136"/>
-      <c r="X2" s="136"/>
-      <c r="Y2" s="136"/>
-      <c r="Z2" s="136"/>
+      <c r="R2" s="133"/>
+      <c r="S2" s="133"/>
+      <c r="T2" s="133"/>
+      <c r="U2" s="133"/>
+      <c r="V2" s="133"/>
+      <c r="W2" s="133"/>
+      <c r="X2" s="133"/>
+      <c r="Y2" s="133"/>
+      <c r="Z2" s="133"/>
       <c r="AU2"/>
       <c r="AV2"/>
       <c r="AW2"/>
@@ -2642,28 +2651,28 @@
       <c r="E3" s="21"/>
       <c r="F3" s="22"/>
       <c r="G3" s="21"/>
-      <c r="J3" s="137" t="s">
+      <c r="J3" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="138"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="138"/>
-      <c r="O3" s="138"/>
-      <c r="P3" s="138"/>
+      <c r="K3" s="131"/>
+      <c r="L3" s="131"/>
+      <c r="M3" s="131"/>
+      <c r="N3" s="131"/>
+      <c r="O3" s="131"/>
+      <c r="P3" s="131"/>
       <c r="Q3" s="112"/>
-      <c r="R3" s="133">
+      <c r="R3" s="143">
         <v>1</v>
       </c>
-      <c r="S3" s="134"/>
-      <c r="T3" s="134"/>
-      <c r="U3" s="134"/>
-      <c r="V3" s="134"/>
-      <c r="W3" s="134"/>
-      <c r="X3" s="134"/>
-      <c r="Y3" s="134"/>
-      <c r="Z3" s="134"/>
-      <c r="AA3" s="134"/>
+      <c r="S3" s="144"/>
+      <c r="T3" s="144"/>
+      <c r="U3" s="144"/>
+      <c r="V3" s="144"/>
+      <c r="W3" s="144"/>
+      <c r="X3" s="144"/>
+      <c r="Y3" s="144"/>
+      <c r="Z3" s="144"/>
+      <c r="AA3" s="144"/>
       <c r="AU3"/>
       <c r="AV3"/>
       <c r="AW3"/>
@@ -2678,87 +2687,87 @@
       <c r="D4" s="25"/>
       <c r="E4" s="25"/>
       <c r="F4" s="26"/>
-      <c r="J4" s="139" t="s">
+      <c r="J4" s="136" t="s">
         <v>41</v>
       </c>
-      <c r="K4" s="130"/>
-      <c r="L4" s="130"/>
-      <c r="M4" s="130"/>
-      <c r="N4" s="130"/>
-      <c r="O4" s="130"/>
-      <c r="P4" s="130"/>
-      <c r="Q4" s="130" t="s">
+      <c r="K4" s="134"/>
+      <c r="L4" s="134"/>
+      <c r="M4" s="134"/>
+      <c r="N4" s="134"/>
+      <c r="O4" s="134"/>
+      <c r="P4" s="134"/>
+      <c r="Q4" s="134" t="s">
         <v>42</v>
       </c>
-      <c r="R4" s="130"/>
-      <c r="S4" s="130"/>
-      <c r="T4" s="130"/>
-      <c r="U4" s="130"/>
-      <c r="V4" s="130"/>
-      <c r="W4" s="130"/>
-      <c r="X4" s="130" t="s">
+      <c r="R4" s="134"/>
+      <c r="S4" s="134"/>
+      <c r="T4" s="134"/>
+      <c r="U4" s="134"/>
+      <c r="V4" s="134"/>
+      <c r="W4" s="134"/>
+      <c r="X4" s="134" t="s">
         <v>43</v>
       </c>
-      <c r="Y4" s="130"/>
-      <c r="Z4" s="130"/>
-      <c r="AA4" s="130"/>
-      <c r="AB4" s="130"/>
-      <c r="AC4" s="130"/>
-      <c r="AD4" s="130"/>
-      <c r="AE4" s="130" t="s">
+      <c r="Y4" s="134"/>
+      <c r="Z4" s="134"/>
+      <c r="AA4" s="134"/>
+      <c r="AB4" s="134"/>
+      <c r="AC4" s="134"/>
+      <c r="AD4" s="134"/>
+      <c r="AE4" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="AF4" s="130"/>
-      <c r="AG4" s="130"/>
-      <c r="AH4" s="130"/>
-      <c r="AI4" s="130"/>
-      <c r="AJ4" s="130"/>
-      <c r="AK4" s="130"/>
-      <c r="AL4" s="130" t="s">
+      <c r="AF4" s="134"/>
+      <c r="AG4" s="134"/>
+      <c r="AH4" s="134"/>
+      <c r="AI4" s="134"/>
+      <c r="AJ4" s="134"/>
+      <c r="AK4" s="134"/>
+      <c r="AL4" s="134" t="s">
         <v>45</v>
       </c>
-      <c r="AM4" s="130"/>
-      <c r="AN4" s="130"/>
-      <c r="AO4" s="130"/>
-      <c r="AP4" s="130"/>
-      <c r="AQ4" s="130"/>
-      <c r="AR4" s="130"/>
-      <c r="AS4" s="130" t="s">
+      <c r="AM4" s="134"/>
+      <c r="AN4" s="134"/>
+      <c r="AO4" s="134"/>
+      <c r="AP4" s="134"/>
+      <c r="AQ4" s="134"/>
+      <c r="AR4" s="134"/>
+      <c r="AS4" s="134" t="s">
         <v>46</v>
       </c>
-      <c r="AT4" s="130"/>
-      <c r="AU4" s="130"/>
-      <c r="AV4" s="130"/>
-      <c r="AW4" s="130"/>
-      <c r="AX4" s="130"/>
-      <c r="AY4" s="130"/>
-      <c r="AZ4" s="130" t="s">
+      <c r="AT4" s="134"/>
+      <c r="AU4" s="134"/>
+      <c r="AV4" s="134"/>
+      <c r="AW4" s="134"/>
+      <c r="AX4" s="134"/>
+      <c r="AY4" s="134"/>
+      <c r="AZ4" s="134" t="s">
         <v>47</v>
       </c>
-      <c r="BA4" s="130"/>
-      <c r="BB4" s="130"/>
-      <c r="BC4" s="130"/>
-      <c r="BD4" s="130"/>
-      <c r="BE4" s="130"/>
-      <c r="BF4" s="130"/>
-      <c r="BG4" s="130" t="s">
+      <c r="BA4" s="134"/>
+      <c r="BB4" s="134"/>
+      <c r="BC4" s="134"/>
+      <c r="BD4" s="134"/>
+      <c r="BE4" s="134"/>
+      <c r="BF4" s="134"/>
+      <c r="BG4" s="134" t="s">
         <v>48</v>
       </c>
-      <c r="BH4" s="130"/>
-      <c r="BI4" s="130"/>
-      <c r="BJ4" s="130"/>
-      <c r="BK4" s="130"/>
-      <c r="BL4" s="130"/>
-      <c r="BM4" s="130"/>
-      <c r="BN4" s="130" t="s">
+      <c r="BH4" s="134"/>
+      <c r="BI4" s="134"/>
+      <c r="BJ4" s="134"/>
+      <c r="BK4" s="134"/>
+      <c r="BL4" s="134"/>
+      <c r="BM4" s="134"/>
+      <c r="BN4" s="134" t="s">
         <v>49</v>
       </c>
-      <c r="BO4" s="130"/>
-      <c r="BP4" s="130"/>
-      <c r="BQ4" s="130"/>
-      <c r="BR4" s="130"/>
-      <c r="BS4" s="130"/>
-      <c r="BT4" s="130"/>
+      <c r="BO4" s="134"/>
+      <c r="BP4" s="134"/>
+      <c r="BQ4" s="134"/>
+      <c r="BR4" s="134"/>
+      <c r="BS4" s="134"/>
+      <c r="BT4" s="134"/>
     </row>
     <row r="5" spans="1:72" s="24" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13"/>
@@ -2766,115 +2775,115 @@
         <v>13</v>
       </c>
       <c r="F5" s="28"/>
-      <c r="J5" s="139">
+      <c r="J5" s="136">
         <f>J6</f>
         <v>45215</v>
       </c>
-      <c r="K5" s="130"/>
-      <c r="L5" s="130"/>
-      <c r="M5" s="130"/>
-      <c r="N5" s="130"/>
-      <c r="O5" s="130"/>
-      <c r="P5" s="130"/>
-      <c r="Q5" s="130">
+      <c r="K5" s="134"/>
+      <c r="L5" s="134"/>
+      <c r="M5" s="134"/>
+      <c r="N5" s="134"/>
+      <c r="O5" s="134"/>
+      <c r="P5" s="134"/>
+      <c r="Q5" s="134">
         <f>Q6</f>
         <v>45222</v>
       </c>
-      <c r="R5" s="130"/>
-      <c r="S5" s="130"/>
-      <c r="T5" s="130"/>
-      <c r="U5" s="130"/>
-      <c r="V5" s="130"/>
-      <c r="W5" s="130"/>
-      <c r="X5" s="130">
+      <c r="R5" s="134"/>
+      <c r="S5" s="134"/>
+      <c r="T5" s="134"/>
+      <c r="U5" s="134"/>
+      <c r="V5" s="134"/>
+      <c r="W5" s="134"/>
+      <c r="X5" s="134">
         <f>X6</f>
         <v>45229</v>
       </c>
-      <c r="Y5" s="130"/>
-      <c r="Z5" s="130"/>
-      <c r="AA5" s="130"/>
-      <c r="AB5" s="130"/>
-      <c r="AC5" s="130"/>
-      <c r="AD5" s="130"/>
-      <c r="AE5" s="130">
+      <c r="Y5" s="134"/>
+      <c r="Z5" s="134"/>
+      <c r="AA5" s="134"/>
+      <c r="AB5" s="134"/>
+      <c r="AC5" s="134"/>
+      <c r="AD5" s="134"/>
+      <c r="AE5" s="134">
         <f>AE6</f>
         <v>45236</v>
       </c>
-      <c r="AF5" s="130"/>
-      <c r="AG5" s="130"/>
-      <c r="AH5" s="130"/>
-      <c r="AI5" s="130"/>
-      <c r="AJ5" s="130"/>
-      <c r="AK5" s="130"/>
-      <c r="AL5" s="130">
+      <c r="AF5" s="134"/>
+      <c r="AG5" s="134"/>
+      <c r="AH5" s="134"/>
+      <c r="AI5" s="134"/>
+      <c r="AJ5" s="134"/>
+      <c r="AK5" s="134"/>
+      <c r="AL5" s="134">
         <f>AL6</f>
         <v>45243</v>
       </c>
-      <c r="AM5" s="130"/>
-      <c r="AN5" s="130"/>
-      <c r="AO5" s="130"/>
-      <c r="AP5" s="130"/>
-      <c r="AQ5" s="130"/>
-      <c r="AR5" s="130"/>
-      <c r="AS5" s="130">
+      <c r="AM5" s="134"/>
+      <c r="AN5" s="134"/>
+      <c r="AO5" s="134"/>
+      <c r="AP5" s="134"/>
+      <c r="AQ5" s="134"/>
+      <c r="AR5" s="134"/>
+      <c r="AS5" s="134">
         <f>AS6</f>
         <v>45250</v>
       </c>
-      <c r="AT5" s="130"/>
-      <c r="AU5" s="130"/>
-      <c r="AV5" s="130"/>
-      <c r="AW5" s="130"/>
-      <c r="AX5" s="130"/>
-      <c r="AY5" s="130"/>
-      <c r="AZ5" s="130">
+      <c r="AT5" s="134"/>
+      <c r="AU5" s="134"/>
+      <c r="AV5" s="134"/>
+      <c r="AW5" s="134"/>
+      <c r="AX5" s="134"/>
+      <c r="AY5" s="134"/>
+      <c r="AZ5" s="134">
         <f>AZ6</f>
         <v>45257</v>
       </c>
-      <c r="BA5" s="130"/>
-      <c r="BB5" s="130"/>
-      <c r="BC5" s="130"/>
-      <c r="BD5" s="130"/>
-      <c r="BE5" s="130"/>
-      <c r="BF5" s="130"/>
-      <c r="BG5" s="130">
+      <c r="BA5" s="134"/>
+      <c r="BB5" s="134"/>
+      <c r="BC5" s="134"/>
+      <c r="BD5" s="134"/>
+      <c r="BE5" s="134"/>
+      <c r="BF5" s="134"/>
+      <c r="BG5" s="134">
         <f>BG6</f>
         <v>45264</v>
       </c>
-      <c r="BH5" s="130"/>
-      <c r="BI5" s="130"/>
-      <c r="BJ5" s="130"/>
-      <c r="BK5" s="130"/>
-      <c r="BL5" s="130"/>
-      <c r="BM5" s="144"/>
-      <c r="BN5" s="130">
+      <c r="BH5" s="134"/>
+      <c r="BI5" s="134"/>
+      <c r="BJ5" s="134"/>
+      <c r="BK5" s="134"/>
+      <c r="BL5" s="134"/>
+      <c r="BM5" s="135"/>
+      <c r="BN5" s="134">
         <f>BN6</f>
         <v>45271</v>
       </c>
-      <c r="BO5" s="130"/>
-      <c r="BP5" s="130"/>
-      <c r="BQ5" s="130"/>
-      <c r="BR5" s="130"/>
-      <c r="BS5" s="130"/>
-      <c r="BT5" s="144"/>
+      <c r="BO5" s="134"/>
+      <c r="BP5" s="134"/>
+      <c r="BQ5" s="134"/>
+      <c r="BR5" s="134"/>
+      <c r="BS5" s="134"/>
+      <c r="BT5" s="135"/>
     </row>
     <row r="6" spans="1:72" s="24" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="140"/>
-      <c r="B6" s="141" t="s">
+      <c r="A6" s="137"/>
+      <c r="B6" s="138" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="143" t="s">
+      <c r="C6" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="131" t="s">
+      <c r="D6" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="131" t="s">
+      <c r="E6" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="131" t="s">
+      <c r="F6" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="131" t="s">
+      <c r="G6" s="142" t="s">
         <v>4</v>
       </c>
       <c r="J6" s="29">
@@ -3131,13 +3140,13 @@
       </c>
     </row>
     <row r="7" spans="1:72" s="24" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="140"/>
-      <c r="B7" s="142"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132"/>
-      <c r="E7" s="132"/>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
+      <c r="A7" s="137"/>
+      <c r="B7" s="139"/>
+      <c r="C7" s="141"/>
+      <c r="D7" s="141"/>
+      <c r="E7" s="141"/>
+      <c r="F7" s="141"/>
+      <c r="G7" s="141"/>
       <c r="J7" s="32" t="str">
         <f t="shared" ref="J7:AO7" si="8">LEFT(TEXT(J6,"ddd"),1)</f>
         <v>M</v>
@@ -3481,7 +3490,7 @@
       <c r="G9" s="42"/>
       <c r="H9" s="16"/>
       <c r="I9" s="5" t="str">
-        <f t="shared" ref="I9:I44" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="I9:I45" si="11">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="J9" s="43"/>
@@ -3545,7 +3554,7 @@
       <c r="BL9" s="43"/>
       <c r="BM9" s="43"/>
       <c r="BN9" s="106" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BO9" s="106"/>
       <c r="BP9" s="106"/>
@@ -3557,7 +3566,7 @@
     <row r="10" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="13"/>
       <c r="B10" s="45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="46" t="s">
         <v>31</v>
@@ -3566,7 +3575,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E10" s="114" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F10" s="48">
         <f>Q1</f>
@@ -3647,7 +3656,7 @@
     <row r="11" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="13"/>
       <c r="B11" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" s="46" t="s">
         <v>31</v>
@@ -3656,7 +3665,7 @@
         <v>0.5</v>
       </c>
       <c r="E11" s="114" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="48">
         <f>DATE(2023,9,20)</f>
@@ -3737,7 +3746,7 @@
     <row r="12" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="13"/>
       <c r="B12" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C12" s="46" t="s">
         <v>31</v>
@@ -3837,7 +3846,7 @@
         <v>0.5</v>
       </c>
       <c r="E13" s="123" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="53">
         <f>DATE(2023,10,13)</f>
@@ -3928,7 +3937,7 @@
         <v>0.4</v>
       </c>
       <c r="E14" s="123" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" s="53">
         <f>Project_Start</f>
@@ -4007,16 +4016,16 @@
     <row r="15" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="12"/>
       <c r="B15" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" s="51" t="s">
         <v>31</v>
       </c>
       <c r="D15" s="52">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="E15" s="114" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F15" s="53">
         <f>DATE(2023,9,27)</f>
@@ -4098,16 +4107,16 @@
     <row r="16" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="12"/>
       <c r="B16" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="51" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="52">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="E16" s="123" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="F16" s="53">
         <f>DATE(2023,10,25)</f>
@@ -4189,7 +4198,7 @@
     <row r="17" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="12"/>
       <c r="B17" s="50" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="51" t="s">
         <v>31</v>
@@ -4198,7 +4207,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="123" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F17" s="53">
         <f>DATE(2023,10,12)</f>
@@ -5011,7 +5020,7 @@
     <row r="27" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="12"/>
       <c r="B27" s="70" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C27" s="71" t="s">
         <v>35</v>
@@ -5102,7 +5111,7 @@
     <row r="28" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="12"/>
       <c r="B28" s="70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="71" t="s">
         <v>35</v>
@@ -5190,13 +5199,13 @@
     <row r="29" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="12"/>
       <c r="B29" s="70" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C29" s="71" t="s">
         <v>35</v>
       </c>
       <c r="D29" s="72">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E29" s="121" t="s">
         <v>53</v>
@@ -5284,10 +5293,10 @@
         <v>51</v>
       </c>
       <c r="C30" s="71" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" s="72">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="120" t="s">
         <v>54</v>
@@ -5372,7 +5381,7 @@
     <row r="31" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="12"/>
       <c r="B31" s="70" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" s="71" t="s">
         <v>38</v>
@@ -5463,24 +5472,24 @@
     <row r="32" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="12"/>
       <c r="B32" s="70" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C32" s="71" t="s">
         <v>35</v>
       </c>
       <c r="D32" s="72">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="E32" s="122" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F32" s="73">
         <f>DATE(2023,10,23)</f>
         <v>45222</v>
       </c>
       <c r="G32" s="73">
-        <f>DATE(2023,11,11)</f>
-        <v>45241</v>
+        <f>DATE(2023,11,12)</f>
+        <v>45242</v>
       </c>
       <c r="H32" s="16"/>
       <c r="I32" s="5"/>
@@ -5551,24 +5560,24 @@
     <row r="33" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="12"/>
       <c r="B33" s="70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" s="71" t="s">
         <v>35</v>
       </c>
       <c r="D33" s="72">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E33" s="122" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F33" s="73">
         <f>DATE(2023,10,23)</f>
         <v>45222</v>
       </c>
       <c r="G33" s="73">
-        <f>DATE(2023,11,11)</f>
-        <v>45241</v>
+        <f>DATE(2023,11,12)</f>
+        <v>45242</v>
       </c>
       <c r="H33" s="16"/>
       <c r="I33" s="5"/>
@@ -5639,13 +5648,13 @@
     <row r="34" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="12"/>
       <c r="B34" s="70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C34" s="71" t="s">
         <v>31</v>
       </c>
       <c r="D34" s="72">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E34" s="122" t="s">
         <v>60</v>
@@ -5736,23 +5745,23 @@
         <v>31</v>
       </c>
       <c r="D35" s="72">
-        <v>0.1</v>
-      </c>
-      <c r="E35" s="120" t="s">
-        <v>60</v>
+        <v>0.5</v>
+      </c>
+      <c r="E35" s="121" t="s">
+        <v>97</v>
       </c>
       <c r="F35" s="73">
         <f>G31+1</f>
         <v>45236</v>
       </c>
       <c r="G35" s="73">
-        <f>F35+13</f>
-        <v>45249</v>
+        <f>DATE(2023,11,26)</f>
+        <v>45256</v>
       </c>
       <c r="H35" s="16"/>
       <c r="I35" s="5">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="J35" s="49"/>
       <c r="K35" s="49"/>
@@ -5821,29 +5830,29 @@
     <row r="36" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="12"/>
       <c r="B36" s="70" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="C36" s="71" t="s">
         <v>31</v>
       </c>
       <c r="D36" s="72">
-        <v>0</v>
-      </c>
-      <c r="E36" s="120" t="s">
-        <v>61</v>
+        <v>0.05</v>
+      </c>
+      <c r="E36" s="120">
+        <v>6</v>
       </c>
       <c r="F36" s="73">
         <f>DATE(2023,11,20)</f>
         <v>45250</v>
       </c>
       <c r="G36" s="73">
-        <f>F36+13</f>
-        <v>45263</v>
+        <f>DATE(2023,11,26)</f>
+        <v>45256</v>
       </c>
       <c r="H36" s="16"/>
       <c r="I36" s="5">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="J36" s="49"/>
       <c r="K36" s="49"/>
@@ -5911,198 +5920,200 @@
     </row>
     <row r="37" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="12"/>
-      <c r="B37" s="74" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="75"/>
-      <c r="D37" s="76"/>
-      <c r="E37" s="119"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="78"/>
+      <c r="B37" s="70" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="71" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="72">
+        <v>0.05</v>
+      </c>
+      <c r="E37" s="120" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" s="73">
+        <f>DATE(2023,11,20)</f>
+        <v>45250</v>
+      </c>
+      <c r="G37" s="73">
+        <f>F37+13</f>
+        <v>45263</v>
+      </c>
       <c r="H37" s="16"/>
-      <c r="I37" s="5" t="str">
+      <c r="I37" s="5">
         <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="J37" s="79"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="79"/>
-      <c r="N37" s="79"/>
-      <c r="O37" s="79"/>
-      <c r="P37" s="110"/>
-      <c r="Q37" s="110"/>
-      <c r="R37" s="110"/>
-      <c r="S37" s="79"/>
-      <c r="T37" s="79"/>
-      <c r="U37" s="79"/>
-      <c r="V37" s="79"/>
-      <c r="W37" s="79"/>
-      <c r="X37" s="79"/>
-      <c r="Y37" s="79"/>
-      <c r="Z37" s="79"/>
-      <c r="AA37" s="79"/>
-      <c r="AB37" s="79"/>
-      <c r="AC37" s="79"/>
-      <c r="AD37" s="79"/>
-      <c r="AE37" s="79"/>
-      <c r="AF37" s="79"/>
-      <c r="AG37" s="79"/>
-      <c r="AH37" s="79"/>
-      <c r="AI37" s="79"/>
-      <c r="AJ37" s="79"/>
-      <c r="AK37" s="79"/>
-      <c r="AL37" s="79"/>
-      <c r="AM37" s="79"/>
-      <c r="AN37" s="79"/>
-      <c r="AO37" s="79"/>
-      <c r="AP37" s="79"/>
-      <c r="AQ37" s="79"/>
-      <c r="AR37" s="79"/>
-      <c r="AS37" s="79"/>
-      <c r="AT37" s="79"/>
-      <c r="AU37" s="110"/>
-      <c r="AV37" s="110"/>
-      <c r="AW37" s="110"/>
-      <c r="AX37" s="110"/>
-      <c r="AY37" s="110"/>
-      <c r="AZ37" s="79"/>
-      <c r="BA37" s="79"/>
-      <c r="BB37" s="79"/>
-      <c r="BC37" s="79"/>
-      <c r="BD37" s="79"/>
-      <c r="BE37" s="79"/>
-      <c r="BF37" s="79"/>
-      <c r="BG37" s="79"/>
-      <c r="BH37" s="79"/>
-      <c r="BI37" s="79"/>
-      <c r="BJ37" s="79"/>
-      <c r="BK37" s="79"/>
-      <c r="BL37" s="79"/>
-      <c r="BM37" s="79"/>
-      <c r="BN37" s="110"/>
-      <c r="BO37" s="110"/>
-      <c r="BP37" s="110"/>
-      <c r="BQ37" s="110"/>
-      <c r="BR37" s="110"/>
-      <c r="BS37" s="110"/>
-      <c r="BT37" s="110"/>
+        <v>14</v>
+      </c>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="49"/>
+      <c r="N37" s="49"/>
+      <c r="O37" s="49"/>
+      <c r="P37" s="107"/>
+      <c r="Q37" s="107"/>
+      <c r="R37" s="107"/>
+      <c r="S37" s="49"/>
+      <c r="T37" s="49"/>
+      <c r="U37" s="49"/>
+      <c r="V37" s="49"/>
+      <c r="W37" s="49"/>
+      <c r="X37" s="49"/>
+      <c r="Y37" s="49"/>
+      <c r="Z37" s="49"/>
+      <c r="AA37" s="49"/>
+      <c r="AB37" s="49"/>
+      <c r="AC37" s="49"/>
+      <c r="AD37" s="49"/>
+      <c r="AE37" s="49"/>
+      <c r="AF37" s="49"/>
+      <c r="AG37" s="49"/>
+      <c r="AH37" s="49"/>
+      <c r="AI37" s="49"/>
+      <c r="AJ37" s="49"/>
+      <c r="AK37" s="49"/>
+      <c r="AL37" s="49"/>
+      <c r="AM37" s="49"/>
+      <c r="AN37" s="49"/>
+      <c r="AO37" s="49"/>
+      <c r="AP37" s="49"/>
+      <c r="AQ37" s="49"/>
+      <c r="AR37" s="49"/>
+      <c r="AS37" s="49"/>
+      <c r="AT37" s="49"/>
+      <c r="AU37" s="107"/>
+      <c r="AV37" s="107"/>
+      <c r="AW37" s="107"/>
+      <c r="AX37" s="107"/>
+      <c r="AY37" s="107"/>
+      <c r="AZ37" s="49"/>
+      <c r="BA37" s="49"/>
+      <c r="BB37" s="49"/>
+      <c r="BC37" s="49"/>
+      <c r="BD37" s="49"/>
+      <c r="BE37" s="49"/>
+      <c r="BF37" s="49"/>
+      <c r="BG37" s="49"/>
+      <c r="BH37" s="49"/>
+      <c r="BI37" s="49"/>
+      <c r="BJ37" s="49"/>
+      <c r="BK37" s="49"/>
+      <c r="BL37" s="49"/>
+      <c r="BM37" s="49"/>
+      <c r="BN37" s="107"/>
+      <c r="BO37" s="107"/>
+      <c r="BP37" s="107"/>
+      <c r="BQ37" s="107"/>
+      <c r="BR37" s="107"/>
+      <c r="BS37" s="107"/>
+      <c r="BT37" s="107"/>
     </row>
     <row r="38" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="12"/>
-      <c r="B38" s="80" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="82">
-        <v>1</v>
-      </c>
-      <c r="E38" s="124" t="s">
-        <v>68</v>
-      </c>
-      <c r="F38" s="83">
-        <f>DATE(2023,10,13)</f>
-        <v>45212</v>
-      </c>
-      <c r="G38" s="83">
-        <f>DATE(2023,10,18)</f>
-        <v>45217</v>
-      </c>
+      <c r="B38" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="75"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="119"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="78"/>
       <c r="H38" s="16"/>
-      <c r="I38" s="5">
+      <c r="I38" s="5" t="str">
         <f t="shared" si="11"/>
-        <v>6</v>
-      </c>
-      <c r="J38" s="49"/>
-      <c r="K38" s="49"/>
-      <c r="L38" s="49"/>
-      <c r="M38" s="49"/>
-      <c r="N38" s="49"/>
-      <c r="O38" s="49"/>
-      <c r="P38" s="107"/>
-      <c r="Q38" s="107"/>
-      <c r="R38" s="107"/>
-      <c r="S38" s="49"/>
-      <c r="T38" s="49"/>
-      <c r="U38" s="49"/>
-      <c r="V38" s="49"/>
-      <c r="W38" s="49"/>
-      <c r="X38" s="49"/>
-      <c r="Y38" s="49"/>
-      <c r="Z38" s="49"/>
-      <c r="AA38" s="49"/>
-      <c r="AB38" s="49"/>
-      <c r="AC38" s="49"/>
-      <c r="AD38" s="49"/>
-      <c r="AE38" s="49"/>
-      <c r="AF38" s="49"/>
-      <c r="AG38" s="49"/>
-      <c r="AH38" s="49"/>
-      <c r="AI38" s="49"/>
-      <c r="AJ38" s="49"/>
-      <c r="AK38" s="49"/>
-      <c r="AL38" s="49"/>
-      <c r="AM38" s="49"/>
-      <c r="AN38" s="49"/>
-      <c r="AO38" s="49"/>
-      <c r="AP38" s="49"/>
-      <c r="AQ38" s="49"/>
-      <c r="AR38" s="49"/>
-      <c r="AS38" s="49"/>
-      <c r="AT38" s="49"/>
-      <c r="AU38" s="107"/>
-      <c r="AV38" s="107"/>
-      <c r="AW38" s="107"/>
-      <c r="AX38" s="107"/>
-      <c r="AY38" s="107"/>
-      <c r="AZ38" s="49"/>
-      <c r="BA38" s="49"/>
-      <c r="BB38" s="49"/>
-      <c r="BC38" s="49"/>
-      <c r="BD38" s="49"/>
-      <c r="BE38" s="49"/>
-      <c r="BF38" s="49"/>
-      <c r="BG38" s="49"/>
-      <c r="BH38" s="49"/>
-      <c r="BI38" s="49"/>
-      <c r="BJ38" s="49"/>
-      <c r="BK38" s="49"/>
-      <c r="BL38" s="49"/>
-      <c r="BM38" s="49"/>
-      <c r="BN38" s="107"/>
-      <c r="BO38" s="107"/>
-      <c r="BP38" s="107"/>
-      <c r="BQ38" s="107"/>
-      <c r="BR38" s="107"/>
-      <c r="BS38" s="107"/>
-      <c r="BT38" s="107"/>
+        <v/>
+      </c>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="79"/>
+      <c r="M38" s="79"/>
+      <c r="N38" s="79"/>
+      <c r="O38" s="79"/>
+      <c r="P38" s="110"/>
+      <c r="Q38" s="110"/>
+      <c r="R38" s="110"/>
+      <c r="S38" s="79"/>
+      <c r="T38" s="79"/>
+      <c r="U38" s="79"/>
+      <c r="V38" s="79"/>
+      <c r="W38" s="79"/>
+      <c r="X38" s="79"/>
+      <c r="Y38" s="79"/>
+      <c r="Z38" s="79"/>
+      <c r="AA38" s="79"/>
+      <c r="AB38" s="79"/>
+      <c r="AC38" s="79"/>
+      <c r="AD38" s="79"/>
+      <c r="AE38" s="79"/>
+      <c r="AF38" s="79"/>
+      <c r="AG38" s="79"/>
+      <c r="AH38" s="79"/>
+      <c r="AI38" s="79"/>
+      <c r="AJ38" s="79"/>
+      <c r="AK38" s="79"/>
+      <c r="AL38" s="79"/>
+      <c r="AM38" s="79"/>
+      <c r="AN38" s="79"/>
+      <c r="AO38" s="79"/>
+      <c r="AP38" s="79"/>
+      <c r="AQ38" s="79"/>
+      <c r="AR38" s="79"/>
+      <c r="AS38" s="79"/>
+      <c r="AT38" s="79"/>
+      <c r="AU38" s="110"/>
+      <c r="AV38" s="110"/>
+      <c r="AW38" s="110"/>
+      <c r="AX38" s="110"/>
+      <c r="AY38" s="110"/>
+      <c r="AZ38" s="79"/>
+      <c r="BA38" s="79"/>
+      <c r="BB38" s="79"/>
+      <c r="BC38" s="79"/>
+      <c r="BD38" s="79"/>
+      <c r="BE38" s="79"/>
+      <c r="BF38" s="79"/>
+      <c r="BG38" s="79"/>
+      <c r="BH38" s="79"/>
+      <c r="BI38" s="79"/>
+      <c r="BJ38" s="79"/>
+      <c r="BK38" s="79"/>
+      <c r="BL38" s="79"/>
+      <c r="BM38" s="79"/>
+      <c r="BN38" s="110"/>
+      <c r="BO38" s="110"/>
+      <c r="BP38" s="110"/>
+      <c r="BQ38" s="110"/>
+      <c r="BR38" s="110"/>
+      <c r="BS38" s="110"/>
+      <c r="BT38" s="110"/>
     </row>
     <row r="39" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="12"/>
       <c r="B39" s="80" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C39" s="81" t="s">
         <v>31</v>
       </c>
       <c r="D39" s="82">
-        <v>0</v>
-      </c>
-      <c r="E39" s="124">
-        <v>7</v>
+        <v>1</v>
+      </c>
+      <c r="E39" s="124" t="s">
+        <v>68</v>
       </c>
       <c r="F39" s="83">
-        <v>45257</v>
+        <f>DATE(2023,10,13)</f>
+        <v>45212</v>
       </c>
       <c r="G39" s="83">
-        <v>45263</v>
+        <f>DATE(2023,10,18)</f>
+        <v>45217</v>
       </c>
       <c r="H39" s="16"/>
       <c r="I39" s="5">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J39" s="49"/>
       <c r="K39" s="49"/>
@@ -6171,7 +6182,7 @@
     <row r="40" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="12"/>
       <c r="B40" s="80" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C40" s="81" t="s">
         <v>31</v>
@@ -6179,15 +6190,20 @@
       <c r="D40" s="82">
         <v>0</v>
       </c>
-      <c r="E40" s="124"/>
+      <c r="E40" s="124">
+        <v>7</v>
+      </c>
       <c r="F40" s="83">
-        <v>45229</v>
+        <v>45257</v>
       </c>
       <c r="G40" s="83">
         <v>45263</v>
       </c>
       <c r="H40" s="16"/>
-      <c r="I40" s="5"/>
+      <c r="I40" s="5">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
       <c r="J40" s="49"/>
       <c r="K40" s="49"/>
       <c r="L40" s="49"/>
@@ -6255,7 +6271,7 @@
     <row r="41" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="12"/>
       <c r="B41" s="80" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C41" s="81" t="s">
         <v>31</v>
@@ -6263,20 +6279,17 @@
       <c r="D41" s="82">
         <v>0</v>
       </c>
-      <c r="E41" s="129" t="s">
-        <v>76</v>
+      <c r="E41" s="124" t="s">
+        <v>100</v>
       </c>
       <c r="F41" s="83">
-        <v>45257</v>
+        <v>45229</v>
       </c>
       <c r="G41" s="83">
-        <v>45270</v>
+        <v>45263</v>
       </c>
       <c r="H41" s="16"/>
-      <c r="I41" s="5">
-        <f t="shared" si="11"/>
-        <v>14</v>
-      </c>
+      <c r="I41" s="5"/>
       <c r="J41" s="49"/>
       <c r="K41" s="49"/>
       <c r="L41" s="49"/>
@@ -6344,7 +6357,7 @@
     <row r="42" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="12"/>
       <c r="B42" s="80" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C42" s="81" t="s">
         <v>31</v>
@@ -6352,19 +6365,19 @@
       <c r="D42" s="82">
         <v>0</v>
       </c>
-      <c r="E42" s="128" t="s">
-        <v>85</v>
+      <c r="E42" s="129" t="s">
+        <v>75</v>
       </c>
       <c r="F42" s="83">
-        <v>45264</v>
+        <v>45257</v>
       </c>
       <c r="G42" s="83">
-        <v>45270</v>
+        <v>45269</v>
       </c>
       <c r="H42" s="16"/>
       <c r="I42" s="5">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J42" s="49"/>
       <c r="K42" s="49"/>
@@ -6432,174 +6445,278 @@
     </row>
     <row r="43" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="12"/>
-      <c r="B43" s="125" t="s">
-        <v>79</v>
-      </c>
-      <c r="C43" s="126"/>
-      <c r="D43" s="127"/>
-      <c r="E43" s="84"/>
-      <c r="F43" s="85"/>
-      <c r="G43" s="85"/>
+      <c r="B43" s="80" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="82">
+        <v>0</v>
+      </c>
+      <c r="E43" s="128" t="s">
+        <v>84</v>
+      </c>
+      <c r="F43" s="83">
+        <v>45264</v>
+      </c>
+      <c r="G43" s="83">
+        <v>45269</v>
+      </c>
       <c r="H43" s="16"/>
-      <c r="I43" s="5" t="str">
+      <c r="I43" s="5">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="J43" s="49"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49"/>
+      <c r="O43" s="49"/>
+      <c r="P43" s="107"/>
+      <c r="Q43" s="107"/>
+      <c r="R43" s="107"/>
+      <c r="S43" s="49"/>
+      <c r="T43" s="49"/>
+      <c r="U43" s="49"/>
+      <c r="V43" s="49"/>
+      <c r="W43" s="49"/>
+      <c r="X43" s="49"/>
+      <c r="Y43" s="49"/>
+      <c r="Z43" s="49"/>
+      <c r="AA43" s="49"/>
+      <c r="AB43" s="49"/>
+      <c r="AC43" s="49"/>
+      <c r="AD43" s="49"/>
+      <c r="AE43" s="49"/>
+      <c r="AF43" s="49"/>
+      <c r="AG43" s="49"/>
+      <c r="AH43" s="49"/>
+      <c r="AI43" s="49"/>
+      <c r="AJ43" s="49"/>
+      <c r="AK43" s="49"/>
+      <c r="AL43" s="49"/>
+      <c r="AM43" s="49"/>
+      <c r="AN43" s="49"/>
+      <c r="AO43" s="49"/>
+      <c r="AP43" s="49"/>
+      <c r="AQ43" s="49"/>
+      <c r="AR43" s="49"/>
+      <c r="AS43" s="49"/>
+      <c r="AT43" s="49"/>
+      <c r="AU43" s="107"/>
+      <c r="AV43" s="107"/>
+      <c r="AW43" s="107"/>
+      <c r="AX43" s="107"/>
+      <c r="AY43" s="107"/>
+      <c r="AZ43" s="49"/>
+      <c r="BA43" s="49"/>
+      <c r="BB43" s="49"/>
+      <c r="BC43" s="49"/>
+      <c r="BD43" s="49"/>
+      <c r="BE43" s="49"/>
+      <c r="BF43" s="49"/>
+      <c r="BG43" s="49"/>
+      <c r="BH43" s="49"/>
+      <c r="BI43" s="49"/>
+      <c r="BJ43" s="49"/>
+      <c r="BK43" s="49"/>
+      <c r="BL43" s="49"/>
+      <c r="BM43" s="49"/>
+      <c r="BN43" s="107"/>
+      <c r="BO43" s="107"/>
+      <c r="BP43" s="107"/>
+      <c r="BQ43" s="107"/>
+      <c r="BR43" s="107"/>
+      <c r="BS43" s="107"/>
+      <c r="BT43" s="107"/>
+    </row>
+    <row r="44" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="12"/>
+      <c r="B44" s="125" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="126"/>
+      <c r="D44" s="127"/>
+      <c r="E44" s="84"/>
+      <c r="F44" s="85"/>
+      <c r="G44" s="85"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="5" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="J43" s="43"/>
-      <c r="K43" s="43"/>
-      <c r="L43" s="43"/>
-      <c r="M43" s="43"/>
-      <c r="N43" s="43"/>
-      <c r="O43" s="43"/>
-      <c r="P43" s="106"/>
-      <c r="Q43" s="106"/>
-      <c r="R43" s="106"/>
-      <c r="S43" s="43"/>
-      <c r="T43" s="43"/>
-      <c r="U43" s="43"/>
-      <c r="V43" s="43"/>
-      <c r="W43" s="43"/>
-      <c r="X43" s="43"/>
-      <c r="Y43" s="43"/>
-      <c r="Z43" s="43"/>
-      <c r="AA43" s="43"/>
-      <c r="AB43" s="43"/>
-      <c r="AC43" s="43"/>
-      <c r="AD43" s="43"/>
-      <c r="AE43" s="43"/>
-      <c r="AF43" s="43"/>
-      <c r="AG43" s="43"/>
-      <c r="AH43" s="43"/>
-      <c r="AI43" s="43"/>
-      <c r="AJ43" s="43"/>
-      <c r="AK43" s="43"/>
-      <c r="AL43" s="43"/>
-      <c r="AM43" s="43"/>
-      <c r="AN43" s="43"/>
-      <c r="AO43" s="43"/>
-      <c r="AP43" s="43"/>
-      <c r="AQ43" s="43"/>
-      <c r="AR43" s="43"/>
-      <c r="AS43" s="43"/>
-      <c r="AT43" s="43"/>
-      <c r="AU43" s="106"/>
-      <c r="AV43" s="106"/>
-      <c r="AW43" s="106"/>
-      <c r="AX43" s="106"/>
-      <c r="AY43" s="106"/>
-      <c r="AZ43" s="43"/>
-      <c r="BA43" s="43"/>
-      <c r="BB43" s="43"/>
-      <c r="BC43" s="43"/>
-      <c r="BD43" s="43"/>
-      <c r="BE43" s="43"/>
-      <c r="BF43" s="43"/>
-      <c r="BG43" s="43"/>
-      <c r="BH43" s="43"/>
-      <c r="BI43" s="43"/>
-      <c r="BJ43" s="43"/>
-      <c r="BK43" s="43"/>
-      <c r="BL43" s="43"/>
-      <c r="BM43" s="43"/>
-      <c r="BN43" s="106"/>
-      <c r="BO43" s="106"/>
-      <c r="BP43" s="106"/>
-      <c r="BQ43" s="106"/>
-      <c r="BR43" s="106"/>
-      <c r="BS43" s="106"/>
-      <c r="BT43" s="106"/>
+      <c r="J44" s="43"/>
+      <c r="K44" s="43"/>
+      <c r="L44" s="43"/>
+      <c r="M44" s="43"/>
+      <c r="N44" s="43"/>
+      <c r="O44" s="43"/>
+      <c r="P44" s="106"/>
+      <c r="Q44" s="106"/>
+      <c r="R44" s="106"/>
+      <c r="S44" s="43"/>
+      <c r="T44" s="43"/>
+      <c r="U44" s="43"/>
+      <c r="V44" s="43"/>
+      <c r="W44" s="43"/>
+      <c r="X44" s="43"/>
+      <c r="Y44" s="43"/>
+      <c r="Z44" s="43"/>
+      <c r="AA44" s="43"/>
+      <c r="AB44" s="43"/>
+      <c r="AC44" s="43"/>
+      <c r="AD44" s="43"/>
+      <c r="AE44" s="43"/>
+      <c r="AF44" s="43"/>
+      <c r="AG44" s="43"/>
+      <c r="AH44" s="43"/>
+      <c r="AI44" s="43"/>
+      <c r="AJ44" s="43"/>
+      <c r="AK44" s="43"/>
+      <c r="AL44" s="43"/>
+      <c r="AM44" s="43"/>
+      <c r="AN44" s="43"/>
+      <c r="AO44" s="43"/>
+      <c r="AP44" s="43"/>
+      <c r="AQ44" s="43"/>
+      <c r="AR44" s="43"/>
+      <c r="AS44" s="43"/>
+      <c r="AT44" s="43"/>
+      <c r="AU44" s="106"/>
+      <c r="AV44" s="106"/>
+      <c r="AW44" s="106"/>
+      <c r="AX44" s="106"/>
+      <c r="AY44" s="106"/>
+      <c r="AZ44" s="43"/>
+      <c r="BA44" s="43"/>
+      <c r="BB44" s="43"/>
+      <c r="BC44" s="43"/>
+      <c r="BD44" s="43"/>
+      <c r="BE44" s="43"/>
+      <c r="BF44" s="43"/>
+      <c r="BG44" s="43"/>
+      <c r="BH44" s="43"/>
+      <c r="BI44" s="43"/>
+      <c r="BJ44" s="43"/>
+      <c r="BK44" s="43"/>
+      <c r="BL44" s="43"/>
+      <c r="BM44" s="43"/>
+      <c r="BN44" s="106"/>
+      <c r="BO44" s="106"/>
+      <c r="BP44" s="106"/>
+      <c r="BQ44" s="106"/>
+      <c r="BR44" s="106"/>
+      <c r="BS44" s="106"/>
+      <c r="BT44" s="106"/>
     </row>
-    <row r="44" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="13"/>
-      <c r="B44" s="86" t="s">
+    <row r="45" spans="1:72" s="44" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="13"/>
+      <c r="B45" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C44" s="87"/>
-      <c r="D44" s="88"/>
-      <c r="E44" s="88"/>
-      <c r="F44" s="89"/>
-      <c r="G44" s="90"/>
-      <c r="H44" s="90"/>
-      <c r="I44" s="90" t="str">
+      <c r="C45" s="87"/>
+      <c r="D45" s="88"/>
+      <c r="E45" s="88"/>
+      <c r="F45" s="89"/>
+      <c r="G45" s="90"/>
+      <c r="H45" s="90"/>
+      <c r="I45" s="90" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="J44" s="90"/>
-      <c r="K44" s="90"/>
-      <c r="L44" s="90"/>
-      <c r="M44" s="90"/>
-      <c r="N44" s="90"/>
-      <c r="O44" s="90"/>
-      <c r="P44" s="90"/>
-      <c r="Q44" s="90"/>
-      <c r="R44" s="90"/>
-      <c r="S44" s="90"/>
-      <c r="T44" s="90"/>
-      <c r="U44" s="90"/>
-      <c r="V44" s="90"/>
-      <c r="W44" s="90"/>
-      <c r="X44" s="90"/>
-      <c r="Y44" s="90"/>
-      <c r="Z44" s="90"/>
-      <c r="AA44" s="90"/>
-      <c r="AB44" s="90"/>
-      <c r="AC44" s="90"/>
-      <c r="AD44" s="90"/>
-      <c r="AE44" s="90"/>
-      <c r="AF44" s="90"/>
-      <c r="AG44" s="90"/>
-      <c r="AH44" s="90"/>
-      <c r="AI44" s="90"/>
-      <c r="AJ44" s="90"/>
-      <c r="AK44" s="90"/>
-      <c r="AL44" s="90"/>
-      <c r="AM44" s="90"/>
-      <c r="AN44" s="90"/>
-      <c r="AO44" s="90"/>
-      <c r="AP44" s="90"/>
-      <c r="AQ44" s="90"/>
-      <c r="AR44" s="90"/>
-      <c r="AS44" s="90"/>
-      <c r="AT44" s="90"/>
-      <c r="AU44" s="90"/>
-      <c r="AV44" s="90"/>
-      <c r="AW44" s="90"/>
-      <c r="AX44" s="90"/>
-      <c r="AY44" s="90"/>
-      <c r="AZ44" s="90"/>
-      <c r="BA44" s="90"/>
-      <c r="BB44" s="90"/>
-      <c r="BC44" s="90"/>
-      <c r="BD44" s="90"/>
-      <c r="BE44" s="90"/>
-      <c r="BF44" s="90"/>
-      <c r="BG44" s="90"/>
-      <c r="BH44" s="90"/>
-      <c r="BI44" s="90"/>
-      <c r="BJ44" s="90"/>
-      <c r="BK44" s="90"/>
-      <c r="BL44" s="90"/>
-      <c r="BM44" s="90"/>
-      <c r="BN44" s="90"/>
-      <c r="BO44" s="90"/>
-      <c r="BP44" s="90"/>
-      <c r="BQ44" s="90"/>
-      <c r="BR44" s="90"/>
-      <c r="BS44" s="90"/>
-      <c r="BT44" s="90"/>
+      <c r="J45" s="90"/>
+      <c r="K45" s="90"/>
+      <c r="L45" s="90"/>
+      <c r="M45" s="90"/>
+      <c r="N45" s="90"/>
+      <c r="O45" s="90"/>
+      <c r="P45" s="90"/>
+      <c r="Q45" s="90"/>
+      <c r="R45" s="90"/>
+      <c r="S45" s="90"/>
+      <c r="T45" s="90"/>
+      <c r="U45" s="90"/>
+      <c r="V45" s="90"/>
+      <c r="W45" s="90"/>
+      <c r="X45" s="90"/>
+      <c r="Y45" s="90"/>
+      <c r="Z45" s="90"/>
+      <c r="AA45" s="90"/>
+      <c r="AB45" s="90"/>
+      <c r="AC45" s="90"/>
+      <c r="AD45" s="90"/>
+      <c r="AE45" s="90"/>
+      <c r="AF45" s="90"/>
+      <c r="AG45" s="90"/>
+      <c r="AH45" s="90"/>
+      <c r="AI45" s="90"/>
+      <c r="AJ45" s="90"/>
+      <c r="AK45" s="90"/>
+      <c r="AL45" s="90"/>
+      <c r="AM45" s="90"/>
+      <c r="AN45" s="90"/>
+      <c r="AO45" s="90"/>
+      <c r="AP45" s="90"/>
+      <c r="AQ45" s="90"/>
+      <c r="AR45" s="90"/>
+      <c r="AS45" s="90"/>
+      <c r="AT45" s="90"/>
+      <c r="AU45" s="90"/>
+      <c r="AV45" s="90"/>
+      <c r="AW45" s="90"/>
+      <c r="AX45" s="90"/>
+      <c r="AY45" s="90"/>
+      <c r="AZ45" s="90"/>
+      <c r="BA45" s="90"/>
+      <c r="BB45" s="90"/>
+      <c r="BC45" s="90"/>
+      <c r="BD45" s="90"/>
+      <c r="BE45" s="90"/>
+      <c r="BF45" s="90"/>
+      <c r="BG45" s="90"/>
+      <c r="BH45" s="90"/>
+      <c r="BI45" s="90"/>
+      <c r="BJ45" s="90"/>
+      <c r="BK45" s="90"/>
+      <c r="BL45" s="90"/>
+      <c r="BM45" s="90"/>
+      <c r="BN45" s="90"/>
+      <c r="BO45" s="90"/>
+      <c r="BP45" s="90"/>
+      <c r="BQ45" s="90"/>
+      <c r="BR45" s="90"/>
+      <c r="BS45" s="90"/>
+      <c r="BT45" s="90"/>
     </row>
-    <row r="45" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H45" s="3"/>
+    <row r="46" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H46" s="3"/>
     </row>
-    <row r="46" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C46" s="15"/>
-      <c r="G46" s="14"/>
+    <row r="47" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C47" s="15"/>
+      <c r="G47" s="14"/>
     </row>
-    <row r="47" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C47" s="4"/>
+    <row r="48" spans="1:72" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C48" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="AZ5:BF5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="R3:AA3"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="J5:P5"/>
+    <mergeCell ref="Q5:W5"/>
+    <mergeCell ref="X5:AD5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="E6:E7"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="Q1:Z1"/>
     <mergeCell ref="BN5:BT5"/>
@@ -6616,24 +6733,9 @@
     <mergeCell ref="AE5:AK5"/>
     <mergeCell ref="AL5:AR5"/>
     <mergeCell ref="AS5:AY5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="AZ5:BF5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="R3:AA3"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="J3:P3"/>
-    <mergeCell ref="J5:P5"/>
-    <mergeCell ref="Q5:W5"/>
-    <mergeCell ref="X5:AD5"/>
   </mergeCells>
   <phoneticPr fontId="32" type="noConversion"/>
-  <conditionalFormatting sqref="D37:E37 D43:E44 D38:D42 D8:E24 D25:D36">
+  <conditionalFormatting sqref="D38:E38 D44:E45 D39:D43 D8:E24 D25:D37">
     <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6663,7 +6765,7 @@
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J25:BL36 BN25:BT36">
+  <conditionalFormatting sqref="J25:BL37 BN25:BT37">
     <cfRule type="expression" dxfId="47" priority="51">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
@@ -6671,7 +6773,7 @@
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J39:BL42">
+  <conditionalFormatting sqref="J40:BL43">
     <cfRule type="expression" dxfId="45" priority="85">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
@@ -6679,7 +6781,7 @@
       <formula>AND(task_end&gt;=J$6,task_start&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN5:BS8 J5:BL9 J10:BM11 BN9:BT42 J12:BL42">
+  <conditionalFormatting sqref="BN5:BS8 J5:BL9 J10:BM11 BN9:BT43 J12:BL43">
     <cfRule type="expression" dxfId="43" priority="50">
       <formula>AND(TODAY()&gt;=J$6, TODAY()&lt;K$6)</formula>
     </cfRule>
@@ -6700,7 +6802,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BU$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM25:BM36">
+  <conditionalFormatting sqref="BM25:BM37">
     <cfRule type="expression" dxfId="38" priority="97">
       <formula>AND(task_start&lt;=BM$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$6)</formula>
     </cfRule>
@@ -6708,7 +6810,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BU$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM38:BM40">
+  <conditionalFormatting sqref="BM39:BM41">
     <cfRule type="expression" dxfId="36" priority="101">
       <formula>AND(task_start&lt;=BM$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$6)</formula>
     </cfRule>
@@ -6716,7 +6818,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BU$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BT5:BT8 BM5:BM9 BM12:BM40">
+  <conditionalFormatting sqref="BT5:BT8 BM5:BM9 BM12:BM41">
     <cfRule type="expression" dxfId="34" priority="104">
       <formula>AND(TODAY()&gt;=BM$6, TODAY()&lt;BU$6)</formula>
     </cfRule>
@@ -6726,7 +6828,7 @@
       <formula>AND(TODAY()&gt;=J$6, TODAY()&lt;K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J38:BL38">
+  <conditionalFormatting sqref="J39:BL39">
     <cfRule type="expression" dxfId="32" priority="34">
       <formula>AND(task_start&lt;=J$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=J$6)</formula>
     </cfRule>
@@ -6750,7 +6852,7 @@
       <formula>AND(task_end&gt;=BN$6,task_start&lt;BO$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN39:BO42">
+  <conditionalFormatting sqref="BN40:BO43">
     <cfRule type="expression" dxfId="26" priority="30">
       <formula>AND(task_start&lt;=BN$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BN$6)</formula>
     </cfRule>
@@ -6758,7 +6860,7 @@
       <formula>AND(task_end&gt;=BN$6,task_start&lt;BO$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BN38:BO38">
+  <conditionalFormatting sqref="BN39:BO39">
     <cfRule type="expression" dxfId="24" priority="24">
       <formula>AND(task_start&lt;=BN$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BN$6)</formula>
     </cfRule>
@@ -6782,7 +6884,7 @@
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP39:BT42">
+  <conditionalFormatting sqref="BP40:BT43">
     <cfRule type="expression" dxfId="18" priority="22">
       <formula>AND(task_start&lt;=BP$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BP$6)</formula>
     </cfRule>
@@ -6790,7 +6892,7 @@
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BP38:BT38">
+  <conditionalFormatting sqref="BP39:BT39">
     <cfRule type="expression" dxfId="16" priority="16">
       <formula>AND(task_start&lt;=BP$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BP$6)</formula>
     </cfRule>
@@ -6798,7 +6900,7 @@
       <formula>AND(task_end&gt;=BP$6,task_start&lt;BQ$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM41:BM42">
+  <conditionalFormatting sqref="BM42:BM43">
     <cfRule type="expression" dxfId="14" priority="14">
       <formula>AND(task_start&lt;=BM$6,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=BM$6)</formula>
     </cfRule>
@@ -6806,7 +6908,7 @@
       <formula>AND(task_end&gt;=BM$6,task_start&lt;BN$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BM41:BM42">
+  <conditionalFormatting sqref="BM42:BM43">
     <cfRule type="expression" dxfId="12" priority="13">
       <formula>AND(TODAY()&gt;=BM$6, TODAY()&lt;BN$6)</formula>
     </cfRule>
@@ -6869,8 +6971,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Rows 10 through 13 repeat the pattern from row 9. _x000a__x000a_Repeat the instructions from cell A9 for all task rows in this worksheet. _x000a__x000a_Continue entering tasks in cells A10 through A13 or go to cell A14 to learn more." sqref="A13:A14" xr:uid="{872449A7-C3CC-45B6-BA90-B1AAD66BA0E5}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Cell B14 contains the Phase 2 sample title. Enter a new title in cell B14._x000a_To delete the phase and work only from tasks, simply delete this row. To remove the phase, simply delete the row. Add tasks to previous phase by entering a new row above this one._x000a_" sqref="A18" xr:uid="{4F48FC41-E335-47F1-87AA-3333A52AD81C}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 3's sample block starts in cell B20." sqref="A24" xr:uid="{956902D1-D3B5-416D-BB69-9362D193BC0A}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A37" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A44" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Phase 4's sample block starts in cell B26." sqref="A38" xr:uid="{DE54E5DE-526D-4D71-8D03-E99B4AB2FEE5}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Project Schedule. DO NOT enter anything in this row. _x000a_Insert new rows ABOVE this one to continue building out your Project Schedule." sqref="A45" xr:uid="{79B9237E-4DD3-4E0F-8ED6-E0B695A99D96}"/>
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="R3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -6882,7 +6984,7 @@
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="3" scale="55" orientation="landscape" r:id="rId3"/>
+  <pageSetup paperSize="3" scale="53" orientation="landscape" r:id="rId3"/>
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
@@ -6905,7 +7007,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D37:E37 D43:E44 D38:D42 D8:E24 D25:D36</xm:sqref>
+          <xm:sqref>D38:E38 D44:E45 D39:D43 D8:E24 D25:D37</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -7040,35 +7142,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7380,10 +7453,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7408,22 +7523,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>